<commit_message>
Penambahan dan Dokumentasi API Engine, Penambahan Model Database
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -386,6 +386,24 @@
   </si>
   <si>
     <t>Menghapus Data Kurs Mata Uang Pajak</t>
+  </si>
+  <si>
+    <t>transaction.delete.master.setDayOffGovernmentPolicy</t>
+  </si>
+  <si>
+    <t>transaction.delete.master.setDayOffNational</t>
+  </si>
+  <si>
+    <t>Menghapus Data Hari Libur Kebijakan Pemerintah</t>
+  </si>
+  <si>
+    <t>Menghapus Data Hari Libur Nasional</t>
+  </si>
+  <si>
+    <t>transaction.delete.master.setDayOffRegional</t>
+  </si>
+  <si>
+    <t>Menghapus Data Hari Libur Regional</t>
   </si>
 </sst>
 </file>
@@ -889,13 +907,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C85"/>
+  <dimension ref="B1:C93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -939,29 +957,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-    </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
@@ -969,147 +983,163 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>95</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>98</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="4"/>
-    </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="4"/>
+      <c r="B30" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="4"/>
+      <c r="B31" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
@@ -1131,365 +1161,397 @@
       <c r="B37" s="7"/>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="12"/>
-      <c r="C38" s="13"/>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="7"/>
+      <c r="C38" s="4"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="4"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="4"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>61</v>
-      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="12"/>
+      <c r="C42" s="13"/>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="7" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="7" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="12"/>
-      <c r="C59" s="13"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="7" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="B63" s="7"/>
+      <c r="C63" s="4"/>
+    </row>
+    <row r="64" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="12"/>
+      <c r="C64" s="13"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="7" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="7" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="7" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="7" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="7" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="7" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="7" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="7" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="7" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="7" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="12"/>
-      <c r="C79" s="13"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="12"/>
-      <c r="C81" s="13"/>
+        <v>45</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" s="7"/>
+      <c r="C84" s="4"/>
+    </row>
+    <row r="85" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="12"/>
+      <c r="C85" s="13"/>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" s="7"/>
+      <c r="C87" s="4"/>
+    </row>
+    <row r="88" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="12"/>
+      <c r="C88" s="13"/>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C89" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="83" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="12"/>
-      <c r="C83" s="13"/>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="7" t="s">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90" s="7"/>
+      <c r="C90" s="4"/>
+    </row>
+    <row r="91" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="12"/>
+      <c r="C91" s="13"/>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C92" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="85" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="8"/>
-      <c r="C85" s="6"/>
+    <row r="93" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="8"/>
+      <c r="C93" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Perubahan Script.Docker.Reinitializing.Database.PostgreSQL.sh agar database Docker bisa berjalan secara mandiri
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="316">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -58,9 +58,6 @@
     <t>transaction.create.master.setBloodAglutinogenType</t>
   </si>
   <si>
-    <t>Menyimpan data baru jenis golongan darah</t>
-  </si>
-  <si>
     <t>transaction.read.master.getDataListBloodAglutinogenType</t>
   </si>
   <si>
@@ -956,6 +953,15 @@
   </si>
   <si>
     <t>Menghapus Data Rotate Log - API</t>
+  </si>
+  <si>
+    <t>transaction.create.master.set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menyimpan Data Baru </t>
+  </si>
+  <si>
+    <t>Menyimpan Data Baru Jenis Golongan Darah</t>
   </si>
 </sst>
 </file>
@@ -1478,13 +1484,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C194"/>
+  <dimension ref="B1:C206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1573,419 +1579,427 @@
         <v>13</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>14</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
+      <c r="B15" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
+      <c r="C22" s="4" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
-        <v>52</v>
+        <v>313</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>94</v>
+        <v>314</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>96</v>
+        <v>313</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>97</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
-        <v>98</v>
+        <v>313</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>101</v>
+        <v>314</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
-        <v>115</v>
+        <v>313</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>116</v>
+        <v>314</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
-        <v>100</v>
+        <v>305</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>102</v>
+        <v>307</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
-        <v>131</v>
+        <v>306</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>134</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
-        <v>99</v>
+        <v>303</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>103</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
-        <v>107</v>
+        <v>310</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>111</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
-        <v>108</v>
+        <v>309</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>113</v>
-      </c>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="7" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>205</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="7" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>206</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>207</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="7" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>208</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>209</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>212</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="7" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>210</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="7" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>211</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="7" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>214</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="7" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>215</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>216</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="7" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="7" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="7" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="14"/>
-      <c r="C57" s="15"/>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="7" t="s">
-        <v>240</v>
+        <v>144</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>248</v>
+        <v>207</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="7" t="s">
-        <v>241</v>
+        <v>143</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="s">
-        <v>242</v>
+        <v>142</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="7" t="s">
-        <v>243</v>
+        <v>141</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>247</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="7" t="s">
-        <v>244</v>
+        <v>140</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="14"/>
-      <c r="C63" s="15"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="7" t="s">
-        <v>224</v>
+        <v>138</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="7" t="s">
-        <v>225</v>
+        <v>137</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="7" t="s">
-        <v>226</v>
+        <v>136</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="7" t="s">
-        <v>227</v>
+        <v>135</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="7" t="s">
-        <v>228</v>
+        <v>134</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1994,939 +2008,1027 @@
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="7" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="14"/>
-      <c r="C71" s="15"/>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="7" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="7" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="14"/>
-      <c r="C74" s="15"/>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="14"/>
-      <c r="C76" s="15"/>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="14"/>
+      <c r="C75" s="15"/>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="7" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="7" t="s">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>288</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="7" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>290</v>
+        <v>231</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="7" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>291</v>
-      </c>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="14"/>
+      <c r="C81" s="15"/>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="7" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B83" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>270</v>
-      </c>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="14"/>
+      <c r="C83" s="15"/>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="7" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>292</v>
+        <v>237</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="7" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>269</v>
-      </c>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="14"/>
+      <c r="C86" s="15"/>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="7" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>272</v>
-      </c>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="14"/>
+      <c r="C88" s="15"/>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="7" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>278</v>
+        <v>252</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="7" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="7" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>266</v>
+        <v>289</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="7" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="7" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="7" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="7" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="7" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="7" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="14"/>
-      <c r="C98" s="15"/>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="7" t="s">
-        <v>150</v>
+        <v>263</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>220</v>
+        <v>270</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="7" t="s">
-        <v>221</v>
+        <v>264</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="14"/>
-      <c r="C101" s="15"/>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="7" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="7" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>296</v>
+        <v>265</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="7" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>303</v>
+        <v>276</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="7" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="7" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="7"/>
-      <c r="C107" s="4"/>
-    </row>
-    <row r="108" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="12"/>
-      <c r="C108" s="13"/>
+      <c r="B107" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B108" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="7" t="s">
-        <v>54</v>
+        <v>282</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B110" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C110" s="4" t="s">
-        <v>57</v>
-      </c>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="14"/>
+      <c r="C110" s="15"/>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="7" t="s">
-        <v>59</v>
+        <v>149</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>58</v>
+        <v>219</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="7" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B113" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C113" s="4" t="s">
-        <v>67</v>
-      </c>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="14"/>
+      <c r="C113" s="15"/>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="7" t="s">
-        <v>63</v>
+        <v>293</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>66</v>
+        <v>301</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="7" t="s">
-        <v>64</v>
+        <v>294</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>69</v>
+        <v>295</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="7" t="s">
-        <v>65</v>
+        <v>296</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>68</v>
+        <v>302</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="7" t="s">
-        <v>70</v>
+        <v>297</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>82</v>
+        <v>298</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="7" t="s">
-        <v>72</v>
+        <v>299</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>83</v>
+        <v>300</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B119" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B120" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C120" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="B119" s="7"/>
+      <c r="C119" s="4"/>
+    </row>
+    <row r="120" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="12"/>
+      <c r="C120" s="13"/>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="7" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" s="7" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" s="7" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" s="7" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>213</v>
+        <v>60</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" s="7" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" s="7" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" s="7" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C129" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C128" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B129" s="7"/>
-      <c r="C129" s="4"/>
-    </row>
-    <row r="130" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="12"/>
-      <c r="C130" s="13"/>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="7" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" s="7" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" s="7" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" s="7" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" s="7" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" s="7" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>26</v>
+        <v>212</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" s="7" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="7" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" s="7" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" s="7" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B141" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C141" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B142" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C142" s="4" t="s">
-        <v>87</v>
-      </c>
+      <c r="B141" s="7"/>
+      <c r="C141" s="4"/>
+    </row>
+    <row r="142" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B142" s="12"/>
+      <c r="C142" s="13"/>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" s="7" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" s="7" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="7" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C146" s="5" t="s">
-        <v>46</v>
+        <v>20</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" s="7" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" s="7" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" s="7" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B150" s="7"/>
-      <c r="C150" s="4"/>
-    </row>
-    <row r="151" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="12"/>
-      <c r="C151" s="13"/>
+      <c r="B150" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B151" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" s="7" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B153" s="7"/>
-      <c r="C153" s="4"/>
-    </row>
-    <row r="154" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="12"/>
-      <c r="C154" s="13"/>
+      <c r="B153" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B154" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" s="7" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>95</v>
+        <v>39</v>
       </c>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" s="7" t="s">
-        <v>170</v>
+        <v>40</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>151</v>
+        <v>41</v>
       </c>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" s="7" t="s">
-        <v>171</v>
+        <v>42</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>152</v>
+        <v>43</v>
       </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C158" s="4" t="s">
-        <v>153</v>
+        <v>44</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" s="7" t="s">
-        <v>173</v>
+        <v>46</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>154</v>
+        <v>47</v>
       </c>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" s="7" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>155</v>
+        <v>37</v>
       </c>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" s="7" t="s">
-        <v>175</v>
+        <v>49</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>156</v>
+        <v>50</v>
       </c>
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B162" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="C162" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B163" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C163" s="4" t="s">
-        <v>158</v>
-      </c>
+      <c r="B162" s="7"/>
+      <c r="C162" s="4"/>
+    </row>
+    <row r="163" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="12"/>
+      <c r="C163" s="13"/>
     </row>
     <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" s="7" t="s">
-        <v>178</v>
+        <v>103</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>159</v>
+        <v>104</v>
       </c>
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B165" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C165" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B166" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="C166" s="4" t="s">
-        <v>161</v>
-      </c>
+      <c r="B165" s="7"/>
+      <c r="C165" s="4"/>
+    </row>
+    <row r="166" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B166" s="12"/>
+      <c r="C166" s="13"/>
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" s="7" t="s">
-        <v>181</v>
+        <v>52</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>162</v>
+        <v>94</v>
       </c>
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" s="7" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" s="7" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" s="7" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" s="7" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" s="7" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" s="7" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" s="7" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" s="7" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" s="7" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" s="7" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" s="7" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" s="7" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" s="7" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" s="7" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" s="7" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" s="7" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" s="7" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" s="7" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" s="7" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" s="7" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" s="7" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" s="7" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" s="7" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B191" s="7"/>
-      <c r="C191" s="4"/>
-    </row>
-    <row r="192" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B192" s="12"/>
-      <c r="C192" s="13"/>
+      <c r="B191" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C191" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B192" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C192" s="4" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C193" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B194" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C194" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B195" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C195" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B196" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B197" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B198" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B199" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B200" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C200" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B201" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B202" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B203" s="7"/>
+      <c r="C203" s="4"/>
+    </row>
+    <row r="204" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B204" s="12"/>
+      <c r="C204" s="13"/>
+    </row>
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B205" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C193" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="194" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B194" s="8"/>
-      <c r="C194" s="6"/>
+      <c r="C205" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="206" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B206" s="8"/>
+      <c r="C206" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Penambahan dan Update API Engine, Dokumentasi API Engine, serta Penambahan Model Database
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
@@ -1952,10 +1952,10 @@
   <dimension ref="A1:H234"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3282,12 +3282,14 @@
         <v>242</v>
       </c>
       <c r="D78" s="35"/>
-      <c r="E78" s="29"/>
+      <c r="E78" s="29">
+        <v>44188</v>
+      </c>
       <c r="F78" s="19">
         <v>1</v>
       </c>
       <c r="G78" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H78" s="35"/>
     </row>

</xml_diff>

<commit_message>
Perbaikan Helper_APICall pada BackEnd
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="410">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -1202,6 +1202,48 @@
   </si>
   <si>
     <t>instruction.device.fingerprintAttendance.Solution.x601.getDataAttendance</t>
+  </si>
+  <si>
+    <t>scheduler.everyDay.system.setJobs</t>
+  </si>
+  <si>
+    <t>scheduler.everyHour.system.setJobs</t>
+  </si>
+  <si>
+    <t>scheduler.everyMinute.system.setJobs</t>
+  </si>
+  <si>
+    <t>scheduler.everyMonth.system.setJobs</t>
+  </si>
+  <si>
+    <t>scheduler.everyTwoHours.system.setJobs</t>
+  </si>
+  <si>
+    <t>scheduler.everyWeek.system.setJobs</t>
+  </si>
+  <si>
+    <t>scheduler.everyYear.system.setJobs</t>
+  </si>
+  <si>
+    <t>Mengeset Jobs pada Scheduler harian</t>
+  </si>
+  <si>
+    <t>Mengeset Jobs pada Scheduler jaman</t>
+  </si>
+  <si>
+    <t>Mengeset Jobs pada Scheduler menitan</t>
+  </si>
+  <si>
+    <t>Mengeset Jobs pada Scheduler bulanan</t>
+  </si>
+  <si>
+    <t>Mengeset Jobs pada Scheduler dua jaman</t>
+  </si>
+  <si>
+    <t>Mengeset Jobs pada Scheduler mingguan</t>
+  </si>
+  <si>
+    <t>Mengeset Jobs pada Scheduler tahunan</t>
   </si>
 </sst>
 </file>
@@ -1980,13 +2022,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H238"/>
+  <dimension ref="A1:H247"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B142" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E147" sqref="E147"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2287,30 +2329,24 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" s="7" t="s">
-        <v>12</v>
+        <v>396</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>308</v>
+        <v>403</v>
       </c>
       <c r="D20" s="35"/>
-      <c r="E20" s="29">
-        <v>44200</v>
-      </c>
-      <c r="F20" s="19">
-        <v>1</v>
-      </c>
-      <c r="G20" s="20">
-        <v>1</v>
-      </c>
+      <c r="E20" s="29"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
-      <c r="B21" s="45" t="s">
-        <v>321</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>323</v>
+      <c r="B21" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>404</v>
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="29"/>
@@ -2320,11 +2356,11 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
-      <c r="B22" s="45" t="s">
-        <v>322</v>
-      </c>
-      <c r="C22" s="46" t="s">
-        <v>324</v>
+      <c r="B22" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>405</v>
       </c>
       <c r="D22" s="35"/>
       <c r="E22" s="29"/>
@@ -2335,134 +2371,90 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="35"/>
       <c r="B23" s="7" t="s">
-        <v>317</v>
+        <v>399</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>318</v>
+        <v>406</v>
       </c>
       <c r="D23" s="35"/>
-      <c r="E23" s="29">
-        <v>44204</v>
-      </c>
-      <c r="F23" s="19">
-        <v>1</v>
-      </c>
-      <c r="G23" s="20">
-        <v>1</v>
-      </c>
+      <c r="E23" s="29"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="35"/>
     </row>
-    <row r="24" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
-      <c r="B24" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="29">
-        <v>44204</v>
-      </c>
-      <c r="F24" s="19">
-        <v>1</v>
-      </c>
-      <c r="G24" s="20">
-        <v>1</v>
-      </c>
-      <c r="H24" s="37"/>
-    </row>
-    <row r="25" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
-      <c r="B25" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="29">
-        <v>44204</v>
-      </c>
-      <c r="F25" s="19">
-        <v>1</v>
-      </c>
-      <c r="G25" s="20">
-        <v>1</v>
-      </c>
-      <c r="H25" s="37"/>
-    </row>
-    <row r="26" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
-      <c r="B26" s="13" t="s">
-        <v>367</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>379</v>
-      </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="29">
-        <v>44204</v>
-      </c>
-      <c r="F26" s="19">
-        <v>1</v>
-      </c>
-      <c r="G26" s="20">
-        <v>1</v>
-      </c>
-      <c r="H26" s="37"/>
-    </row>
-    <row r="27" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
-      <c r="B27" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>380</v>
-      </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="29">
-        <v>44207</v>
-      </c>
-      <c r="F27" s="19">
-        <v>1</v>
-      </c>
-      <c r="G27" s="20">
-        <v>1</v>
-      </c>
-      <c r="H27" s="37"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
+      <c r="B24" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="D24" s="35"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="35"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="35"/>
+      <c r="B25" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="D25" s="35"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="35"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="35"/>
+      <c r="B26" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="D26" s="35"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="35"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="35"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="35"/>
+    </row>
+    <row r="28" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="35"/>
-      <c r="B28" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>362</v>
-      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="35"/>
-      <c r="E28" s="29">
-        <v>44207</v>
-      </c>
-      <c r="F28" s="19">
-        <v>1</v>
-      </c>
-      <c r="G28" s="20">
-        <v>1</v>
-      </c>
+      <c r="E28" s="30"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="22"/>
       <c r="H28" s="35"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="35"/>
       <c r="B29" s="7" t="s">
-        <v>360</v>
+        <v>12</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>363</v>
+        <v>308</v>
       </c>
       <c r="D29" s="35"/>
       <c r="E29" s="29">
-        <v>44207</v>
+        <v>44200</v>
       </c>
       <c r="F29" s="19">
         <v>1</v>
@@ -2474,55 +2466,43 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="35"/>
-      <c r="B30" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>364</v>
+      <c r="B30" s="45" t="s">
+        <v>321</v>
+      </c>
+      <c r="C30" s="46" t="s">
+        <v>323</v>
       </c>
       <c r="D30" s="35"/>
-      <c r="E30" s="29">
-        <v>44207</v>
-      </c>
-      <c r="F30" s="19">
-        <v>1</v>
-      </c>
-      <c r="G30" s="20">
-        <v>1</v>
-      </c>
+      <c r="E30" s="29"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20"/>
       <c r="H30" s="35"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="35"/>
-      <c r="B31" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>344</v>
+      <c r="B31" s="45" t="s">
+        <v>322</v>
+      </c>
+      <c r="C31" s="46" t="s">
+        <v>324</v>
       </c>
       <c r="D31" s="35"/>
-      <c r="E31" s="29">
-        <v>44207</v>
-      </c>
-      <c r="F31" s="19">
-        <v>1</v>
-      </c>
-      <c r="G31" s="20">
-        <v>1</v>
-      </c>
+      <c r="E31" s="29"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="20"/>
       <c r="H31" s="35"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="35"/>
       <c r="B32" s="7" t="s">
-        <v>342</v>
+        <v>317</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>345</v>
+        <v>318</v>
       </c>
       <c r="D32" s="35"/>
       <c r="E32" s="29">
-        <v>44207</v>
+        <v>44204</v>
       </c>
       <c r="F32" s="19">
         <v>1</v>
@@ -2532,17 +2512,17 @@
       </c>
       <c r="H32" s="35"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
-      <c r="B33" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="D33" s="35"/>
+    <row r="33" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="37"/>
+      <c r="B33" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="D33" s="37"/>
       <c r="E33" s="29">
-        <v>44207</v>
+        <v>44204</v>
       </c>
       <c r="F33" s="19">
         <v>1</v>
@@ -2550,19 +2530,19 @@
       <c r="G33" s="20">
         <v>1</v>
       </c>
-      <c r="H33" s="35"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
-      <c r="B34" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="D34" s="35"/>
+      <c r="H33" s="37"/>
+    </row>
+    <row r="34" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="37"/>
+      <c r="B34" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="D34" s="37"/>
       <c r="E34" s="29">
-        <v>44207</v>
+        <v>44204</v>
       </c>
       <c r="F34" s="19">
         <v>1</v>
@@ -2570,19 +2550,19 @@
       <c r="G34" s="20">
         <v>1</v>
       </c>
-      <c r="H34" s="35"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
-      <c r="B35" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="D35" s="35"/>
+      <c r="H34" s="37"/>
+    </row>
+    <row r="35" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="37"/>
+      <c r="B35" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="D35" s="37"/>
       <c r="E35" s="29">
-        <v>44207</v>
+        <v>44204</v>
       </c>
       <c r="F35" s="19">
         <v>1</v>
@@ -2590,17 +2570,17 @@
       <c r="G35" s="20">
         <v>1</v>
       </c>
-      <c r="H35" s="35"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
-      <c r="B36" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="D36" s="35"/>
+      <c r="H35" s="37"/>
+    </row>
+    <row r="36" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="37"/>
+      <c r="B36" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="D36" s="37"/>
       <c r="E36" s="29">
         <v>44207</v>
       </c>
@@ -2610,189 +2590,215 @@
       <c r="G36" s="20">
         <v>1</v>
       </c>
-      <c r="H36" s="35"/>
+      <c r="H36" s="37"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="4"/>
+      <c r="B37" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>362</v>
+      </c>
       <c r="D37" s="35"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="20"/>
+      <c r="E37" s="29">
+        <v>44207</v>
+      </c>
+      <c r="F37" s="19">
+        <v>1</v>
+      </c>
+      <c r="G37" s="20">
+        <v>1</v>
+      </c>
       <c r="H37" s="35"/>
     </row>
-    <row r="38" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
+      <c r="B38" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>363</v>
+      </c>
       <c r="D38" s="35"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="22"/>
+      <c r="E38" s="29">
+        <v>44207</v>
+      </c>
+      <c r="F38" s="19">
+        <v>1</v>
+      </c>
+      <c r="G38" s="20">
+        <v>1</v>
+      </c>
       <c r="H38" s="35"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" s="7" t="s">
-        <v>300</v>
+        <v>359</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>302</v>
+        <v>364</v>
       </c>
       <c r="D39" s="35"/>
-      <c r="E39" s="29"/>
+      <c r="E39" s="29">
+        <v>44207</v>
+      </c>
       <c r="F39" s="19">
         <v>1</v>
       </c>
       <c r="G39" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="35"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" s="7" t="s">
-        <v>301</v>
+        <v>343</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>303</v>
+        <v>344</v>
       </c>
       <c r="D40" s="35"/>
-      <c r="E40" s="29"/>
+      <c r="E40" s="29">
+        <v>44207</v>
+      </c>
       <c r="F40" s="19">
         <v>1</v>
       </c>
       <c r="G40" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="35"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" s="7" t="s">
-        <v>298</v>
+        <v>342</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>299</v>
+        <v>345</v>
       </c>
       <c r="D41" s="35"/>
-      <c r="E41" s="29"/>
+      <c r="E41" s="29">
+        <v>44207</v>
+      </c>
       <c r="F41" s="19">
         <v>1</v>
       </c>
       <c r="G41" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="35"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" s="7" t="s">
-        <v>305</v>
+        <v>341</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>306</v>
+        <v>346</v>
       </c>
       <c r="D42" s="35"/>
-      <c r="E42" s="29"/>
+      <c r="E42" s="29">
+        <v>44207</v>
+      </c>
       <c r="F42" s="19">
         <v>1</v>
       </c>
       <c r="G42" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" s="35"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" s="7" t="s">
-        <v>304</v>
+        <v>339</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>307</v>
+        <v>340</v>
       </c>
       <c r="D43" s="35"/>
-      <c r="E43" s="29"/>
+      <c r="E43" s="29">
+        <v>44207</v>
+      </c>
       <c r="F43" s="19">
         <v>1</v>
       </c>
       <c r="G43" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" s="35"/>
     </row>
-    <row r="44" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="12"/>
+      <c r="B44" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>334</v>
+      </c>
       <c r="D44" s="35"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="24"/>
+      <c r="E44" s="29">
+        <v>44207</v>
+      </c>
+      <c r="F44" s="19">
+        <v>1</v>
+      </c>
+      <c r="G44" s="20">
+        <v>1</v>
+      </c>
       <c r="H44" s="35"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="35"/>
       <c r="B45" s="7" t="s">
-        <v>50</v>
+        <v>331</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>92</v>
+        <v>332</v>
       </c>
       <c r="D45" s="35"/>
-      <c r="E45" s="29"/>
+      <c r="E45" s="29">
+        <v>44207</v>
+      </c>
       <c r="F45" s="19">
         <v>1</v>
       </c>
       <c r="G45" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" s="35"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="35"/>
-      <c r="B46" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>95</v>
-      </c>
+      <c r="B46" s="7"/>
+      <c r="C46" s="4"/>
       <c r="D46" s="35"/>
       <c r="E46" s="29"/>
-      <c r="F46" s="19">
-        <v>1</v>
-      </c>
-      <c r="G46" s="20">
-        <v>0</v>
-      </c>
+      <c r="F46" s="19"/>
+      <c r="G46" s="20"/>
       <c r="H46" s="35"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="35"/>
-      <c r="B47" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>312</v>
-      </c>
+      <c r="B47" s="9"/>
+      <c r="C47" s="10"/>
       <c r="D47" s="35"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="19">
-        <v>1</v>
-      </c>
-      <c r="G47" s="20">
-        <v>0</v>
-      </c>
+      <c r="E47" s="30"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="22"/>
       <c r="H47" s="35"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="35"/>
       <c r="B48" s="7" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="D48" s="35"/>
       <c r="E48" s="29"/>
@@ -2807,10 +2813,10 @@
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="35"/>
       <c r="B49" s="7" t="s">
-        <v>96</v>
+        <v>301</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>99</v>
+        <v>303</v>
       </c>
       <c r="D49" s="35"/>
       <c r="E49" s="29"/>
@@ -2825,10 +2831,10 @@
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="35"/>
       <c r="B50" s="7" t="s">
-        <v>109</v>
+        <v>298</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>110</v>
+        <v>299</v>
       </c>
       <c r="D50" s="35"/>
       <c r="E50" s="29"/>
@@ -2843,10 +2849,10 @@
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="35"/>
       <c r="B51" s="7" t="s">
-        <v>123</v>
+        <v>305</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>126</v>
+        <v>306</v>
       </c>
       <c r="D51" s="35"/>
       <c r="E51" s="29"/>
@@ -2861,10 +2867,10 @@
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="35"/>
       <c r="B52" s="7" t="s">
-        <v>124</v>
+        <v>304</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>127</v>
+        <v>307</v>
       </c>
       <c r="D52" s="35"/>
       <c r="E52" s="29"/>
@@ -2876,31 +2882,23 @@
       </c>
       <c r="H52" s="35"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="35"/>
-      <c r="B53" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>100</v>
-      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="12"/>
       <c r="D53" s="35"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="19">
-        <v>1</v>
-      </c>
-      <c r="G53" s="20">
-        <v>0</v>
-      </c>
+      <c r="E53" s="32"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="24"/>
       <c r="H53" s="35"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="35"/>
       <c r="B54" s="7" t="s">
-        <v>125</v>
+        <v>50</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
       <c r="D54" s="35"/>
       <c r="E54" s="29"/>
@@ -2915,10 +2913,10 @@
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="35"/>
       <c r="B55" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D55" s="35"/>
       <c r="E55" s="29"/>
@@ -2933,10 +2931,10 @@
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="35"/>
       <c r="B56" s="7" t="s">
-        <v>105</v>
+        <v>311</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>381</v>
+        <v>312</v>
       </c>
       <c r="D56" s="35"/>
       <c r="E56" s="29"/>
@@ -2951,10 +2949,10 @@
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="35"/>
       <c r="B57" s="7" t="s">
-        <v>106</v>
+        <v>313</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>382</v>
+        <v>314</v>
       </c>
       <c r="D57" s="35"/>
       <c r="E57" s="29"/>
@@ -2969,10 +2967,10 @@
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="35"/>
       <c r="B58" s="7" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>383</v>
+        <v>99</v>
       </c>
       <c r="D58" s="35"/>
       <c r="E58" s="29"/>
@@ -2987,10 +2985,10 @@
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="35"/>
       <c r="B59" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>384</v>
+        <v>110</v>
       </c>
       <c r="D59" s="35"/>
       <c r="E59" s="29"/>
@@ -3005,10 +3003,10 @@
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="35"/>
       <c r="B60" s="7" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="D60" s="35"/>
       <c r="E60" s="29"/>
@@ -3023,10 +3021,10 @@
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="35"/>
       <c r="B61" s="7" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="D61" s="35"/>
       <c r="E61" s="29"/>
@@ -3041,10 +3039,10 @@
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="35"/>
       <c r="B62" s="7" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D62" s="35"/>
       <c r="E62" s="29"/>
@@ -3059,10 +3057,10 @@
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="35"/>
       <c r="B63" s="7" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="D63" s="35"/>
       <c r="E63" s="29"/>
@@ -3077,10 +3075,10 @@
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="35"/>
       <c r="B64" s="7" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="D64" s="35"/>
       <c r="E64" s="29"/>
@@ -3095,10 +3093,10 @@
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="35"/>
       <c r="B65" s="7" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>122</v>
+        <v>381</v>
       </c>
       <c r="D65" s="35"/>
       <c r="E65" s="29"/>
@@ -3113,10 +3111,10 @@
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="35"/>
       <c r="B66" s="7" t="s">
-        <v>143</v>
+        <v>106</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>198</v>
+        <v>382</v>
       </c>
       <c r="D66" s="35"/>
       <c r="E66" s="29"/>
@@ -3131,10 +3129,10 @@
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="35"/>
       <c r="B67" s="7" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>199</v>
+        <v>383</v>
       </c>
       <c r="D67" s="35"/>
       <c r="E67" s="29"/>
@@ -3149,10 +3147,10 @@
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="35"/>
       <c r="B68" s="7" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>200</v>
+        <v>384</v>
       </c>
       <c r="D68" s="35"/>
       <c r="E68" s="29"/>
@@ -3167,10 +3165,10 @@
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="35"/>
       <c r="B69" s="7" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>201</v>
+        <v>114</v>
       </c>
       <c r="D69" s="35"/>
       <c r="E69" s="29"/>
@@ -3185,10 +3183,10 @@
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="35"/>
       <c r="B70" s="7" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>202</v>
+        <v>115</v>
       </c>
       <c r="D70" s="35"/>
       <c r="E70" s="29"/>
@@ -3203,10 +3201,10 @@
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="35"/>
       <c r="B71" s="7" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>203</v>
+        <v>116</v>
       </c>
       <c r="D71" s="35"/>
       <c r="E71" s="29"/>
@@ -3221,10 +3219,10 @@
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="35"/>
       <c r="B72" s="7" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>206</v>
+        <v>119</v>
       </c>
       <c r="D72" s="35"/>
       <c r="E72" s="29"/>
@@ -3239,10 +3237,10 @@
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="35"/>
       <c r="B73" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="D73" s="35"/>
       <c r="E73" s="29"/>
@@ -3257,10 +3255,10 @@
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="35"/>
       <c r="B74" s="7" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>205</v>
+        <v>122</v>
       </c>
       <c r="D74" s="35"/>
       <c r="E74" s="29"/>
@@ -3275,10 +3273,10 @@
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="35"/>
       <c r="B75" s="7" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="D75" s="35"/>
       <c r="E75" s="29"/>
@@ -3293,10 +3291,10 @@
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="35"/>
       <c r="B76" s="7" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D76" s="35"/>
       <c r="E76" s="29"/>
@@ -3311,10 +3309,10 @@
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="35"/>
       <c r="B77" s="7" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="D77" s="35"/>
       <c r="E77" s="29"/>
@@ -3329,10 +3327,10 @@
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="35"/>
       <c r="B78" s="7" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D78" s="35"/>
       <c r="E78" s="29"/>
@@ -3347,10 +3345,10 @@
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="35"/>
       <c r="B79" s="7" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="D79" s="35"/>
       <c r="E79" s="29"/>
@@ -3365,10 +3363,10 @@
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="35"/>
       <c r="B80" s="7" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="D80" s="35"/>
       <c r="E80" s="29"/>
@@ -3380,43 +3378,49 @@
       </c>
       <c r="H80" s="35"/>
     </row>
-    <row r="81" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="35"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="12"/>
+      <c r="B81" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>206</v>
+      </c>
       <c r="D81" s="35"/>
-      <c r="E81" s="32"/>
-      <c r="F81" s="23"/>
-      <c r="G81" s="24"/>
+      <c r="E81" s="29"/>
+      <c r="F81" s="19">
+        <v>1</v>
+      </c>
+      <c r="G81" s="20">
+        <v>0</v>
+      </c>
       <c r="H81" s="35"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="35"/>
       <c r="B82" s="7" t="s">
-        <v>234</v>
+        <v>136</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="D82" s="35"/>
-      <c r="E82" s="29">
-        <v>44188</v>
-      </c>
+      <c r="E82" s="29"/>
       <c r="F82" s="19">
         <v>1</v>
       </c>
       <c r="G82" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82" s="35"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="35"/>
       <c r="B83" s="7" t="s">
-        <v>235</v>
+        <v>135</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
       <c r="D83" s="35"/>
       <c r="E83" s="29"/>
@@ -3431,10 +3435,10 @@
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="35"/>
       <c r="B84" s="7" t="s">
-        <v>236</v>
+        <v>134</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
       <c r="D84" s="35"/>
       <c r="E84" s="29"/>
@@ -3449,10 +3453,10 @@
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="35"/>
       <c r="B85" s="7" t="s">
-        <v>237</v>
+        <v>133</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="D85" s="35"/>
       <c r="E85" s="29"/>
@@ -3467,10 +3471,10 @@
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="35"/>
       <c r="B86" s="7" t="s">
-        <v>238</v>
+        <v>132</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>243</v>
+        <v>210</v>
       </c>
       <c r="D86" s="35"/>
       <c r="E86" s="29"/>
@@ -3482,23 +3486,31 @@
       </c>
       <c r="H86" s="35"/>
     </row>
-    <row r="87" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="35"/>
-      <c r="B87" s="11"/>
-      <c r="C87" s="12"/>
+      <c r="B87" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>211</v>
+      </c>
       <c r="D87" s="35"/>
-      <c r="E87" s="32"/>
-      <c r="F87" s="23"/>
-      <c r="G87" s="24"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="19">
+        <v>1</v>
+      </c>
+      <c r="G87" s="20">
+        <v>0</v>
+      </c>
       <c r="H87" s="35"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="35"/>
       <c r="B88" s="7" t="s">
-        <v>218</v>
+        <v>130</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="D88" s="35"/>
       <c r="E88" s="29"/>
@@ -3513,10 +3525,10 @@
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="35"/>
       <c r="B89" s="7" t="s">
-        <v>219</v>
+        <v>129</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="D89" s="35"/>
       <c r="E89" s="29"/>
@@ -3528,49 +3540,43 @@
       </c>
       <c r="H89" s="35"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="35"/>
-      <c r="B90" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>225</v>
-      </c>
+      <c r="B90" s="11"/>
+      <c r="C90" s="12"/>
       <c r="D90" s="35"/>
-      <c r="E90" s="29"/>
-      <c r="F90" s="19">
-        <v>1</v>
-      </c>
-      <c r="G90" s="20">
-        <v>0</v>
-      </c>
+      <c r="E90" s="32"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="24"/>
       <c r="H90" s="35"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="35"/>
       <c r="B91" s="7" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="D91" s="35"/>
-      <c r="E91" s="29"/>
+      <c r="E91" s="29">
+        <v>44188</v>
+      </c>
       <c r="F91" s="19">
         <v>1</v>
       </c>
       <c r="G91" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91" s="35"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="35"/>
       <c r="B92" s="7" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="D92" s="35"/>
       <c r="E92" s="29"/>
@@ -3582,23 +3588,31 @@
       </c>
       <c r="H92" s="35"/>
     </row>
-    <row r="93" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="35"/>
-      <c r="B93" s="11"/>
-      <c r="C93" s="12"/>
+      <c r="B93" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="D93" s="35"/>
-      <c r="E93" s="32"/>
-      <c r="F93" s="23"/>
-      <c r="G93" s="24"/>
+      <c r="E93" s="29"/>
+      <c r="F93" s="19">
+        <v>1</v>
+      </c>
+      <c r="G93" s="20">
+        <v>0</v>
+      </c>
       <c r="H93" s="35"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="35"/>
       <c r="B94" s="7" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="D94" s="35"/>
       <c r="E94" s="29"/>
@@ -3610,41 +3624,41 @@
       </c>
       <c r="H94" s="35"/>
     </row>
-    <row r="95" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="35"/>
-      <c r="B95" s="11"/>
-      <c r="C95" s="12"/>
+      <c r="B95" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>243</v>
+      </c>
       <c r="D95" s="35"/>
-      <c r="E95" s="32"/>
-      <c r="F95" s="23"/>
-      <c r="G95" s="24"/>
+      <c r="E95" s="29"/>
+      <c r="F95" s="19">
+        <v>1</v>
+      </c>
+      <c r="G95" s="20">
+        <v>0</v>
+      </c>
       <c r="H95" s="35"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="35"/>
-      <c r="B96" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>232</v>
-      </c>
+      <c r="B96" s="11"/>
+      <c r="C96" s="12"/>
       <c r="D96" s="35"/>
-      <c r="E96" s="29"/>
-      <c r="F96" s="19">
-        <v>1</v>
-      </c>
-      <c r="G96" s="20">
-        <v>0</v>
-      </c>
+      <c r="E96" s="32"/>
+      <c r="F96" s="23"/>
+      <c r="G96" s="24"/>
       <c r="H96" s="35"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="35"/>
       <c r="B97" s="7" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="D97" s="35"/>
       <c r="E97" s="29"/>
@@ -3656,23 +3670,31 @@
       </c>
       <c r="H97" s="35"/>
     </row>
-    <row r="98" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="35"/>
-      <c r="B98" s="11"/>
-      <c r="C98" s="12"/>
+      <c r="B98" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>224</v>
+      </c>
       <c r="D98" s="35"/>
-      <c r="E98" s="32"/>
-      <c r="F98" s="23"/>
-      <c r="G98" s="24"/>
+      <c r="E98" s="29"/>
+      <c r="F98" s="19">
+        <v>1</v>
+      </c>
+      <c r="G98" s="20">
+        <v>0</v>
+      </c>
       <c r="H98" s="35"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="35"/>
       <c r="B99" s="7" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="D99" s="35"/>
       <c r="E99" s="29"/>
@@ -3684,23 +3706,31 @@
       </c>
       <c r="H99" s="35"/>
     </row>
-    <row r="100" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="35"/>
-      <c r="B100" s="11"/>
-      <c r="C100" s="12"/>
+      <c r="B100" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>226</v>
+      </c>
       <c r="D100" s="35"/>
-      <c r="E100" s="32"/>
-      <c r="F100" s="23"/>
-      <c r="G100" s="24"/>
+      <c r="E100" s="29"/>
+      <c r="F100" s="19">
+        <v>1</v>
+      </c>
+      <c r="G100" s="20">
+        <v>0</v>
+      </c>
       <c r="H100" s="35"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="35"/>
       <c r="B101" s="7" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="D101" s="35"/>
       <c r="E101" s="29"/>
@@ -3712,31 +3742,23 @@
       </c>
       <c r="H101" s="35"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="35"/>
-      <c r="B102" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="C102" s="4" t="s">
-        <v>282</v>
-      </c>
+      <c r="B102" s="11"/>
+      <c r="C102" s="12"/>
       <c r="D102" s="35"/>
-      <c r="E102" s="29"/>
-      <c r="F102" s="19">
-        <v>1</v>
-      </c>
-      <c r="G102" s="20">
-        <v>0</v>
-      </c>
+      <c r="E102" s="32"/>
+      <c r="F102" s="23"/>
+      <c r="G102" s="24"/>
       <c r="H102" s="35"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="35"/>
       <c r="B103" s="7" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>284</v>
+        <v>229</v>
       </c>
       <c r="D103" s="35"/>
       <c r="E103" s="29"/>
@@ -3748,31 +3770,23 @@
       </c>
       <c r="H103" s="35"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>283</v>
-      </c>
+      <c r="B104" s="11"/>
+      <c r="C104" s="12"/>
       <c r="D104" s="35"/>
-      <c r="E104" s="29"/>
-      <c r="F104" s="19">
-        <v>1</v>
-      </c>
-      <c r="G104" s="20">
-        <v>0</v>
-      </c>
+      <c r="E104" s="32"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="24"/>
       <c r="H104" s="35"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="35"/>
       <c r="B105" s="7" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>285</v>
+        <v>232</v>
       </c>
       <c r="D105" s="35"/>
       <c r="E105" s="29"/>
@@ -3787,10 +3801,10 @@
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="35"/>
       <c r="B106" s="7" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
       <c r="D106" s="35"/>
       <c r="E106" s="29"/>
@@ -3802,31 +3816,23 @@
       </c>
       <c r="H106" s="35"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="35"/>
-      <c r="B107" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>264</v>
-      </c>
+      <c r="B107" s="11"/>
+      <c r="C107" s="12"/>
       <c r="D107" s="35"/>
-      <c r="E107" s="29"/>
-      <c r="F107" s="19">
-        <v>1</v>
-      </c>
-      <c r="G107" s="20">
-        <v>0</v>
-      </c>
+      <c r="E107" s="32"/>
+      <c r="F107" s="23"/>
+      <c r="G107" s="24"/>
       <c r="H107" s="35"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="35"/>
       <c r="B108" s="7" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>286</v>
+        <v>245</v>
       </c>
       <c r="D108" s="35"/>
       <c r="E108" s="29"/>
@@ -3838,31 +3844,23 @@
       </c>
       <c r="H108" s="35"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="35"/>
-      <c r="B109" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>287</v>
-      </c>
+      <c r="B109" s="11"/>
+      <c r="C109" s="12"/>
       <c r="D109" s="35"/>
-      <c r="E109" s="29"/>
-      <c r="F109" s="19">
-        <v>1</v>
-      </c>
-      <c r="G109" s="20">
-        <v>0</v>
-      </c>
+      <c r="E109" s="32"/>
+      <c r="F109" s="23"/>
+      <c r="G109" s="24"/>
       <c r="H109" s="35"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="35"/>
       <c r="B110" s="7" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="D110" s="35"/>
       <c r="E110" s="29"/>
@@ -3877,10 +3875,10 @@
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="35"/>
       <c r="B111" s="7" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>265</v>
+        <v>282</v>
       </c>
       <c r="D111" s="35"/>
       <c r="E111" s="29"/>
@@ -3895,10 +3893,10 @@
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="35"/>
       <c r="B112" s="7" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>266</v>
+        <v>284</v>
       </c>
       <c r="D112" s="35"/>
       <c r="E112" s="29"/>
@@ -3913,10 +3911,10 @@
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="35"/>
       <c r="B113" s="7" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="D113" s="35"/>
       <c r="E113" s="29"/>
@@ -3931,10 +3929,10 @@
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="35"/>
       <c r="B114" s="7" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="D114" s="35"/>
       <c r="E114" s="29"/>
@@ -3949,10 +3947,10 @@
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="35"/>
       <c r="B115" s="7" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D115" s="35"/>
       <c r="E115" s="29"/>
@@ -3967,10 +3965,10 @@
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="35"/>
       <c r="B116" s="7" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D116" s="35"/>
       <c r="E116" s="29"/>
@@ -3985,10 +3983,10 @@
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="35"/>
       <c r="B117" s="7" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="D117" s="35"/>
       <c r="E117" s="29"/>
@@ -4003,10 +4001,10 @@
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="35"/>
       <c r="B118" s="7" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="D118" s="35"/>
       <c r="E118" s="29"/>
@@ -4021,10 +4019,10 @@
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="35"/>
       <c r="B119" s="7" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="D119" s="35"/>
       <c r="E119" s="29"/>
@@ -4039,10 +4037,10 @@
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="35"/>
       <c r="B120" s="7" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D120" s="35"/>
       <c r="E120" s="29"/>
@@ -4057,10 +4055,10 @@
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="35"/>
       <c r="B121" s="7" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="D121" s="35"/>
       <c r="E121" s="29"/>
@@ -4072,23 +4070,31 @@
       </c>
       <c r="H121" s="35"/>
     </row>
-    <row r="122" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="35"/>
-      <c r="B122" s="11"/>
-      <c r="C122" s="12"/>
+      <c r="B122" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>272</v>
+      </c>
       <c r="D122" s="35"/>
-      <c r="E122" s="32"/>
-      <c r="F122" s="23"/>
-      <c r="G122" s="24"/>
+      <c r="E122" s="29"/>
+      <c r="F122" s="19">
+        <v>1</v>
+      </c>
+      <c r="G122" s="20">
+        <v>0</v>
+      </c>
       <c r="H122" s="35"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="35"/>
       <c r="B123" s="7" t="s">
-        <v>144</v>
+        <v>262</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>214</v>
+        <v>273</v>
       </c>
       <c r="D123" s="35"/>
       <c r="E123" s="29"/>
@@ -4103,10 +4109,10 @@
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="35"/>
       <c r="B124" s="7" t="s">
-        <v>215</v>
+        <v>267</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>216</v>
+        <v>260</v>
       </c>
       <c r="D124" s="35"/>
       <c r="E124" s="29"/>
@@ -4118,23 +4124,31 @@
       </c>
       <c r="H124" s="35"/>
     </row>
-    <row r="125" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="35"/>
-      <c r="B125" s="11"/>
-      <c r="C125" s="12"/>
+      <c r="B125" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>271</v>
+      </c>
       <c r="D125" s="35"/>
-      <c r="E125" s="32"/>
-      <c r="F125" s="23"/>
-      <c r="G125" s="24"/>
+      <c r="E125" s="29"/>
+      <c r="F125" s="19">
+        <v>1</v>
+      </c>
+      <c r="G125" s="20">
+        <v>0</v>
+      </c>
       <c r="H125" s="35"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="35"/>
       <c r="B126" s="7" t="s">
-        <v>288</v>
+        <v>269</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>296</v>
+        <v>270</v>
       </c>
       <c r="D126" s="35"/>
       <c r="E126" s="29"/>
@@ -4149,10 +4163,10 @@
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="35"/>
       <c r="B127" s="7" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="D127" s="35"/>
       <c r="E127" s="29"/>
@@ -4167,10 +4181,10 @@
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="35"/>
       <c r="B128" s="7" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="D128" s="35"/>
       <c r="E128" s="29"/>
@@ -4185,10 +4199,10 @@
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="35"/>
       <c r="B129" s="7" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="D129" s="35"/>
       <c r="E129" s="29"/>
@@ -4203,10 +4217,10 @@
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="35"/>
       <c r="B130" s="7" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="D130" s="35"/>
       <c r="E130" s="29"/>
@@ -4218,217 +4232,183 @@
       </c>
       <c r="H130" s="35"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="35"/>
-      <c r="B131" s="7"/>
-      <c r="C131" s="4"/>
+      <c r="B131" s="11"/>
+      <c r="C131" s="12"/>
       <c r="D131" s="35"/>
-      <c r="E131" s="29"/>
-      <c r="F131" s="19"/>
-      <c r="G131" s="20"/>
+      <c r="E131" s="32"/>
+      <c r="F131" s="23"/>
+      <c r="G131" s="24"/>
       <c r="H131" s="35"/>
     </row>
-    <row r="132" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="35"/>
-      <c r="B132" s="9"/>
-      <c r="C132" s="10"/>
+      <c r="B132" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>214</v>
+      </c>
       <c r="D132" s="35"/>
-      <c r="E132" s="30"/>
-      <c r="F132" s="21"/>
-      <c r="G132" s="22"/>
+      <c r="E132" s="29"/>
+      <c r="F132" s="19">
+        <v>1</v>
+      </c>
+      <c r="G132" s="20">
+        <v>0</v>
+      </c>
       <c r="H132" s="35"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="35"/>
       <c r="B133" s="7" t="s">
-        <v>52</v>
+        <v>215</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>53</v>
+        <v>216</v>
       </c>
       <c r="D133" s="35"/>
-      <c r="E133" s="29">
-        <v>44207</v>
-      </c>
+      <c r="E133" s="29"/>
       <c r="F133" s="19">
         <v>1</v>
       </c>
       <c r="G133" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H133" s="35"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="35"/>
-      <c r="B134" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C134" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="B134" s="11"/>
+      <c r="C134" s="12"/>
       <c r="D134" s="35"/>
-      <c r="E134" s="29">
-        <v>44211</v>
-      </c>
-      <c r="F134" s="19">
-        <v>1</v>
-      </c>
-      <c r="G134" s="20">
-        <v>1</v>
-      </c>
+      <c r="E134" s="32"/>
+      <c r="F134" s="23"/>
+      <c r="G134" s="24"/>
       <c r="H134" s="35"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="35"/>
       <c r="B135" s="7" t="s">
-        <v>57</v>
+        <v>288</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>56</v>
+        <v>296</v>
       </c>
       <c r="D135" s="35"/>
-      <c r="E135" s="29">
-        <v>44211</v>
-      </c>
+      <c r="E135" s="29"/>
       <c r="F135" s="19">
         <v>1</v>
       </c>
       <c r="G135" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H135" s="35"/>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="35"/>
       <c r="B136" s="7" t="s">
-        <v>58</v>
+        <v>289</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>59</v>
+        <v>290</v>
       </c>
       <c r="D136" s="35"/>
-      <c r="E136" s="29">
-        <v>44211</v>
-      </c>
+      <c r="E136" s="29"/>
       <c r="F136" s="19">
         <v>1</v>
       </c>
       <c r="G136" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H136" s="35"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="35"/>
       <c r="B137" s="7" t="s">
-        <v>60</v>
+        <v>291</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>65</v>
+        <v>297</v>
       </c>
       <c r="D137" s="35"/>
-      <c r="E137" s="29">
-        <v>44211</v>
-      </c>
+      <c r="E137" s="29"/>
       <c r="F137" s="19">
         <v>1</v>
       </c>
       <c r="G137" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H137" s="35"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="35"/>
       <c r="B138" s="7" t="s">
-        <v>61</v>
+        <v>292</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>64</v>
+        <v>293</v>
       </c>
       <c r="D138" s="35"/>
-      <c r="E138" s="29">
-        <v>44211</v>
-      </c>
+      <c r="E138" s="29"/>
       <c r="F138" s="19">
         <v>1</v>
       </c>
       <c r="G138" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H138" s="35"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="35"/>
       <c r="B139" s="7" t="s">
-        <v>62</v>
+        <v>294</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>67</v>
+        <v>295</v>
       </c>
       <c r="D139" s="35"/>
-      <c r="E139" s="29">
-        <v>44211</v>
-      </c>
+      <c r="E139" s="29"/>
       <c r="F139" s="19">
         <v>1</v>
       </c>
       <c r="G139" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H139" s="35"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="35"/>
-      <c r="B140" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C140" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="B140" s="7"/>
+      <c r="C140" s="4"/>
       <c r="D140" s="35"/>
-      <c r="E140" s="29">
-        <v>44211</v>
-      </c>
-      <c r="F140" s="19">
-        <v>1</v>
-      </c>
-      <c r="G140" s="20">
-        <v>1</v>
-      </c>
+      <c r="E140" s="29"/>
+      <c r="F140" s="19"/>
+      <c r="G140" s="20"/>
       <c r="H140" s="35"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="35"/>
-      <c r="B141" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C141" s="4" t="s">
-        <v>80</v>
-      </c>
+      <c r="B141" s="9"/>
+      <c r="C141" s="10"/>
       <c r="D141" s="35"/>
-      <c r="E141" s="29">
-        <v>44211</v>
-      </c>
-      <c r="F141" s="19">
-        <v>1</v>
-      </c>
-      <c r="G141" s="20">
-        <v>1</v>
-      </c>
+      <c r="E141" s="30"/>
+      <c r="F141" s="21"/>
+      <c r="G141" s="22"/>
       <c r="H141" s="35"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="35"/>
       <c r="B142" s="7" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="D142" s="35"/>
       <c r="E142" s="29">
-        <v>44211</v>
+        <v>44207</v>
       </c>
       <c r="F142" s="19">
         <v>1</v>
@@ -4441,10 +4421,10 @@
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="35"/>
       <c r="B143" s="7" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="D143" s="35"/>
       <c r="E143" s="29">
@@ -4461,10 +4441,10 @@
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="35"/>
       <c r="B144" s="7" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="D144" s="35"/>
       <c r="E144" s="29">
@@ -4481,10 +4461,10 @@
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="35"/>
       <c r="B145" s="7" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="D145" s="35"/>
       <c r="E145" s="29">
@@ -4501,10 +4481,10 @@
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="35"/>
       <c r="B146" s="7" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="D146" s="35"/>
       <c r="E146" s="29">
@@ -4521,10 +4501,10 @@
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="35"/>
       <c r="B147" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="D147" s="35"/>
       <c r="E147" s="29">
@@ -4541,10 +4521,10 @@
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="35"/>
       <c r="B148" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>207</v>
+        <v>67</v>
       </c>
       <c r="D148" s="35"/>
       <c r="E148" s="29">
@@ -4561,10 +4541,10 @@
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="35"/>
       <c r="B149" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="D149" s="35"/>
       <c r="E149" s="29">
@@ -4581,10 +4561,10 @@
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="35"/>
       <c r="B150" s="7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D150" s="35"/>
       <c r="E150" s="29">
@@ -4601,10 +4581,10 @@
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="35"/>
       <c r="B151" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D151" s="35"/>
       <c r="E151" s="29">
@@ -4621,10 +4601,10 @@
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="35"/>
       <c r="B152" s="7" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D152" s="35"/>
       <c r="E152" s="29">
@@ -4640,193 +4620,211 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="35"/>
-      <c r="B153" s="7"/>
-      <c r="C153" s="4"/>
+      <c r="B153" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="D153" s="35"/>
-      <c r="E153" s="29"/>
-      <c r="F153" s="19"/>
-      <c r="G153" s="20"/>
+      <c r="E153" s="29">
+        <v>44211</v>
+      </c>
+      <c r="F153" s="19">
+        <v>1</v>
+      </c>
+      <c r="G153" s="20">
+        <v>1</v>
+      </c>
       <c r="H153" s="35"/>
     </row>
-    <row r="154" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="35"/>
-      <c r="B154" s="9"/>
-      <c r="C154" s="10"/>
+      <c r="B154" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="D154" s="35"/>
-      <c r="E154" s="30"/>
-      <c r="F154" s="21"/>
-      <c r="G154" s="22"/>
+      <c r="E154" s="29">
+        <v>44211</v>
+      </c>
+      <c r="F154" s="19">
+        <v>1</v>
+      </c>
+      <c r="G154" s="20">
+        <v>1</v>
+      </c>
       <c r="H154" s="35"/>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="35"/>
       <c r="B155" s="7" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="D155" s="35"/>
-      <c r="E155" s="29"/>
+      <c r="E155" s="29">
+        <v>44211</v>
+      </c>
       <c r="F155" s="19">
         <v>1</v>
       </c>
       <c r="G155" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H155" s="35"/>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="35"/>
       <c r="B156" s="7" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="D156" s="35"/>
-      <c r="E156" s="29"/>
+      <c r="E156" s="29">
+        <v>44211</v>
+      </c>
       <c r="F156" s="19">
         <v>1</v>
       </c>
       <c r="G156" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H156" s="35"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="35"/>
       <c r="B157" s="7" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>18</v>
+        <v>207</v>
       </c>
       <c r="D157" s="35"/>
-      <c r="E157" s="29"/>
+      <c r="E157" s="29">
+        <v>44211</v>
+      </c>
       <c r="F157" s="19">
         <v>1</v>
       </c>
       <c r="G157" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H157" s="35"/>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="35"/>
       <c r="B158" s="7" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="D158" s="35"/>
-      <c r="E158" s="29"/>
+      <c r="E158" s="29">
+        <v>44211</v>
+      </c>
       <c r="F158" s="19">
         <v>1</v>
       </c>
       <c r="G158" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H158" s="35"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="35"/>
       <c r="B159" s="7" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="D159" s="35"/>
-      <c r="E159" s="29"/>
+      <c r="E159" s="29">
+        <v>44211</v>
+      </c>
       <c r="F159" s="19">
         <v>1</v>
       </c>
       <c r="G159" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H159" s="35"/>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="35"/>
       <c r="B160" s="7" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="D160" s="35"/>
-      <c r="E160" s="29"/>
+      <c r="E160" s="29">
+        <v>44211</v>
+      </c>
       <c r="F160" s="19">
         <v>1</v>
       </c>
       <c r="G160" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H160" s="35"/>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="35"/>
       <c r="B161" s="7" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="D161" s="35"/>
-      <c r="E161" s="29"/>
+      <c r="E161" s="29">
+        <v>44211</v>
+      </c>
       <c r="F161" s="19">
         <v>1</v>
       </c>
       <c r="G161" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H161" s="35"/>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="35"/>
-      <c r="B162" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C162" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="B162" s="7"/>
+      <c r="C162" s="4"/>
       <c r="D162" s="35"/>
       <c r="E162" s="29"/>
-      <c r="F162" s="19">
-        <v>1</v>
-      </c>
-      <c r="G162" s="20">
-        <v>0</v>
-      </c>
+      <c r="F162" s="19"/>
+      <c r="G162" s="20"/>
       <c r="H162" s="35"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="35"/>
-      <c r="B163" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C163" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="B163" s="9"/>
+      <c r="C163" s="10"/>
       <c r="D163" s="35"/>
-      <c r="E163" s="29"/>
-      <c r="F163" s="19">
-        <v>1</v>
-      </c>
-      <c r="G163" s="20">
-        <v>0</v>
-      </c>
+      <c r="E163" s="30"/>
+      <c r="F163" s="21"/>
+      <c r="G163" s="22"/>
       <c r="H163" s="35"/>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="35"/>
       <c r="B164" s="7" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D164" s="35"/>
       <c r="E164" s="29"/>
@@ -4841,10 +4839,10 @@
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="35"/>
       <c r="B165" s="7" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D165" s="35"/>
       <c r="E165" s="29"/>
@@ -4859,10 +4857,10 @@
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="35"/>
       <c r="B166" s="7" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="D166" s="35"/>
       <c r="E166" s="29"/>
@@ -4877,10 +4875,10 @@
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="35"/>
       <c r="B167" s="7" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D167" s="35"/>
       <c r="E167" s="29"/>
@@ -4895,10 +4893,10 @@
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="35"/>
       <c r="B168" s="7" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D168" s="35"/>
       <c r="E168" s="29"/>
@@ -4913,10 +4911,10 @@
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="35"/>
       <c r="B169" s="7" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D169" s="35"/>
       <c r="E169" s="29"/>
@@ -4931,10 +4929,10 @@
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="35"/>
       <c r="B170" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C170" s="5" t="s">
-        <v>44</v>
+        <v>28</v>
+      </c>
+      <c r="C170" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="D170" s="35"/>
       <c r="E170" s="29"/>
@@ -4949,10 +4947,10 @@
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="35"/>
       <c r="B171" s="7" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="D171" s="35"/>
       <c r="E171" s="29"/>
@@ -4967,10 +4965,10 @@
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="35"/>
       <c r="B172" s="7" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D172" s="35"/>
       <c r="E172" s="29"/>
@@ -4985,10 +4983,10 @@
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="35"/>
       <c r="B173" s="7" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D173" s="35"/>
       <c r="E173" s="29"/>
@@ -5002,31 +5000,47 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="35"/>
-      <c r="B174" s="7"/>
-      <c r="C174" s="4"/>
+      <c r="B174" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="D174" s="35"/>
       <c r="E174" s="29"/>
-      <c r="F174" s="19"/>
-      <c r="G174" s="20"/>
+      <c r="F174" s="19">
+        <v>1</v>
+      </c>
+      <c r="G174" s="20">
+        <v>0</v>
+      </c>
       <c r="H174" s="35"/>
     </row>
-    <row r="175" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="35"/>
-      <c r="B175" s="9"/>
-      <c r="C175" s="10"/>
+      <c r="B175" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="D175" s="35"/>
-      <c r="E175" s="30"/>
-      <c r="F175" s="21"/>
-      <c r="G175" s="22"/>
+      <c r="E175" s="29"/>
+      <c r="F175" s="19">
+        <v>1</v>
+      </c>
+      <c r="G175" s="20">
+        <v>0</v>
+      </c>
       <c r="H175" s="35"/>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="35"/>
       <c r="B176" s="7" t="s">
-        <v>309</v>
+        <v>37</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>310</v>
+        <v>38</v>
       </c>
       <c r="D176" s="35"/>
       <c r="E176" s="29"/>
@@ -5038,23 +5052,31 @@
       </c>
       <c r="H176" s="35"/>
     </row>
-    <row r="177" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="35"/>
-      <c r="B177" s="11"/>
-      <c r="C177" s="12"/>
+      <c r="B177" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D177" s="35"/>
-      <c r="E177" s="32"/>
-      <c r="F177" s="23"/>
-      <c r="G177" s="24"/>
+      <c r="E177" s="29"/>
+      <c r="F177" s="19">
+        <v>1</v>
+      </c>
+      <c r="G177" s="20">
+        <v>0</v>
+      </c>
       <c r="H177" s="35"/>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="35"/>
       <c r="B178" s="7" t="s">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>103</v>
+        <v>42</v>
       </c>
       <c r="D178" s="35"/>
       <c r="E178" s="29"/>
@@ -5068,31 +5090,47 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="35"/>
-      <c r="B179" s="7"/>
-      <c r="C179" s="4"/>
+      <c r="B179" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="D179" s="35"/>
       <c r="E179" s="29"/>
-      <c r="F179" s="19"/>
-      <c r="G179" s="20"/>
+      <c r="F179" s="19">
+        <v>1</v>
+      </c>
+      <c r="G179" s="20">
+        <v>0</v>
+      </c>
       <c r="H179" s="35"/>
     </row>
-    <row r="180" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="35"/>
-      <c r="B180" s="9"/>
-      <c r="C180" s="10"/>
+      <c r="B180" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="D180" s="35"/>
-      <c r="E180" s="30"/>
-      <c r="F180" s="21"/>
-      <c r="G180" s="22"/>
+      <c r="E180" s="29"/>
+      <c r="F180" s="19">
+        <v>1</v>
+      </c>
+      <c r="G180" s="20">
+        <v>0</v>
+      </c>
       <c r="H180" s="35"/>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="35"/>
       <c r="B181" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="D181" s="35"/>
       <c r="E181" s="29"/>
@@ -5107,10 +5145,10 @@
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="35"/>
       <c r="B182" s="7" t="s">
-        <v>164</v>
+        <v>48</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>145</v>
+        <v>49</v>
       </c>
       <c r="D182" s="35"/>
       <c r="E182" s="29"/>
@@ -5124,47 +5162,31 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="35"/>
-      <c r="B183" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="C183" s="4" t="s">
-        <v>316</v>
-      </c>
+      <c r="B183" s="7"/>
+      <c r="C183" s="4"/>
       <c r="D183" s="35"/>
       <c r="E183" s="29"/>
-      <c r="F183" s="19">
-        <v>1</v>
-      </c>
-      <c r="G183" s="20">
-        <v>0</v>
-      </c>
+      <c r="F183" s="19"/>
+      <c r="G183" s="20"/>
       <c r="H183" s="35"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="35"/>
-      <c r="B184" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C184" s="4" t="s">
-        <v>146</v>
-      </c>
+      <c r="B184" s="9"/>
+      <c r="C184" s="10"/>
       <c r="D184" s="35"/>
-      <c r="E184" s="29"/>
-      <c r="F184" s="19">
-        <v>1</v>
-      </c>
-      <c r="G184" s="20">
-        <v>0</v>
-      </c>
+      <c r="E184" s="30"/>
+      <c r="F184" s="21"/>
+      <c r="G184" s="22"/>
       <c r="H184" s="35"/>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="35"/>
       <c r="B185" s="7" t="s">
-        <v>166</v>
+        <v>309</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>147</v>
+        <v>310</v>
       </c>
       <c r="D185" s="35"/>
       <c r="E185" s="29"/>
@@ -5176,31 +5198,23 @@
       </c>
       <c r="H185" s="35"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="35"/>
-      <c r="B186" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C186" s="4" t="s">
-        <v>148</v>
-      </c>
+      <c r="B186" s="11"/>
+      <c r="C186" s="12"/>
       <c r="D186" s="35"/>
-      <c r="E186" s="29"/>
-      <c r="F186" s="19">
-        <v>1</v>
-      </c>
-      <c r="G186" s="20">
-        <v>0</v>
-      </c>
+      <c r="E186" s="32"/>
+      <c r="F186" s="23"/>
+      <c r="G186" s="24"/>
       <c r="H186" s="35"/>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="35"/>
       <c r="B187" s="7" t="s">
-        <v>168</v>
+        <v>102</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
       <c r="D187" s="35"/>
       <c r="E187" s="29"/>
@@ -5214,47 +5228,31 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="35"/>
-      <c r="B188" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C188" s="4" t="s">
-        <v>150</v>
-      </c>
+      <c r="B188" s="7"/>
+      <c r="C188" s="4"/>
       <c r="D188" s="35"/>
       <c r="E188" s="29"/>
-      <c r="F188" s="19">
-        <v>1</v>
-      </c>
-      <c r="G188" s="20">
-        <v>0</v>
-      </c>
+      <c r="F188" s="19"/>
+      <c r="G188" s="20"/>
       <c r="H188" s="35"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="35"/>
-      <c r="B189" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C189" s="4" t="s">
-        <v>151</v>
-      </c>
+      <c r="B189" s="9"/>
+      <c r="C189" s="10"/>
       <c r="D189" s="35"/>
-      <c r="E189" s="29"/>
-      <c r="F189" s="19">
-        <v>1</v>
-      </c>
-      <c r="G189" s="20">
-        <v>0</v>
-      </c>
+      <c r="E189" s="30"/>
+      <c r="F189" s="21"/>
+      <c r="G189" s="22"/>
       <c r="H189" s="35"/>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="35"/>
       <c r="B190" s="7" t="s">
-        <v>171</v>
+        <v>51</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>152</v>
+        <v>93</v>
       </c>
       <c r="D190" s="35"/>
       <c r="E190" s="29"/>
@@ -5269,10 +5267,10 @@
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="35"/>
       <c r="B191" s="7" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D191" s="35"/>
       <c r="E191" s="29"/>
@@ -5287,10 +5285,10 @@
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="35"/>
       <c r="B192" s="7" t="s">
-        <v>173</v>
+        <v>315</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>154</v>
+        <v>316</v>
       </c>
       <c r="D192" s="35"/>
       <c r="E192" s="29"/>
@@ -5305,10 +5303,10 @@
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="35"/>
       <c r="B193" s="7" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D193" s="35"/>
       <c r="E193" s="29"/>
@@ -5323,10 +5321,10 @@
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="35"/>
       <c r="B194" s="7" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D194" s="35"/>
       <c r="E194" s="29"/>
@@ -5341,10 +5339,10 @@
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="35"/>
       <c r="B195" s="7" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D195" s="35"/>
       <c r="E195" s="29"/>
@@ -5359,10 +5357,10 @@
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="35"/>
       <c r="B196" s="7" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D196" s="35"/>
       <c r="E196" s="29"/>
@@ -5377,10 +5375,10 @@
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="35"/>
       <c r="B197" s="7" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D197" s="35"/>
       <c r="E197" s="29"/>
@@ -5395,10 +5393,10 @@
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="35"/>
       <c r="B198" s="7" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D198" s="35"/>
       <c r="E198" s="29"/>
@@ -5413,10 +5411,10 @@
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="35"/>
       <c r="B199" s="7" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D199" s="35"/>
       <c r="E199" s="29"/>
@@ -5431,10 +5429,10 @@
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="35"/>
       <c r="B200" s="7" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D200" s="35"/>
       <c r="E200" s="29"/>
@@ -5449,10 +5447,10 @@
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="35"/>
       <c r="B201" s="7" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D201" s="35"/>
       <c r="E201" s="29"/>
@@ -5467,10 +5465,10 @@
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="35"/>
       <c r="B202" s="7" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D202" s="35"/>
       <c r="E202" s="29"/>
@@ -5485,10 +5483,10 @@
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="35"/>
       <c r="B203" s="7" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D203" s="35"/>
       <c r="E203" s="29"/>
@@ -5503,10 +5501,10 @@
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="35"/>
       <c r="B204" s="7" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D204" s="35"/>
       <c r="E204" s="29"/>
@@ -5521,10 +5519,10 @@
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="35"/>
       <c r="B205" s="7" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D205" s="35"/>
       <c r="E205" s="29"/>
@@ -5539,10 +5537,10 @@
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="35"/>
       <c r="B206" s="7" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D206" s="35"/>
       <c r="E206" s="29"/>
@@ -5557,10 +5555,10 @@
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="35"/>
       <c r="B207" s="7" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D207" s="35"/>
       <c r="E207" s="29"/>
@@ -5575,10 +5573,10 @@
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="35"/>
       <c r="B208" s="7" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D208" s="35"/>
       <c r="E208" s="29"/>
@@ -5593,10 +5591,10 @@
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="35"/>
       <c r="B209" s="7" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D209" s="35"/>
       <c r="E209" s="29"/>
@@ -5611,7 +5609,7 @@
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="35"/>
       <c r="B210" s="7" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C210" s="4" t="s">
         <v>163</v>
@@ -5629,7 +5627,7 @@
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="35"/>
       <c r="B211" s="7" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C211" s="4" t="s">
         <v>163</v>
@@ -5647,7 +5645,7 @@
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="35"/>
       <c r="B212" s="7" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C212" s="4" t="s">
         <v>163</v>
@@ -5665,7 +5663,7 @@
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="35"/>
       <c r="B213" s="7" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C213" s="4" t="s">
         <v>163</v>
@@ -5683,7 +5681,7 @@
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="35"/>
       <c r="B214" s="7" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C214" s="4" t="s">
         <v>163</v>
@@ -5701,7 +5699,7 @@
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="35"/>
       <c r="B215" s="7" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C215" s="4" t="s">
         <v>163</v>
@@ -5719,7 +5717,7 @@
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="35"/>
       <c r="B216" s="7" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C216" s="4" t="s">
         <v>163</v>
@@ -5737,7 +5735,7 @@
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="35"/>
       <c r="B217" s="7" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="C217" s="4" t="s">
         <v>163</v>
@@ -5754,31 +5752,47 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="35"/>
-      <c r="B218" s="7"/>
-      <c r="C218" s="4"/>
+      <c r="B218" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C218" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="D218" s="35"/>
       <c r="E218" s="29"/>
-      <c r="F218" s="19"/>
-      <c r="G218" s="20"/>
+      <c r="F218" s="19">
+        <v>1</v>
+      </c>
+      <c r="G218" s="20">
+        <v>0</v>
+      </c>
       <c r="H218" s="35"/>
     </row>
-    <row r="219" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="35"/>
-      <c r="B219" s="9"/>
-      <c r="C219" s="10"/>
+      <c r="B219" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C219" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="D219" s="35"/>
-      <c r="E219" s="30"/>
-      <c r="F219" s="21"/>
-      <c r="G219" s="22"/>
+      <c r="E219" s="29"/>
+      <c r="F219" s="19">
+        <v>1</v>
+      </c>
+      <c r="G219" s="20">
+        <v>0</v>
+      </c>
       <c r="H219" s="35"/>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="35"/>
       <c r="B220" s="7" t="s">
-        <v>0</v>
+        <v>192</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="D220" s="35"/>
       <c r="E220" s="29"/>
@@ -5793,10 +5807,10 @@
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="35"/>
       <c r="B221" s="7" t="s">
-        <v>325</v>
+        <v>193</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>327</v>
+        <v>163</v>
       </c>
       <c r="D221" s="35"/>
       <c r="E221" s="29"/>
@@ -5811,10 +5825,10 @@
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="35"/>
       <c r="B222" s="7" t="s">
-        <v>326</v>
+        <v>194</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>328</v>
+        <v>163</v>
       </c>
       <c r="D222" s="35"/>
       <c r="E222" s="29"/>
@@ -5829,10 +5843,10 @@
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="35"/>
       <c r="B223" s="7" t="s">
-        <v>319</v>
+        <v>195</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>320</v>
+        <v>163</v>
       </c>
       <c r="D223" s="35"/>
       <c r="E223" s="29"/>
@@ -5844,103 +5858,87 @@
       </c>
       <c r="H223" s="35"/>
     </row>
-    <row r="224" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A224" s="37"/>
-      <c r="B224" s="13" t="s">
-        <v>369</v>
-      </c>
-      <c r="C224" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="D224" s="37"/>
-      <c r="E224" s="31"/>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A224" s="35"/>
+      <c r="B224" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C224" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D224" s="35"/>
+      <c r="E224" s="29"/>
       <c r="F224" s="19">
         <v>1</v>
       </c>
       <c r="G224" s="20">
         <v>0</v>
       </c>
-      <c r="H224" s="37"/>
-    </row>
-    <row r="225" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="37"/>
-      <c r="B225" s="13" t="s">
-        <v>370</v>
-      </c>
-      <c r="C225" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="D225" s="37"/>
-      <c r="E225" s="31"/>
+      <c r="H224" s="35"/>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A225" s="35"/>
+      <c r="B225" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C225" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D225" s="35"/>
+      <c r="E225" s="29"/>
       <c r="F225" s="19">
         <v>1</v>
       </c>
       <c r="G225" s="20">
         <v>0</v>
       </c>
-      <c r="H225" s="37"/>
-    </row>
-    <row r="226" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="37"/>
-      <c r="B226" s="13" t="s">
-        <v>371</v>
-      </c>
-      <c r="C226" s="14" t="s">
-        <v>375</v>
-      </c>
-      <c r="D226" s="37"/>
-      <c r="E226" s="31"/>
+      <c r="H225" s="35"/>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A226" s="35"/>
+      <c r="B226" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C226" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D226" s="35"/>
+      <c r="E226" s="29"/>
       <c r="F226" s="19">
         <v>1</v>
       </c>
       <c r="G226" s="20">
         <v>0</v>
       </c>
-      <c r="H226" s="37"/>
-    </row>
-    <row r="227" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="37"/>
-      <c r="B227" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="C227" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="D227" s="37"/>
-      <c r="E227" s="31"/>
-      <c r="F227" s="19">
-        <v>1</v>
-      </c>
-      <c r="G227" s="20">
-        <v>0</v>
-      </c>
-      <c r="H227" s="37"/>
-    </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H226" s="35"/>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A227" s="35"/>
+      <c r="B227" s="7"/>
+      <c r="C227" s="4"/>
+      <c r="D227" s="35"/>
+      <c r="E227" s="29"/>
+      <c r="F227" s="19"/>
+      <c r="G227" s="20"/>
+      <c r="H227" s="35"/>
+    </row>
+    <row r="228" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="35"/>
-      <c r="B228" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="C228" s="4" t="s">
-        <v>357</v>
-      </c>
+      <c r="B228" s="9"/>
+      <c r="C228" s="10"/>
       <c r="D228" s="35"/>
-      <c r="E228" s="29"/>
-      <c r="F228" s="19">
-        <v>1</v>
-      </c>
-      <c r="G228" s="20">
-        <v>0</v>
-      </c>
+      <c r="E228" s="30"/>
+      <c r="F228" s="21"/>
+      <c r="G228" s="22"/>
       <c r="H228" s="35"/>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="35"/>
       <c r="B229" s="7" t="s">
-        <v>354</v>
+        <v>0</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>356</v>
+        <v>104</v>
       </c>
       <c r="D229" s="35"/>
       <c r="E229" s="29"/>
@@ -5955,10 +5953,10 @@
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="35"/>
       <c r="B230" s="7" t="s">
-        <v>355</v>
+        <v>325</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>358</v>
+        <v>327</v>
       </c>
       <c r="D230" s="35"/>
       <c r="E230" s="29"/>
@@ -5973,10 +5971,10 @@
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="35"/>
       <c r="B231" s="7" t="s">
-        <v>349</v>
+        <v>326</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="D231" s="35"/>
       <c r="E231" s="29"/>
@@ -5991,10 +5989,10 @@
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="35"/>
       <c r="B232" s="7" t="s">
-        <v>348</v>
+        <v>319</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>351</v>
+        <v>320</v>
       </c>
       <c r="D232" s="35"/>
       <c r="E232" s="29"/>
@@ -6006,97 +6004,259 @@
       </c>
       <c r="H232" s="35"/>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A233" s="35"/>
-      <c r="B233" s="7" t="s">
+    <row r="233" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="37"/>
+      <c r="B233" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="C233" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="D233" s="37"/>
+      <c r="E233" s="31"/>
+      <c r="F233" s="19">
+        <v>1</v>
+      </c>
+      <c r="G233" s="20">
+        <v>0</v>
+      </c>
+      <c r="H233" s="37"/>
+    </row>
+    <row r="234" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="37"/>
+      <c r="B234" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="C234" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="D234" s="37"/>
+      <c r="E234" s="31"/>
+      <c r="F234" s="19">
+        <v>1</v>
+      </c>
+      <c r="G234" s="20">
+        <v>0</v>
+      </c>
+      <c r="H234" s="37"/>
+    </row>
+    <row r="235" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="37"/>
+      <c r="B235" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="C235" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="D235" s="37"/>
+      <c r="E235" s="31"/>
+      <c r="F235" s="19">
+        <v>1</v>
+      </c>
+      <c r="G235" s="20">
+        <v>0</v>
+      </c>
+      <c r="H235" s="37"/>
+    </row>
+    <row r="236" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="37"/>
+      <c r="B236" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="C236" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="D236" s="37"/>
+      <c r="E236" s="31"/>
+      <c r="F236" s="19">
+        <v>1</v>
+      </c>
+      <c r="G236" s="20">
+        <v>0</v>
+      </c>
+      <c r="H236" s="37"/>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A237" s="35"/>
+      <c r="B237" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="C237" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="D237" s="35"/>
+      <c r="E237" s="29"/>
+      <c r="F237" s="19">
+        <v>1</v>
+      </c>
+      <c r="G237" s="20">
+        <v>0</v>
+      </c>
+      <c r="H237" s="35"/>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A238" s="35"/>
+      <c r="B238" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C238" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D238" s="35"/>
+      <c r="E238" s="29"/>
+      <c r="F238" s="19">
+        <v>1</v>
+      </c>
+      <c r="G238" s="20">
+        <v>0</v>
+      </c>
+      <c r="H238" s="35"/>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A239" s="35"/>
+      <c r="B239" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="C239" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="D239" s="35"/>
+      <c r="E239" s="29"/>
+      <c r="F239" s="19">
+        <v>1</v>
+      </c>
+      <c r="G239" s="20">
+        <v>0</v>
+      </c>
+      <c r="H239" s="35"/>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A240" s="35"/>
+      <c r="B240" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C240" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="D240" s="35"/>
+      <c r="E240" s="29"/>
+      <c r="F240" s="19">
+        <v>1</v>
+      </c>
+      <c r="G240" s="20">
+        <v>0</v>
+      </c>
+      <c r="H240" s="35"/>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A241" s="35"/>
+      <c r="B241" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C241" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="D241" s="35"/>
+      <c r="E241" s="29"/>
+      <c r="F241" s="19">
+        <v>1</v>
+      </c>
+      <c r="G241" s="20">
+        <v>0</v>
+      </c>
+      <c r="H241" s="35"/>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A242" s="35"/>
+      <c r="B242" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="C233" s="4" t="s">
+      <c r="C242" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="D233" s="35"/>
-      <c r="E233" s="29"/>
-      <c r="F233" s="19">
-        <v>1</v>
-      </c>
-      <c r="G233" s="20">
-        <v>0</v>
-      </c>
-      <c r="H233" s="35"/>
-    </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A234" s="35"/>
-      <c r="B234" s="7" t="s">
+      <c r="D242" s="35"/>
+      <c r="E242" s="29"/>
+      <c r="F242" s="19">
+        <v>1</v>
+      </c>
+      <c r="G242" s="20">
+        <v>0</v>
+      </c>
+      <c r="H242" s="35"/>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A243" s="35"/>
+      <c r="B243" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="C234" s="4" t="s">
+      <c r="C243" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="D234" s="35"/>
-      <c r="E234" s="29"/>
-      <c r="F234" s="19">
-        <v>1</v>
-      </c>
-      <c r="G234" s="20">
-        <v>0</v>
-      </c>
-      <c r="H234" s="35"/>
-    </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A235" s="35"/>
-      <c r="B235" s="7" t="s">
+      <c r="D243" s="35"/>
+      <c r="E243" s="29"/>
+      <c r="F243" s="19">
+        <v>1</v>
+      </c>
+      <c r="G243" s="20">
+        <v>0</v>
+      </c>
+      <c r="H243" s="35"/>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A244" s="35"/>
+      <c r="B244" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="C235" s="4" t="s">
+      <c r="C244" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="D235" s="35"/>
-      <c r="E235" s="29"/>
-      <c r="F235" s="19">
-        <v>1</v>
-      </c>
-      <c r="G235" s="20">
-        <v>0</v>
-      </c>
-      <c r="H235" s="35"/>
-    </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A236" s="35"/>
-      <c r="B236" s="7" t="s">
+      <c r="D244" s="35"/>
+      <c r="E244" s="29"/>
+      <c r="F244" s="19">
+        <v>1</v>
+      </c>
+      <c r="G244" s="20">
+        <v>0</v>
+      </c>
+      <c r="H244" s="35"/>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A245" s="35"/>
+      <c r="B245" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="C236" s="4" t="s">
+      <c r="C245" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="D236" s="35"/>
-      <c r="E236" s="29"/>
-      <c r="F236" s="19">
-        <v>1</v>
-      </c>
-      <c r="G236" s="20">
-        <v>0</v>
-      </c>
-      <c r="H236" s="35"/>
-    </row>
-    <row r="237" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="35"/>
-      <c r="B237" s="8"/>
-      <c r="C237" s="6"/>
-      <c r="D237" s="35"/>
-      <c r="E237" s="33"/>
-      <c r="F237" s="25"/>
-      <c r="G237" s="26"/>
-      <c r="H237" s="35"/>
-    </row>
-    <row r="238" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="35"/>
-      <c r="B238" s="38"/>
-      <c r="C238" s="39"/>
-      <c r="D238" s="35"/>
-      <c r="E238" s="40"/>
-      <c r="F238" s="41"/>
-      <c r="G238" s="41"/>
-      <c r="H238" s="35"/>
+      <c r="D245" s="35"/>
+      <c r="E245" s="29"/>
+      <c r="F245" s="19">
+        <v>1</v>
+      </c>
+      <c r="G245" s="20">
+        <v>0</v>
+      </c>
+      <c r="H245" s="35"/>
+    </row>
+    <row r="246" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A246" s="35"/>
+      <c r="B246" s="8"/>
+      <c r="C246" s="6"/>
+      <c r="D246" s="35"/>
+      <c r="E246" s="33"/>
+      <c r="F246" s="25"/>
+      <c r="G246" s="26"/>
+      <c r="H246" s="35"/>
+    </row>
+    <row r="247" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="35"/>
+      <c r="B247" s="38"/>
+      <c r="C247" s="39"/>
+      <c r="D247" s="35"/>
+      <c r="E247" s="40"/>
+      <c r="F247" s="41"/>
+      <c r="G247" s="41"/>
+      <c r="H247" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Rekonfigurasi Laravel Jobs TwoHours pada BackEnd
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="474">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -1518,6 +1518,33 @@
   <si>
     <t>Menyinkronkan Data Bill Of Material Detail</t>
   </si>
+  <si>
+    <t>instruction.device.swingBarrierGate.Goodwin.ServoSW01.getDataAttendance</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Menginstruksikan kepada Alat </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Swing Barrier Gate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Goodwin ServoSW01 untuk memberikan semua data akses</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1526,7 +1553,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1602,6 +1629,13 @@
     </font>
     <font>
       <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
@@ -2338,13 +2372,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H285"/>
+  <dimension ref="A1:H287"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B206" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C214" sqref="C214"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2648,11 +2682,11 @@
     </row>
     <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
-      <c r="B20" s="47" t="s">
-        <v>418</v>
+      <c r="B20" s="7" t="s">
+        <v>472</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>420</v>
+        <v>473</v>
       </c>
       <c r="D20" s="35"/>
       <c r="E20" s="29"/>
@@ -2660,27 +2694,23 @@
       <c r="G20" s="20"/>
       <c r="H20" s="35"/>
     </row>
-    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
-      <c r="B21" s="47" t="s">
-        <v>419</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>421</v>
-      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="35"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="20"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="35"/>
     </row>
     <row r="22" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" s="47" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="D22" s="35"/>
       <c r="E22" s="29"/>
@@ -2688,61 +2718,61 @@
       <c r="G22" s="20"/>
       <c r="H22" s="35"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="35"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="4"/>
+      <c r="B23" s="47" t="s">
+        <v>419</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>421</v>
+      </c>
       <c r="D23" s="35"/>
       <c r="E23" s="29"/>
       <c r="F23" s="19"/>
       <c r="G23" s="20"/>
       <c r="H23" s="35"/>
     </row>
-    <row r="24" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="35"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
+      <c r="B24" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>416</v>
+      </c>
       <c r="D24" s="35"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="22"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="20"/>
       <c r="H24" s="35"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="35"/>
-      <c r="B25" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>403</v>
-      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="35"/>
       <c r="E25" s="29"/>
       <c r="F25" s="19"/>
       <c r="G25" s="20"/>
       <c r="H25" s="35"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="35"/>
-      <c r="B26" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>404</v>
-      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="35"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="20"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="22"/>
       <c r="H26" s="35"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="35"/>
       <c r="B27" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D27" s="35"/>
       <c r="E27" s="29"/>
@@ -2753,10 +2783,10 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="35"/>
       <c r="B28" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D28" s="35"/>
       <c r="E28" s="29"/>
@@ -2767,10 +2797,10 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="35"/>
       <c r="B29" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D29" s="35"/>
       <c r="E29" s="29"/>
@@ -2781,10 +2811,10 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="35"/>
       <c r="B30" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D30" s="35"/>
       <c r="E30" s="29"/>
@@ -2795,10 +2825,10 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="35"/>
       <c r="B31" s="7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D31" s="35"/>
       <c r="E31" s="29"/>
@@ -2808,121 +2838,109 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="35"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>408</v>
+      </c>
       <c r="D32" s="35"/>
       <c r="E32" s="29"/>
       <c r="F32" s="19"/>
       <c r="G32" s="20"/>
       <c r="H32" s="35"/>
     </row>
-    <row r="33" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="35"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
+      <c r="B33" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>409</v>
+      </c>
       <c r="D33" s="35"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="20"/>
       <c r="H33" s="35"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="35"/>
-      <c r="B34" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>308</v>
-      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="4"/>
       <c r="D34" s="35"/>
-      <c r="E34" s="29">
-        <v>44200</v>
-      </c>
-      <c r="F34" s="19">
-        <v>1</v>
-      </c>
-      <c r="G34" s="20">
-        <v>1</v>
-      </c>
+      <c r="E34" s="29"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="20"/>
       <c r="H34" s="35"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="35"/>
-      <c r="B35" s="45" t="s">
-        <v>321</v>
-      </c>
-      <c r="C35" s="46" t="s">
-        <v>323</v>
-      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="10"/>
       <c r="D35" s="35"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="20"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="22"/>
       <c r="H35" s="35"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
-      <c r="B36" s="45" t="s">
-        <v>322</v>
-      </c>
-      <c r="C36" s="46" t="s">
-        <v>324</v>
+      <c r="B36" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>308</v>
       </c>
       <c r="D36" s="35"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="20"/>
+      <c r="E36" s="29">
+        <v>44200</v>
+      </c>
+      <c r="F36" s="19">
+        <v>1</v>
+      </c>
+      <c r="G36" s="20">
+        <v>1</v>
+      </c>
       <c r="H36" s="35"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="45" t="s">
+        <v>321</v>
+      </c>
+      <c r="C37" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="D37" s="35"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="35"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="35"/>
+      <c r="B38" s="45" t="s">
+        <v>322</v>
+      </c>
+      <c r="C38" s="46" t="s">
+        <v>324</v>
+      </c>
+      <c r="D38" s="35"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="35"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="35"/>
+      <c r="B39" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="D37" s="35"/>
-      <c r="E37" s="29">
-        <v>44204</v>
-      </c>
-      <c r="F37" s="19">
-        <v>1</v>
-      </c>
-      <c r="G37" s="20">
-        <v>1</v>
-      </c>
-      <c r="H37" s="35"/>
-    </row>
-    <row r="38" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="37"/>
-      <c r="B38" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="D38" s="37"/>
-      <c r="E38" s="29">
-        <v>44204</v>
-      </c>
-      <c r="F38" s="19">
-        <v>1</v>
-      </c>
-      <c r="G38" s="20">
-        <v>1</v>
-      </c>
-      <c r="H38" s="37"/>
-    </row>
-    <row r="39" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="37"/>
-      <c r="B39" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="D39" s="37"/>
+      <c r="D39" s="35"/>
       <c r="E39" s="29">
         <v>44204</v>
       </c>
@@ -2932,15 +2950,15 @@
       <c r="G39" s="20">
         <v>1</v>
       </c>
-      <c r="H39" s="37"/>
+      <c r="H39" s="35"/>
     </row>
     <row r="40" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37"/>
       <c r="B40" s="13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D40" s="37"/>
       <c r="E40" s="29">
@@ -2957,14 +2975,14 @@
     <row r="41" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="37"/>
       <c r="B41" s="13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D41" s="37"/>
       <c r="E41" s="29">
-        <v>44207</v>
+        <v>44204</v>
       </c>
       <c r="F41" s="19">
         <v>1</v>
@@ -2976,93 +2994,93 @@
     </row>
     <row r="42" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="37"/>
-      <c r="B42" s="7" t="s">
-        <v>432</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>434</v>
+      <c r="B42" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>379</v>
       </c>
       <c r="D42" s="37"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="20"/>
+      <c r="E42" s="29">
+        <v>44204</v>
+      </c>
+      <c r="F42" s="19">
+        <v>1</v>
+      </c>
+      <c r="G42" s="20">
+        <v>1</v>
+      </c>
       <c r="H42" s="37"/>
     </row>
     <row r="43" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="37"/>
-      <c r="B43" s="7" t="s">
-        <v>433</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>435</v>
+      <c r="B43" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>380</v>
       </c>
       <c r="D43" s="37"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="20"/>
+      <c r="E43" s="29">
+        <v>44207</v>
+      </c>
+      <c r="F43" s="19">
+        <v>1</v>
+      </c>
+      <c r="G43" s="20">
+        <v>1</v>
+      </c>
       <c r="H43" s="37"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
+    <row r="44" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="37"/>
       <c r="B44" s="7" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>431</v>
-      </c>
-      <c r="D44" s="35"/>
+        <v>434</v>
+      </c>
+      <c r="D44" s="37"/>
       <c r="E44" s="29"/>
       <c r="F44" s="19"/>
       <c r="G44" s="20"/>
-      <c r="H44" s="35"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+      <c r="H44" s="37"/>
+    </row>
+    <row r="45" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="37"/>
       <c r="B45" s="7" t="s">
-        <v>361</v>
+        <v>433</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="D45" s="35"/>
-      <c r="E45" s="29">
-        <v>44207</v>
-      </c>
-      <c r="F45" s="19">
-        <v>1</v>
-      </c>
-      <c r="G45" s="20">
-        <v>1</v>
-      </c>
-      <c r="H45" s="35"/>
+        <v>435</v>
+      </c>
+      <c r="D45" s="37"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="37"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="35"/>
       <c r="B46" s="7" t="s">
-        <v>360</v>
+        <v>430</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>363</v>
+        <v>431</v>
       </c>
       <c r="D46" s="35"/>
-      <c r="E46" s="29">
-        <v>44207</v>
-      </c>
-      <c r="F46" s="19">
-        <v>1</v>
-      </c>
-      <c r="G46" s="20">
-        <v>1</v>
-      </c>
+      <c r="E46" s="29"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="20"/>
       <c r="H46" s="35"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="35"/>
       <c r="B47" s="7" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D47" s="35"/>
       <c r="E47" s="29">
@@ -3079,10 +3097,10 @@
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="35"/>
       <c r="B48" s="7" t="s">
-        <v>343</v>
+        <v>360</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>344</v>
+        <v>363</v>
       </c>
       <c r="D48" s="35"/>
       <c r="E48" s="29">
@@ -3099,10 +3117,10 @@
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="35"/>
       <c r="B49" s="7" t="s">
-        <v>342</v>
+        <v>359</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>345</v>
+        <v>364</v>
       </c>
       <c r="D49" s="35"/>
       <c r="E49" s="29">
@@ -3119,10 +3137,10 @@
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="35"/>
       <c r="B50" s="7" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D50" s="35"/>
       <c r="E50" s="29">
@@ -3139,10 +3157,10 @@
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="35"/>
       <c r="B51" s="7" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="D51" s="35"/>
       <c r="E51" s="29">
@@ -3159,10 +3177,10 @@
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="35"/>
       <c r="B52" s="7" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="D52" s="35"/>
       <c r="E52" s="29">
@@ -3179,10 +3197,10 @@
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="35"/>
       <c r="B53" s="7" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="D53" s="35"/>
       <c r="E53" s="29">
@@ -3196,51 +3214,63 @@
       </c>
       <c r="H53" s="35"/>
     </row>
-    <row r="54" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="35"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="12"/>
+      <c r="B54" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>334</v>
+      </c>
       <c r="D54" s="35"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="24"/>
+      <c r="E54" s="29">
+        <v>44207</v>
+      </c>
+      <c r="F54" s="19">
+        <v>1</v>
+      </c>
+      <c r="G54" s="20">
+        <v>1</v>
+      </c>
       <c r="H54" s="35"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="35"/>
       <c r="B55" s="7" t="s">
-        <v>446</v>
+        <v>331</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>448</v>
+        <v>332</v>
       </c>
       <c r="D55" s="35"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="20"/>
+      <c r="E55" s="29">
+        <v>44207</v>
+      </c>
+      <c r="F55" s="19">
+        <v>1</v>
+      </c>
+      <c r="G55" s="20">
+        <v>1</v>
+      </c>
       <c r="H55" s="35"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="35"/>
-      <c r="B56" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>451</v>
-      </c>
+      <c r="B56" s="11"/>
+      <c r="C56" s="12"/>
       <c r="D56" s="35"/>
-      <c r="E56" s="29"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="20"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="24"/>
       <c r="H56" s="35"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="35"/>
       <c r="B57" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D57" s="35"/>
       <c r="E57" s="29"/>
@@ -3250,67 +3280,59 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="35"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="4"/>
+      <c r="B58" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>451</v>
+      </c>
       <c r="D58" s="35"/>
       <c r="E58" s="29"/>
       <c r="F58" s="19"/>
       <c r="G58" s="20"/>
       <c r="H58" s="35"/>
     </row>
-    <row r="59" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="35"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="10"/>
+      <c r="B59" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>449</v>
+      </c>
       <c r="D59" s="35"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="22"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="20"/>
       <c r="H59" s="35"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="35"/>
-      <c r="B60" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>302</v>
-      </c>
+      <c r="B60" s="7"/>
+      <c r="C60" s="4"/>
       <c r="D60" s="35"/>
       <c r="E60" s="29"/>
-      <c r="F60" s="19">
-        <v>1</v>
-      </c>
-      <c r="G60" s="20">
-        <v>0</v>
-      </c>
+      <c r="F60" s="19"/>
+      <c r="G60" s="20"/>
       <c r="H60" s="35"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="35"/>
-      <c r="B61" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>303</v>
-      </c>
+      <c r="B61" s="9"/>
+      <c r="C61" s="10"/>
       <c r="D61" s="35"/>
-      <c r="E61" s="29"/>
-      <c r="F61" s="19">
-        <v>1</v>
-      </c>
-      <c r="G61" s="20">
-        <v>0</v>
-      </c>
+      <c r="E61" s="30"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="22"/>
       <c r="H61" s="35"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="35"/>
       <c r="B62" s="7" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="D62" s="35"/>
       <c r="E62" s="29"/>
@@ -3325,10 +3347,10 @@
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="35"/>
       <c r="B63" s="7" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D63" s="35"/>
       <c r="E63" s="29"/>
@@ -3343,10 +3365,10 @@
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="35"/>
       <c r="B64" s="7" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="D64" s="35"/>
       <c r="E64" s="29"/>
@@ -3358,23 +3380,31 @@
       </c>
       <c r="H64" s="35"/>
     </row>
-    <row r="65" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="35"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="12"/>
+      <c r="B65" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>306</v>
+      </c>
       <c r="D65" s="35"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="23"/>
-      <c r="G65" s="24"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="19">
+        <v>1</v>
+      </c>
+      <c r="G65" s="20">
+        <v>0</v>
+      </c>
       <c r="H65" s="35"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="35"/>
       <c r="B66" s="7" t="s">
-        <v>50</v>
+        <v>304</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>92</v>
+        <v>307</v>
       </c>
       <c r="D66" s="35"/>
       <c r="E66" s="29"/>
@@ -3386,31 +3416,23 @@
       </c>
       <c r="H66" s="35"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="35"/>
-      <c r="B67" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>95</v>
-      </c>
+      <c r="B67" s="11"/>
+      <c r="C67" s="12"/>
       <c r="D67" s="35"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="19">
-        <v>1</v>
-      </c>
-      <c r="G67" s="20">
-        <v>0</v>
-      </c>
+      <c r="E67" s="32"/>
+      <c r="F67" s="23"/>
+      <c r="G67" s="24"/>
       <c r="H67" s="35"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="35"/>
       <c r="B68" s="7" t="s">
-        <v>311</v>
+        <v>50</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>312</v>
+        <v>92</v>
       </c>
       <c r="D68" s="35"/>
       <c r="E68" s="29"/>
@@ -3425,10 +3447,10 @@
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="35"/>
       <c r="B69" s="7" t="s">
-        <v>313</v>
+        <v>94</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>314</v>
+        <v>95</v>
       </c>
       <c r="D69" s="35"/>
       <c r="E69" s="29"/>
@@ -3443,10 +3465,10 @@
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="35"/>
       <c r="B70" s="7" t="s">
-        <v>96</v>
+        <v>311</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>99</v>
+        <v>312</v>
       </c>
       <c r="D70" s="35"/>
       <c r="E70" s="29"/>
@@ -3461,10 +3483,10 @@
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="35"/>
       <c r="B71" s="7" t="s">
-        <v>109</v>
+        <v>313</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>110</v>
+        <v>314</v>
       </c>
       <c r="D71" s="35"/>
       <c r="E71" s="29"/>
@@ -3479,10 +3501,10 @@
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="35"/>
       <c r="B72" s="7" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="D72" s="35"/>
       <c r="E72" s="29"/>
@@ -3497,10 +3519,10 @@
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="35"/>
       <c r="B73" s="7" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="D73" s="35"/>
       <c r="E73" s="29"/>
@@ -3515,10 +3537,10 @@
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="35"/>
       <c r="B74" s="7" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="D74" s="35"/>
       <c r="E74" s="29"/>
@@ -3533,10 +3555,10 @@
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="35"/>
       <c r="B75" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D75" s="35"/>
       <c r="E75" s="29"/>
@@ -3551,10 +3573,10 @@
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="35"/>
       <c r="B76" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D76" s="35"/>
       <c r="E76" s="29"/>
@@ -3569,10 +3591,10 @@
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="35"/>
       <c r="B77" s="7" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>381</v>
+        <v>128</v>
       </c>
       <c r="D77" s="35"/>
       <c r="E77" s="29"/>
@@ -3587,10 +3609,10 @@
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="35"/>
       <c r="B78" s="7" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>382</v>
+        <v>101</v>
       </c>
       <c r="D78" s="35"/>
       <c r="E78" s="29"/>
@@ -3605,10 +3627,10 @@
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="35"/>
       <c r="B79" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D79" s="35"/>
       <c r="E79" s="29"/>
@@ -3623,10 +3645,10 @@
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="35"/>
       <c r="B80" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D80" s="35"/>
       <c r="E80" s="29"/>
@@ -3641,10 +3663,10 @@
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="35"/>
       <c r="B81" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>114</v>
+        <v>383</v>
       </c>
       <c r="D81" s="35"/>
       <c r="E81" s="29"/>
@@ -3659,10 +3681,10 @@
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="35"/>
       <c r="B82" s="7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>115</v>
+        <v>384</v>
       </c>
       <c r="D82" s="35"/>
       <c r="E82" s="29"/>
@@ -3677,10 +3699,10 @@
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="35"/>
       <c r="B83" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D83" s="35"/>
       <c r="E83" s="29"/>
@@ -3695,10 +3717,10 @@
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="35"/>
       <c r="B84" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D84" s="35"/>
       <c r="E84" s="29"/>
@@ -3713,10 +3735,10 @@
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="35"/>
       <c r="B85" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D85" s="35"/>
       <c r="E85" s="29"/>
@@ -3731,10 +3753,10 @@
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="35"/>
       <c r="B86" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D86" s="35"/>
       <c r="E86" s="29"/>
@@ -3749,10 +3771,10 @@
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="35"/>
       <c r="B87" s="7" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>198</v>
+        <v>120</v>
       </c>
       <c r="D87" s="35"/>
       <c r="E87" s="29"/>
@@ -3767,10 +3789,10 @@
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="35"/>
       <c r="B88" s="7" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>199</v>
+        <v>122</v>
       </c>
       <c r="D88" s="35"/>
       <c r="E88" s="29"/>
@@ -3785,10 +3807,10 @@
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="35"/>
       <c r="B89" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D89" s="35"/>
       <c r="E89" s="29"/>
@@ -3803,10 +3825,10 @@
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="35"/>
       <c r="B90" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D90" s="35"/>
       <c r="E90" s="29"/>
@@ -3821,10 +3843,10 @@
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="35"/>
       <c r="B91" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D91" s="35"/>
       <c r="E91" s="29"/>
@@ -3839,10 +3861,10 @@
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="35"/>
       <c r="B92" s="7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D92" s="35"/>
       <c r="E92" s="29"/>
@@ -3857,10 +3879,10 @@
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="35"/>
       <c r="B93" s="7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D93" s="35"/>
       <c r="E93" s="29"/>
@@ -3875,10 +3897,10 @@
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="35"/>
       <c r="B94" s="7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D94" s="35"/>
       <c r="E94" s="29"/>
@@ -3893,10 +3915,10 @@
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="35"/>
       <c r="B95" s="7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D95" s="35"/>
       <c r="E95" s="29"/>
@@ -3911,10 +3933,10 @@
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="35"/>
       <c r="B96" s="7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D96" s="35"/>
       <c r="E96" s="29"/>
@@ -3929,10 +3951,10 @@
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="35"/>
       <c r="B97" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D97" s="35"/>
       <c r="E97" s="29"/>
@@ -3947,10 +3969,10 @@
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="35"/>
       <c r="B98" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D98" s="35"/>
       <c r="E98" s="29"/>
@@ -3965,10 +3987,10 @@
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="35"/>
       <c r="B99" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D99" s="35"/>
       <c r="E99" s="29"/>
@@ -3983,10 +4005,10 @@
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="35"/>
       <c r="B100" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D100" s="35"/>
       <c r="E100" s="29"/>
@@ -4001,10 +4023,10 @@
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="35"/>
       <c r="B101" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D101" s="35"/>
       <c r="E101" s="29"/>
@@ -4016,79 +4038,79 @@
       </c>
       <c r="H101" s="35"/>
     </row>
-    <row r="102" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="35"/>
-      <c r="B102" s="11"/>
-      <c r="C102" s="12"/>
+      <c r="B102" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>212</v>
+      </c>
       <c r="D102" s="35"/>
-      <c r="E102" s="32"/>
-      <c r="F102" s="23"/>
-      <c r="G102" s="24"/>
+      <c r="E102" s="29"/>
+      <c r="F102" s="19">
+        <v>1</v>
+      </c>
+      <c r="G102" s="20">
+        <v>0</v>
+      </c>
       <c r="H102" s="35"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="35"/>
       <c r="B103" s="7" t="s">
-        <v>234</v>
+        <v>129</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="D103" s="35"/>
-      <c r="E103" s="29">
-        <v>44188</v>
-      </c>
+      <c r="E103" s="29"/>
       <c r="F103" s="19">
         <v>1</v>
       </c>
       <c r="G103" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H103" s="35"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>239</v>
-      </c>
+      <c r="B104" s="11"/>
+      <c r="C104" s="12"/>
       <c r="D104" s="35"/>
-      <c r="E104" s="29"/>
-      <c r="F104" s="19">
-        <v>1</v>
-      </c>
-      <c r="G104" s="20">
-        <v>0</v>
-      </c>
+      <c r="E104" s="32"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="24"/>
       <c r="H104" s="35"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="35"/>
       <c r="B105" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D105" s="35"/>
-      <c r="E105" s="29"/>
+      <c r="E105" s="29">
+        <v>44188</v>
+      </c>
       <c r="F105" s="19">
         <v>1</v>
       </c>
       <c r="G105" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H105" s="35"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="35"/>
       <c r="B106" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D106" s="35"/>
       <c r="E106" s="29"/>
@@ -4103,10 +4125,10 @@
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="35"/>
       <c r="B107" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D107" s="35"/>
       <c r="E107" s="29"/>
@@ -4118,23 +4140,31 @@
       </c>
       <c r="H107" s="35"/>
     </row>
-    <row r="108" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="35"/>
-      <c r="B108" s="11"/>
-      <c r="C108" s="12"/>
+      <c r="B108" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>241</v>
+      </c>
       <c r="D108" s="35"/>
-      <c r="E108" s="32"/>
-      <c r="F108" s="23"/>
-      <c r="G108" s="24"/>
+      <c r="E108" s="29"/>
+      <c r="F108" s="19">
+        <v>1</v>
+      </c>
+      <c r="G108" s="20">
+        <v>0</v>
+      </c>
       <c r="H108" s="35"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="35"/>
       <c r="B109" s="7" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="D109" s="35"/>
       <c r="E109" s="29"/>
@@ -4146,31 +4176,23 @@
       </c>
       <c r="H109" s="35"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="35"/>
-      <c r="B110" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="C110" s="4" t="s">
-        <v>224</v>
-      </c>
+      <c r="B110" s="11"/>
+      <c r="C110" s="12"/>
       <c r="D110" s="35"/>
-      <c r="E110" s="29"/>
-      <c r="F110" s="19">
-        <v>1</v>
-      </c>
-      <c r="G110" s="20">
-        <v>0</v>
-      </c>
+      <c r="E110" s="32"/>
+      <c r="F110" s="23"/>
+      <c r="G110" s="24"/>
       <c r="H110" s="35"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="35"/>
       <c r="B111" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D111" s="35"/>
       <c r="E111" s="29"/>
@@ -4185,10 +4207,10 @@
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="35"/>
       <c r="B112" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D112" s="35"/>
       <c r="E112" s="29"/>
@@ -4203,10 +4225,10 @@
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="35"/>
       <c r="B113" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D113" s="35"/>
       <c r="E113" s="29"/>
@@ -4218,23 +4240,31 @@
       </c>
       <c r="H113" s="35"/>
     </row>
-    <row r="114" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="35"/>
-      <c r="B114" s="11"/>
-      <c r="C114" s="12"/>
+      <c r="B114" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>226</v>
+      </c>
       <c r="D114" s="35"/>
-      <c r="E114" s="32"/>
-      <c r="F114" s="23"/>
-      <c r="G114" s="24"/>
+      <c r="E114" s="29"/>
+      <c r="F114" s="19">
+        <v>1</v>
+      </c>
+      <c r="G114" s="20">
+        <v>0</v>
+      </c>
       <c r="H114" s="35"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="35"/>
       <c r="B115" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D115" s="35"/>
       <c r="E115" s="29"/>
@@ -4259,10 +4289,10 @@
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="35"/>
       <c r="B117" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D117" s="35"/>
       <c r="E117" s="29"/>
@@ -4274,41 +4304,41 @@
       </c>
       <c r="H117" s="35"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="35"/>
-      <c r="B118" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B118" s="11"/>
+      <c r="C118" s="12"/>
       <c r="D118" s="35"/>
-      <c r="E118" s="29"/>
-      <c r="F118" s="19">
-        <v>1</v>
-      </c>
-      <c r="G118" s="20">
-        <v>0</v>
-      </c>
+      <c r="E118" s="32"/>
+      <c r="F118" s="23"/>
+      <c r="G118" s="24"/>
       <c r="H118" s="35"/>
     </row>
-    <row r="119" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="35"/>
-      <c r="B119" s="11"/>
-      <c r="C119" s="12"/>
+      <c r="B119" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>232</v>
+      </c>
       <c r="D119" s="35"/>
-      <c r="E119" s="32"/>
-      <c r="F119" s="23"/>
-      <c r="G119" s="24"/>
+      <c r="E119" s="29"/>
+      <c r="F119" s="19">
+        <v>1</v>
+      </c>
+      <c r="G119" s="20">
+        <v>0</v>
+      </c>
       <c r="H119" s="35"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="35"/>
       <c r="B120" s="7" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="D120" s="35"/>
       <c r="E120" s="29"/>
@@ -4333,10 +4363,10 @@
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="35"/>
       <c r="B122" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D122" s="35"/>
       <c r="E122" s="29"/>
@@ -4348,31 +4378,23 @@
       </c>
       <c r="H122" s="35"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="35"/>
-      <c r="B123" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="C123" s="4" t="s">
-        <v>282</v>
-      </c>
+      <c r="B123" s="11"/>
+      <c r="C123" s="12"/>
       <c r="D123" s="35"/>
-      <c r="E123" s="29"/>
-      <c r="F123" s="19">
-        <v>1</v>
-      </c>
-      <c r="G123" s="20">
-        <v>0</v>
-      </c>
+      <c r="E123" s="32"/>
+      <c r="F123" s="23"/>
+      <c r="G123" s="24"/>
       <c r="H123" s="35"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="35"/>
       <c r="B124" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>284</v>
+        <v>247</v>
       </c>
       <c r="D124" s="35"/>
       <c r="E124" s="29"/>
@@ -4387,10 +4409,10 @@
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="35"/>
       <c r="B125" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D125" s="35"/>
       <c r="E125" s="29"/>
@@ -4405,10 +4427,10 @@
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="35"/>
       <c r="B126" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D126" s="35"/>
       <c r="E126" s="29"/>
@@ -4423,10 +4445,10 @@
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="35"/>
       <c r="B127" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
       <c r="D127" s="35"/>
       <c r="E127" s="29"/>
@@ -4441,10 +4463,10 @@
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="35"/>
       <c r="B128" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>264</v>
+        <v>285</v>
       </c>
       <c r="D128" s="35"/>
       <c r="E128" s="29"/>
@@ -4459,10 +4481,10 @@
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="35"/>
       <c r="B129" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>286</v>
+        <v>256</v>
       </c>
       <c r="D129" s="35"/>
       <c r="E129" s="29"/>
@@ -4477,10 +4499,10 @@
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="35"/>
       <c r="B130" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="D130" s="35"/>
       <c r="E130" s="29"/>
@@ -4495,10 +4517,10 @@
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="35"/>
       <c r="B131" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>263</v>
+        <v>286</v>
       </c>
       <c r="D131" s="35"/>
       <c r="E131" s="29"/>
@@ -4513,10 +4535,10 @@
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="35"/>
       <c r="B132" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>265</v>
+        <v>287</v>
       </c>
       <c r="D132" s="35"/>
       <c r="E132" s="29"/>
@@ -4531,10 +4553,10 @@
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="35"/>
       <c r="B133" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D133" s="35"/>
       <c r="E133" s="29"/>
@@ -4549,10 +4571,10 @@
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="35"/>
       <c r="B134" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D134" s="35"/>
       <c r="E134" s="29"/>
@@ -4567,10 +4589,10 @@
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="35"/>
       <c r="B135" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D135" s="35"/>
       <c r="E135" s="29"/>
@@ -4585,10 +4607,10 @@
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="35"/>
       <c r="B136" s="7" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="D136" s="35"/>
       <c r="E136" s="29"/>
@@ -4603,10 +4625,10 @@
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="35"/>
       <c r="B137" s="7" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D137" s="35"/>
       <c r="E137" s="29"/>
@@ -4621,10 +4643,10 @@
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="35"/>
       <c r="B138" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D138" s="35"/>
       <c r="E138" s="29"/>
@@ -4639,10 +4661,10 @@
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="35"/>
       <c r="B139" s="7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D139" s="35"/>
       <c r="E139" s="29"/>
@@ -4657,10 +4679,10 @@
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="35"/>
       <c r="B140" s="7" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="D140" s="35"/>
       <c r="E140" s="29"/>
@@ -4675,10 +4697,10 @@
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="35"/>
       <c r="B141" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D141" s="35"/>
       <c r="E141" s="29"/>
@@ -4693,10 +4715,10 @@
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="35"/>
       <c r="B142" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D142" s="35"/>
       <c r="E142" s="29"/>
@@ -4708,23 +4730,31 @@
       </c>
       <c r="H142" s="35"/>
     </row>
-    <row r="143" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="35"/>
-      <c r="B143" s="11"/>
-      <c r="C143" s="12"/>
+      <c r="B143" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>280</v>
+      </c>
       <c r="D143" s="35"/>
-      <c r="E143" s="32"/>
-      <c r="F143" s="23"/>
-      <c r="G143" s="24"/>
+      <c r="E143" s="29"/>
+      <c r="F143" s="19">
+        <v>1</v>
+      </c>
+      <c r="G143" s="20">
+        <v>0</v>
+      </c>
       <c r="H143" s="35"/>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="35"/>
       <c r="B144" s="7" t="s">
-        <v>144</v>
+        <v>277</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>214</v>
+        <v>279</v>
       </c>
       <c r="D144" s="35"/>
       <c r="E144" s="29"/>
@@ -4736,41 +4766,41 @@
       </c>
       <c r="H144" s="35"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="35"/>
-      <c r="B145" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="C145" s="4" t="s">
-        <v>216</v>
-      </c>
+      <c r="B145" s="11"/>
+      <c r="C145" s="12"/>
       <c r="D145" s="35"/>
-      <c r="E145" s="29"/>
-      <c r="F145" s="19">
-        <v>1</v>
-      </c>
-      <c r="G145" s="20">
-        <v>0</v>
-      </c>
+      <c r="E145" s="32"/>
+      <c r="F145" s="23"/>
+      <c r="G145" s="24"/>
       <c r="H145" s="35"/>
     </row>
-    <row r="146" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="35"/>
-      <c r="B146" s="11"/>
-      <c r="C146" s="12"/>
+      <c r="B146" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>214</v>
+      </c>
       <c r="D146" s="35"/>
-      <c r="E146" s="32"/>
-      <c r="F146" s="23"/>
-      <c r="G146" s="24"/>
+      <c r="E146" s="29"/>
+      <c r="F146" s="19">
+        <v>1</v>
+      </c>
+      <c r="G146" s="20">
+        <v>0</v>
+      </c>
       <c r="H146" s="35"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="35"/>
       <c r="B147" s="7" t="s">
-        <v>288</v>
+        <v>215</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>296</v>
+        <v>216</v>
       </c>
       <c r="D147" s="35"/>
       <c r="E147" s="29"/>
@@ -4782,31 +4812,23 @@
       </c>
       <c r="H147" s="35"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="35"/>
-      <c r="B148" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="C148" s="4" t="s">
-        <v>290</v>
-      </c>
+      <c r="B148" s="11"/>
+      <c r="C148" s="12"/>
       <c r="D148" s="35"/>
-      <c r="E148" s="29"/>
-      <c r="F148" s="19">
-        <v>1</v>
-      </c>
-      <c r="G148" s="20">
-        <v>0</v>
-      </c>
+      <c r="E148" s="32"/>
+      <c r="F148" s="23"/>
+      <c r="G148" s="24"/>
       <c r="H148" s="35"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="35"/>
       <c r="B149" s="7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D149" s="35"/>
       <c r="E149" s="29"/>
@@ -4821,10 +4843,10 @@
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="35"/>
       <c r="B150" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D150" s="35"/>
       <c r="E150" s="29"/>
@@ -4839,10 +4861,10 @@
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="35"/>
       <c r="B151" s="7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D151" s="35"/>
       <c r="E151" s="29"/>
@@ -4856,75 +4878,71 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="35"/>
-      <c r="B152" s="7"/>
-      <c r="C152" s="4"/>
+      <c r="B152" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C152" s="4" t="s">
+        <v>293</v>
+      </c>
       <c r="D152" s="35"/>
       <c r="E152" s="29"/>
-      <c r="F152" s="19"/>
-      <c r="G152" s="20"/>
+      <c r="F152" s="19">
+        <v>1</v>
+      </c>
+      <c r="G152" s="20">
+        <v>0</v>
+      </c>
       <c r="H152" s="35"/>
     </row>
-    <row r="153" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="35"/>
-      <c r="B153" s="9"/>
-      <c r="C153" s="10"/>
+      <c r="B153" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>295</v>
+      </c>
       <c r="D153" s="35"/>
-      <c r="E153" s="30"/>
-      <c r="F153" s="21"/>
-      <c r="G153" s="22"/>
+      <c r="E153" s="29"/>
+      <c r="F153" s="19">
+        <v>1</v>
+      </c>
+      <c r="G153" s="20">
+        <v>0</v>
+      </c>
       <c r="H153" s="35"/>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="35"/>
-      <c r="B154" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C154" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="B154" s="7"/>
+      <c r="C154" s="4"/>
       <c r="D154" s="35"/>
-      <c r="E154" s="29">
-        <v>44207</v>
-      </c>
-      <c r="F154" s="19">
-        <v>1</v>
-      </c>
-      <c r="G154" s="20">
-        <v>1</v>
-      </c>
+      <c r="E154" s="29"/>
+      <c r="F154" s="19"/>
+      <c r="G154" s="20"/>
       <c r="H154" s="35"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="35"/>
-      <c r="B155" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C155" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="B155" s="9"/>
+      <c r="C155" s="10"/>
       <c r="D155" s="35"/>
-      <c r="E155" s="29">
-        <v>44211</v>
-      </c>
-      <c r="F155" s="19">
-        <v>1</v>
-      </c>
-      <c r="G155" s="20">
-        <v>1</v>
-      </c>
+      <c r="E155" s="30"/>
+      <c r="F155" s="21"/>
+      <c r="G155" s="22"/>
       <c r="H155" s="35"/>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="35"/>
       <c r="B156" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D156" s="35"/>
       <c r="E156" s="29">
-        <v>44211</v>
+        <v>44207</v>
       </c>
       <c r="F156" s="19">
         <v>1</v>
@@ -4937,10 +4955,10 @@
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="35"/>
       <c r="B157" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D157" s="35"/>
       <c r="E157" s="29">
@@ -4957,10 +4975,10 @@
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="35"/>
       <c r="B158" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D158" s="35"/>
       <c r="E158" s="29">
@@ -4977,10 +4995,10 @@
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="35"/>
       <c r="B159" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D159" s="35"/>
       <c r="E159" s="29">
@@ -4997,10 +5015,10 @@
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="35"/>
       <c r="B160" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D160" s="35"/>
       <c r="E160" s="29">
@@ -5017,10 +5035,10 @@
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="35"/>
       <c r="B161" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D161" s="35"/>
       <c r="E161" s="29">
@@ -5037,10 +5055,10 @@
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="35"/>
       <c r="B162" s="7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D162" s="35"/>
       <c r="E162" s="29">
@@ -5057,10 +5075,10 @@
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="35"/>
       <c r="B163" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="D163" s="35"/>
       <c r="E163" s="29">
@@ -5077,10 +5095,10 @@
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="35"/>
       <c r="B164" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D164" s="35"/>
       <c r="E164" s="29">
@@ -5097,10 +5115,10 @@
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="35"/>
       <c r="B165" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D165" s="35"/>
       <c r="E165" s="29">
@@ -5117,10 +5135,10 @@
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="35"/>
       <c r="B166" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D166" s="35"/>
       <c r="E166" s="29">
@@ -5137,10 +5155,10 @@
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="35"/>
       <c r="B167" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D167" s="35"/>
       <c r="E167" s="29">
@@ -5157,10 +5175,10 @@
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="35"/>
       <c r="B168" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D168" s="35"/>
       <c r="E168" s="29">
@@ -5177,10 +5195,10 @@
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="35"/>
       <c r="B169" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>207</v>
+        <v>86</v>
       </c>
       <c r="D169" s="35"/>
       <c r="E169" s="29">
@@ -5197,10 +5215,10 @@
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="35"/>
       <c r="B170" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D170" s="35"/>
       <c r="E170" s="29">
@@ -5217,10 +5235,10 @@
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="35"/>
       <c r="B171" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>89</v>
+        <v>207</v>
       </c>
       <c r="D171" s="35"/>
       <c r="E171" s="29">
@@ -5237,10 +5255,10 @@
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="35"/>
       <c r="B172" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D172" s="35"/>
       <c r="E172" s="29">
@@ -5257,10 +5275,10 @@
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="35"/>
       <c r="B173" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D173" s="35"/>
       <c r="E173" s="29">
@@ -5276,81 +5294,85 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="35"/>
-      <c r="B174" s="7"/>
-      <c r="C174" s="4"/>
+      <c r="B174" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="D174" s="35"/>
-      <c r="E174" s="29"/>
-      <c r="F174" s="19"/>
-      <c r="G174" s="20"/>
+      <c r="E174" s="29">
+        <v>44211</v>
+      </c>
+      <c r="F174" s="19">
+        <v>1</v>
+      </c>
+      <c r="G174" s="20">
+        <v>1</v>
+      </c>
       <c r="H174" s="35"/>
     </row>
-    <row r="175" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="35"/>
-      <c r="B175" s="9"/>
-      <c r="C175" s="10"/>
+      <c r="B175" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="D175" s="35"/>
-      <c r="E175" s="30"/>
-      <c r="F175" s="21"/>
-      <c r="G175" s="22"/>
+      <c r="E175" s="29">
+        <v>44211</v>
+      </c>
+      <c r="F175" s="19">
+        <v>1</v>
+      </c>
+      <c r="G175" s="20">
+        <v>1</v>
+      </c>
       <c r="H175" s="35"/>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="35"/>
-      <c r="B176" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="C176" s="4" t="s">
-        <v>423</v>
-      </c>
+      <c r="B176" s="7"/>
+      <c r="C176" s="4"/>
       <c r="D176" s="35"/>
       <c r="E176" s="29"/>
       <c r="F176" s="19"/>
       <c r="G176" s="20"/>
       <c r="H176" s="35"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="35"/>
-      <c r="B177" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C177" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="B177" s="9"/>
+      <c r="C177" s="10"/>
       <c r="D177" s="35"/>
-      <c r="E177" s="29"/>
-      <c r="F177" s="19">
-        <v>1</v>
-      </c>
-      <c r="G177" s="20">
-        <v>0</v>
-      </c>
+      <c r="E177" s="30"/>
+      <c r="F177" s="21"/>
+      <c r="G177" s="22"/>
       <c r="H177" s="35"/>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="35"/>
       <c r="B178" s="7" t="s">
-        <v>17</v>
+        <v>422</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>15</v>
+        <v>423</v>
       </c>
       <c r="D178" s="35"/>
       <c r="E178" s="29"/>
-      <c r="F178" s="19">
-        <v>1</v>
-      </c>
-      <c r="G178" s="20">
-        <v>0</v>
-      </c>
+      <c r="F178" s="19"/>
+      <c r="G178" s="20"/>
       <c r="H178" s="35"/>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="35"/>
       <c r="B179" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D179" s="35"/>
       <c r="E179" s="29"/>
@@ -5365,10 +5387,10 @@
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="35"/>
       <c r="B180" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D180" s="35"/>
       <c r="E180" s="29"/>
@@ -5383,10 +5405,10 @@
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="35"/>
       <c r="B181" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D181" s="35"/>
       <c r="E181" s="29"/>
@@ -5401,10 +5423,10 @@
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="35"/>
       <c r="B182" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D182" s="35"/>
       <c r="E182" s="29"/>
@@ -5419,10 +5441,10 @@
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="35"/>
       <c r="B183" s="7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D183" s="35"/>
       <c r="E183" s="29"/>
@@ -5437,10 +5459,10 @@
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="35"/>
       <c r="B184" s="7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D184" s="35"/>
       <c r="E184" s="29"/>
@@ -5455,10 +5477,10 @@
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="35"/>
       <c r="B185" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D185" s="35"/>
       <c r="E185" s="29"/>
@@ -5473,10 +5495,10 @@
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="35"/>
       <c r="B186" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D186" s="35"/>
       <c r="E186" s="29"/>
@@ -5491,10 +5513,10 @@
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="35"/>
       <c r="B187" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D187" s="35"/>
       <c r="E187" s="29"/>
@@ -5509,10 +5531,10 @@
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="35"/>
       <c r="B188" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="D188" s="35"/>
       <c r="E188" s="29"/>
@@ -5527,10 +5549,10 @@
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="35"/>
       <c r="B189" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D189" s="35"/>
       <c r="E189" s="29"/>
@@ -5545,10 +5567,10 @@
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="35"/>
       <c r="B190" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="D190" s="35"/>
       <c r="E190" s="29"/>
@@ -5563,10 +5585,10 @@
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="35"/>
       <c r="B191" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D191" s="35"/>
       <c r="E191" s="29"/>
@@ -5581,10 +5603,10 @@
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="35"/>
       <c r="B192" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C192" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="C192" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="D192" s="35"/>
       <c r="E192" s="29"/>
@@ -5599,10 +5621,10 @@
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="35"/>
       <c r="B193" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D193" s="35"/>
       <c r="E193" s="29"/>
@@ -5617,10 +5639,10 @@
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="35"/>
       <c r="B194" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C194" s="4" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="C194" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D194" s="35"/>
       <c r="E194" s="29"/>
@@ -5635,10 +5657,10 @@
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="35"/>
       <c r="B195" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D195" s="35"/>
       <c r="E195" s="29"/>
@@ -5650,93 +5672,93 @@
       </c>
       <c r="H195" s="35"/>
     </row>
-    <row r="196" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="35"/>
-      <c r="B196" s="11"/>
-      <c r="C196" s="12"/>
+      <c r="B196" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="D196" s="35"/>
-      <c r="E196" s="32"/>
-      <c r="F196" s="23"/>
-      <c r="G196" s="24"/>
+      <c r="E196" s="29"/>
+      <c r="F196" s="19">
+        <v>1</v>
+      </c>
+      <c r="G196" s="20">
+        <v>0</v>
+      </c>
       <c r="H196" s="35"/>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="35"/>
       <c r="B197" s="7" t="s">
-        <v>424</v>
+        <v>48</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>425</v>
+        <v>49</v>
       </c>
       <c r="D197" s="35"/>
       <c r="E197" s="29"/>
-      <c r="F197" s="19"/>
-      <c r="G197" s="20"/>
+      <c r="F197" s="19">
+        <v>1</v>
+      </c>
+      <c r="G197" s="20">
+        <v>0</v>
+      </c>
       <c r="H197" s="35"/>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="35"/>
-      <c r="B198" s="7"/>
-      <c r="C198" s="4"/>
+      <c r="B198" s="11"/>
+      <c r="C198" s="12"/>
       <c r="D198" s="35"/>
-      <c r="E198" s="29"/>
-      <c r="F198" s="19"/>
-      <c r="G198" s="20"/>
+      <c r="E198" s="32"/>
+      <c r="F198" s="23"/>
+      <c r="G198" s="24"/>
       <c r="H198" s="35"/>
     </row>
-    <row r="199" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="35"/>
-      <c r="B199" s="9"/>
-      <c r="C199" s="10"/>
+      <c r="B199" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>425</v>
+      </c>
       <c r="D199" s="35"/>
-      <c r="E199" s="30"/>
-      <c r="F199" s="21"/>
-      <c r="G199" s="22"/>
+      <c r="E199" s="29"/>
+      <c r="F199" s="19"/>
+      <c r="G199" s="20"/>
       <c r="H199" s="35"/>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="35"/>
-      <c r="B200" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="C200" s="4" t="s">
-        <v>310</v>
-      </c>
+      <c r="B200" s="7"/>
+      <c r="C200" s="4"/>
       <c r="D200" s="35"/>
       <c r="E200" s="29"/>
-      <c r="F200" s="19">
-        <v>1</v>
-      </c>
-      <c r="G200" s="20">
-        <v>0</v>
-      </c>
+      <c r="F200" s="19"/>
+      <c r="G200" s="20"/>
       <c r="H200" s="35"/>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="35"/>
-      <c r="B201" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="C201" s="4" t="s">
-        <v>427</v>
-      </c>
+      <c r="B201" s="9"/>
+      <c r="C201" s="10"/>
       <c r="D201" s="35"/>
-      <c r="E201" s="29"/>
-      <c r="F201" s="19">
-        <v>1</v>
-      </c>
-      <c r="G201" s="20">
-        <v>0</v>
-      </c>
+      <c r="E201" s="30"/>
+      <c r="F201" s="21"/>
+      <c r="G201" s="22"/>
       <c r="H201" s="35"/>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="35"/>
       <c r="B202" s="7" t="s">
-        <v>428</v>
+        <v>309</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>429</v>
+        <v>310</v>
       </c>
       <c r="D202" s="35"/>
       <c r="E202" s="29"/>
@@ -5751,10 +5773,10 @@
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="35"/>
       <c r="B203" s="7" t="s">
-        <v>410</v>
+        <v>426</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>411</v>
+        <v>427</v>
       </c>
       <c r="D203" s="35"/>
       <c r="E203" s="29"/>
@@ -5768,67 +5790,75 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="35"/>
-      <c r="B204" s="48" t="s">
-        <v>462</v>
-      </c>
-      <c r="C204" s="49" t="s">
-        <v>463</v>
-      </c>
-      <c r="D204" s="50"/>
-      <c r="E204" s="51"/>
-      <c r="F204" s="52">
-        <v>1</v>
-      </c>
-      <c r="G204" s="53">
+      <c r="B204" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="C204" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D204" s="35"/>
+      <c r="E204" s="29"/>
+      <c r="F204" s="19">
+        <v>1</v>
+      </c>
+      <c r="G204" s="20">
         <v>0</v>
       </c>
       <c r="H204" s="35"/>
     </row>
-    <row r="205" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="35"/>
-      <c r="B205" s="11"/>
-      <c r="C205" s="12"/>
+      <c r="B205" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="C205" s="4" t="s">
+        <v>411</v>
+      </c>
       <c r="D205" s="35"/>
-      <c r="E205" s="32"/>
-      <c r="F205" s="23"/>
-      <c r="G205" s="24"/>
+      <c r="E205" s="29"/>
+      <c r="F205" s="19">
+        <v>1</v>
+      </c>
+      <c r="G205" s="20">
+        <v>0</v>
+      </c>
       <c r="H205" s="35"/>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="35"/>
-      <c r="B206" s="7" t="s">
-        <v>458</v>
-      </c>
-      <c r="C206" s="4" t="s">
-        <v>459</v>
-      </c>
-      <c r="D206" s="35"/>
-      <c r="E206" s="29"/>
-      <c r="F206" s="19"/>
-      <c r="G206" s="20"/>
+      <c r="B206" s="48" t="s">
+        <v>462</v>
+      </c>
+      <c r="C206" s="49" t="s">
+        <v>463</v>
+      </c>
+      <c r="D206" s="50"/>
+      <c r="E206" s="51"/>
+      <c r="F206" s="52">
+        <v>1</v>
+      </c>
+      <c r="G206" s="53">
+        <v>0</v>
+      </c>
       <c r="H206" s="35"/>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="35"/>
-      <c r="B207" s="7" t="s">
-        <v>454</v>
-      </c>
-      <c r="C207" s="4" t="s">
-        <v>455</v>
-      </c>
+      <c r="B207" s="11"/>
+      <c r="C207" s="12"/>
       <c r="D207" s="35"/>
-      <c r="E207" s="29"/>
-      <c r="F207" s="19"/>
-      <c r="G207" s="20"/>
+      <c r="E207" s="32"/>
+      <c r="F207" s="23"/>
+      <c r="G207" s="24"/>
       <c r="H207" s="35"/>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="35"/>
       <c r="B208" s="7" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D208" s="35"/>
       <c r="E208" s="29"/>
@@ -5836,65 +5866,69 @@
       <c r="G208" s="20"/>
       <c r="H208" s="35"/>
     </row>
-    <row r="209" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="35"/>
-      <c r="B209" s="11"/>
-      <c r="C209" s="12"/>
+      <c r="B209" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="C209" s="4" t="s">
+        <v>455</v>
+      </c>
       <c r="D209" s="35"/>
-      <c r="E209" s="32"/>
-      <c r="F209" s="23"/>
-      <c r="G209" s="24"/>
+      <c r="E209" s="29"/>
+      <c r="F209" s="19"/>
+      <c r="G209" s="20"/>
       <c r="H209" s="35"/>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="35"/>
       <c r="B210" s="7" t="s">
-        <v>102</v>
+        <v>456</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>103</v>
+        <v>457</v>
       </c>
       <c r="D210" s="35"/>
       <c r="E210" s="29"/>
-      <c r="F210" s="19">
-        <v>1</v>
-      </c>
-      <c r="G210" s="20">
-        <v>0</v>
-      </c>
+      <c r="F210" s="19"/>
+      <c r="G210" s="20"/>
       <c r="H210" s="35"/>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="35"/>
-      <c r="B211" s="7" t="s">
-        <v>460</v>
-      </c>
-      <c r="C211" s="4" t="s">
-        <v>461</v>
-      </c>
+      <c r="B211" s="11"/>
+      <c r="C211" s="12"/>
       <c r="D211" s="35"/>
-      <c r="E211" s="29"/>
-      <c r="F211" s="19"/>
-      <c r="G211" s="20"/>
+      <c r="E211" s="32"/>
+      <c r="F211" s="23"/>
+      <c r="G211" s="24"/>
       <c r="H211" s="35"/>
     </row>
-    <row r="212" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="35"/>
-      <c r="B212" s="11"/>
-      <c r="C212" s="12"/>
+      <c r="B212" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="D212" s="35"/>
-      <c r="E212" s="32"/>
-      <c r="F212" s="23"/>
-      <c r="G212" s="24"/>
+      <c r="E212" s="29"/>
+      <c r="F212" s="19">
+        <v>1</v>
+      </c>
+      <c r="G212" s="20">
+        <v>0</v>
+      </c>
       <c r="H212" s="35"/>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="35"/>
       <c r="B213" s="7" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D213" s="35"/>
       <c r="E213" s="29"/>
@@ -5902,27 +5936,23 @@
       <c r="G213" s="20"/>
       <c r="H213" s="35"/>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="35"/>
-      <c r="B214" s="7" t="s">
-        <v>470</v>
-      </c>
-      <c r="C214" s="4" t="s">
-        <v>471</v>
-      </c>
+      <c r="B214" s="11"/>
+      <c r="C214" s="12"/>
       <c r="D214" s="35"/>
-      <c r="E214" s="29"/>
-      <c r="F214" s="19"/>
-      <c r="G214" s="20"/>
+      <c r="E214" s="32"/>
+      <c r="F214" s="23"/>
+      <c r="G214" s="24"/>
       <c r="H214" s="35"/>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="35"/>
       <c r="B215" s="7" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D215" s="35"/>
       <c r="E215" s="29"/>
@@ -5933,10 +5963,10 @@
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="35"/>
       <c r="B216" s="7" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D216" s="35"/>
       <c r="E216" s="29"/>
@@ -5944,97 +5974,89 @@
       <c r="G216" s="20"/>
       <c r="H216" s="35"/>
     </row>
-    <row r="217" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="35"/>
-      <c r="B217" s="11"/>
-      <c r="C217" s="12"/>
+      <c r="B217" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="C217" s="4" t="s">
+        <v>467</v>
+      </c>
       <c r="D217" s="35"/>
-      <c r="E217" s="32"/>
-      <c r="F217" s="23"/>
-      <c r="G217" s="24"/>
+      <c r="E217" s="29"/>
+      <c r="F217" s="19"/>
+      <c r="G217" s="20"/>
       <c r="H217" s="35"/>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="35"/>
       <c r="B218" s="7" t="s">
-        <v>412</v>
+        <v>468</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>413</v>
+        <v>469</v>
       </c>
       <c r="D218" s="35"/>
       <c r="E218" s="29"/>
-      <c r="F218" s="19">
-        <v>1</v>
-      </c>
-      <c r="G218" s="20">
-        <v>0</v>
-      </c>
+      <c r="F218" s="19"/>
+      <c r="G218" s="20"/>
       <c r="H218" s="35"/>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="35"/>
-      <c r="B219" s="7"/>
-      <c r="C219" s="4"/>
+      <c r="B219" s="11"/>
+      <c r="C219" s="12"/>
       <c r="D219" s="35"/>
-      <c r="E219" s="29"/>
-      <c r="F219" s="19"/>
-      <c r="G219" s="20"/>
+      <c r="E219" s="32"/>
+      <c r="F219" s="23"/>
+      <c r="G219" s="24"/>
       <c r="H219" s="35"/>
     </row>
-    <row r="220" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="35"/>
-      <c r="B220" s="9"/>
-      <c r="C220" s="10"/>
+      <c r="B220" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>413</v>
+      </c>
       <c r="D220" s="35"/>
-      <c r="E220" s="30"/>
-      <c r="F220" s="21"/>
-      <c r="G220" s="22"/>
+      <c r="E220" s="29"/>
+      <c r="F220" s="19">
+        <v>1</v>
+      </c>
+      <c r="G220" s="20">
+        <v>0</v>
+      </c>
       <c r="H220" s="35"/>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="35"/>
-      <c r="B221" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C221" s="4" t="s">
-        <v>93</v>
-      </c>
+      <c r="B221" s="7"/>
+      <c r="C221" s="4"/>
       <c r="D221" s="35"/>
       <c r="E221" s="29"/>
-      <c r="F221" s="19">
-        <v>1</v>
-      </c>
-      <c r="G221" s="20">
-        <v>0</v>
-      </c>
+      <c r="F221" s="19"/>
+      <c r="G221" s="20"/>
       <c r="H221" s="35"/>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="35"/>
-      <c r="B222" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C222" s="4" t="s">
-        <v>145</v>
-      </c>
+      <c r="B222" s="9"/>
+      <c r="C222" s="10"/>
       <c r="D222" s="35"/>
-      <c r="E222" s="29"/>
-      <c r="F222" s="19">
-        <v>1</v>
-      </c>
-      <c r="G222" s="20">
-        <v>0</v>
-      </c>
+      <c r="E222" s="30"/>
+      <c r="F222" s="21"/>
+      <c r="G222" s="22"/>
       <c r="H222" s="35"/>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="35"/>
       <c r="B223" s="7" t="s">
-        <v>315</v>
+        <v>51</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>316</v>
+        <v>93</v>
       </c>
       <c r="D223" s="35"/>
       <c r="E223" s="29"/>
@@ -6049,10 +6071,10 @@
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="35"/>
       <c r="B224" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D224" s="35"/>
       <c r="E224" s="29"/>
@@ -6067,10 +6089,10 @@
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="35"/>
       <c r="B225" s="7" t="s">
-        <v>166</v>
+        <v>315</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>147</v>
+        <v>316</v>
       </c>
       <c r="D225" s="35"/>
       <c r="E225" s="29"/>
@@ -6085,10 +6107,10 @@
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="35"/>
       <c r="B226" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D226" s="35"/>
       <c r="E226" s="29"/>
@@ -6103,10 +6125,10 @@
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="35"/>
       <c r="B227" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D227" s="35"/>
       <c r="E227" s="29"/>
@@ -6121,10 +6143,10 @@
     <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="35"/>
       <c r="B228" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D228" s="35"/>
       <c r="E228" s="29"/>
@@ -6139,10 +6161,10 @@
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="35"/>
       <c r="B229" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D229" s="35"/>
       <c r="E229" s="29"/>
@@ -6157,10 +6179,10 @@
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="35"/>
       <c r="B230" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D230" s="35"/>
       <c r="E230" s="29"/>
@@ -6175,10 +6197,10 @@
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="35"/>
       <c r="B231" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D231" s="35"/>
       <c r="E231" s="29"/>
@@ -6193,10 +6215,10 @@
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="35"/>
       <c r="B232" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D232" s="35"/>
       <c r="E232" s="29"/>
@@ -6211,10 +6233,10 @@
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="35"/>
       <c r="B233" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D233" s="35"/>
       <c r="E233" s="29"/>
@@ -6229,10 +6251,10 @@
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="35"/>
       <c r="B234" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D234" s="35"/>
       <c r="E234" s="29"/>
@@ -6247,10 +6269,10 @@
     <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="35"/>
       <c r="B235" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D235" s="35"/>
       <c r="E235" s="29"/>
@@ -6265,10 +6287,10 @@
     <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="35"/>
       <c r="B236" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D236" s="35"/>
       <c r="E236" s="29"/>
@@ -6283,10 +6305,10 @@
     <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="35"/>
       <c r="B237" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C237" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D237" s="35"/>
       <c r="E237" s="29"/>
@@ -6301,10 +6323,10 @@
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="35"/>
       <c r="B238" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D238" s="35"/>
       <c r="E238" s="29"/>
@@ -6319,10 +6341,10 @@
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="35"/>
       <c r="B239" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D239" s="35"/>
       <c r="E239" s="29"/>
@@ -6337,10 +6359,10 @@
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="35"/>
       <c r="B240" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D240" s="35"/>
       <c r="E240" s="29"/>
@@ -6355,10 +6377,10 @@
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="35"/>
       <c r="B241" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D241" s="35"/>
       <c r="E241" s="29"/>
@@ -6373,10 +6395,10 @@
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="35"/>
       <c r="B242" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D242" s="35"/>
       <c r="E242" s="29"/>
@@ -6391,7 +6413,7 @@
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="35"/>
       <c r="B243" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C243" s="4" t="s">
         <v>163</v>
@@ -6409,7 +6431,7 @@
     <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="35"/>
       <c r="B244" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C244" s="4" t="s">
         <v>163</v>
@@ -6427,7 +6449,7 @@
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="35"/>
       <c r="B245" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C245" s="4" t="s">
         <v>163</v>
@@ -6445,7 +6467,7 @@
     <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="35"/>
       <c r="B246" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C246" s="4" t="s">
         <v>163</v>
@@ -6463,7 +6485,7 @@
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="35"/>
       <c r="B247" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C247" s="4" t="s">
         <v>163</v>
@@ -6481,7 +6503,7 @@
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="35"/>
       <c r="B248" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C248" s="4" t="s">
         <v>163</v>
@@ -6499,7 +6521,7 @@
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="35"/>
       <c r="B249" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C249" s="4" t="s">
         <v>163</v>
@@ -6517,7 +6539,7 @@
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="35"/>
       <c r="B250" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C250" s="4" t="s">
         <v>163</v>
@@ -6535,7 +6557,7 @@
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="35"/>
       <c r="B251" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C251" s="4" t="s">
         <v>163</v>
@@ -6553,7 +6575,7 @@
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="35"/>
       <c r="B252" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C252" s="4" t="s">
         <v>163</v>
@@ -6571,7 +6593,7 @@
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="35"/>
       <c r="B253" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C253" s="4" t="s">
         <v>163</v>
@@ -6589,7 +6611,7 @@
     <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="35"/>
       <c r="B254" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C254" s="4" t="s">
         <v>163</v>
@@ -6607,7 +6629,7 @@
     <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="35"/>
       <c r="B255" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C255" s="4" t="s">
         <v>163</v>
@@ -6625,7 +6647,7 @@
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="35"/>
       <c r="B256" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C256" s="4" t="s">
         <v>163</v>
@@ -6643,7 +6665,7 @@
     <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="35"/>
       <c r="B257" s="7" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="C257" s="4" t="s">
         <v>163</v>
@@ -6660,67 +6682,67 @@
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="35"/>
-      <c r="B258" s="7"/>
-      <c r="C258" s="4"/>
+      <c r="B258" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C258" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="D258" s="35"/>
       <c r="E258" s="29"/>
-      <c r="F258" s="19"/>
-      <c r="G258" s="20"/>
+      <c r="F258" s="19">
+        <v>1</v>
+      </c>
+      <c r="G258" s="20">
+        <v>0</v>
+      </c>
       <c r="H258" s="35"/>
     </row>
-    <row r="259" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="35"/>
-      <c r="B259" s="9"/>
-      <c r="C259" s="10"/>
+      <c r="B259" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C259" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="D259" s="35"/>
-      <c r="E259" s="30"/>
-      <c r="F259" s="21"/>
-      <c r="G259" s="22"/>
+      <c r="E259" s="29"/>
+      <c r="F259" s="19">
+        <v>1</v>
+      </c>
+      <c r="G259" s="20">
+        <v>0</v>
+      </c>
       <c r="H259" s="35"/>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="35"/>
-      <c r="B260" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C260" s="4" t="s">
-        <v>104</v>
-      </c>
+      <c r="B260" s="7"/>
+      <c r="C260" s="4"/>
       <c r="D260" s="35"/>
       <c r="E260" s="29"/>
-      <c r="F260" s="19">
-        <v>1</v>
-      </c>
-      <c r="G260" s="20">
-        <v>0</v>
-      </c>
+      <c r="F260" s="19"/>
+      <c r="G260" s="20"/>
       <c r="H260" s="35"/>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="35"/>
-      <c r="B261" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="C261" s="4" t="s">
-        <v>327</v>
-      </c>
+      <c r="B261" s="9"/>
+      <c r="C261" s="10"/>
       <c r="D261" s="35"/>
-      <c r="E261" s="29"/>
-      <c r="F261" s="19">
-        <v>1</v>
-      </c>
-      <c r="G261" s="20">
-        <v>0</v>
-      </c>
+      <c r="E261" s="30"/>
+      <c r="F261" s="21"/>
+      <c r="G261" s="22"/>
       <c r="H261" s="35"/>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" s="35"/>
       <c r="B262" s="7" t="s">
-        <v>326</v>
+        <v>0</v>
       </c>
       <c r="C262" s="4" t="s">
-        <v>328</v>
+        <v>104</v>
       </c>
       <c r="D262" s="35"/>
       <c r="E262" s="29"/>
@@ -6735,10 +6757,10 @@
     <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="35"/>
       <c r="B263" s="7" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="C263" s="4" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="D263" s="35"/>
       <c r="E263" s="29"/>
@@ -6750,49 +6772,49 @@
       </c>
       <c r="H263" s="35"/>
     </row>
-    <row r="264" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A264" s="37"/>
-      <c r="B264" s="13" t="s">
-        <v>369</v>
-      </c>
-      <c r="C264" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="D264" s="37"/>
-      <c r="E264" s="31"/>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A264" s="35"/>
+      <c r="B264" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C264" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="D264" s="35"/>
+      <c r="E264" s="29"/>
       <c r="F264" s="19">
         <v>1</v>
       </c>
       <c r="G264" s="20">
         <v>0</v>
       </c>
-      <c r="H264" s="37"/>
-    </row>
-    <row r="265" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A265" s="37"/>
-      <c r="B265" s="13" t="s">
-        <v>370</v>
-      </c>
-      <c r="C265" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="D265" s="37"/>
-      <c r="E265" s="31"/>
+      <c r="H264" s="35"/>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A265" s="35"/>
+      <c r="B265" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="C265" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="D265" s="35"/>
+      <c r="E265" s="29"/>
       <c r="F265" s="19">
         <v>1</v>
       </c>
       <c r="G265" s="20">
         <v>0</v>
       </c>
-      <c r="H265" s="37"/>
+      <c r="H265" s="35"/>
     </row>
     <row r="266" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A266" s="37"/>
       <c r="B266" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C266" s="14" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D266" s="37"/>
       <c r="E266" s="31"/>
@@ -6807,10 +6829,10 @@
     <row r="267" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A267" s="37"/>
       <c r="B267" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C267" s="14" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D267" s="37"/>
       <c r="E267" s="31"/>
@@ -6824,39 +6846,47 @@
     </row>
     <row r="268" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A268" s="37"/>
-      <c r="B268" s="7" t="s">
-        <v>436</v>
-      </c>
-      <c r="C268" s="4" t="s">
-        <v>437</v>
+      <c r="B268" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="C268" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="D268" s="37"/>
       <c r="E268" s="31"/>
-      <c r="F268" s="19"/>
-      <c r="G268" s="20"/>
+      <c r="F268" s="19">
+        <v>1</v>
+      </c>
+      <c r="G268" s="20">
+        <v>0</v>
+      </c>
       <c r="H268" s="37"/>
     </row>
     <row r="269" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A269" s="37"/>
-      <c r="B269" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="C269" s="4" t="s">
-        <v>441</v>
+      <c r="B269" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="C269" s="14" t="s">
+        <v>376</v>
       </c>
       <c r="D269" s="37"/>
       <c r="E269" s="31"/>
-      <c r="F269" s="19"/>
-      <c r="G269" s="20"/>
+      <c r="F269" s="19">
+        <v>1</v>
+      </c>
+      <c r="G269" s="20">
+        <v>0</v>
+      </c>
       <c r="H269" s="37"/>
     </row>
     <row r="270" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A270" s="37"/>
       <c r="B270" s="7" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C270" s="4" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D270" s="37"/>
       <c r="E270" s="31"/>
@@ -6864,49 +6894,41 @@
       <c r="G270" s="20"/>
       <c r="H270" s="37"/>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A271" s="35"/>
+    <row r="271" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A271" s="37"/>
       <c r="B271" s="7" t="s">
-        <v>353</v>
+        <v>438</v>
       </c>
       <c r="C271" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D271" s="35"/>
-      <c r="E271" s="29"/>
-      <c r="F271" s="19">
-        <v>1</v>
-      </c>
-      <c r="G271" s="20">
-        <v>0</v>
-      </c>
-      <c r="H271" s="35"/>
-    </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A272" s="35"/>
+        <v>441</v>
+      </c>
+      <c r="D271" s="37"/>
+      <c r="E271" s="31"/>
+      <c r="F271" s="19"/>
+      <c r="G271" s="20"/>
+      <c r="H271" s="37"/>
+    </row>
+    <row r="272" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A272" s="37"/>
       <c r="B272" s="7" t="s">
-        <v>354</v>
+        <v>439</v>
       </c>
       <c r="C272" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D272" s="35"/>
-      <c r="E272" s="29"/>
-      <c r="F272" s="19">
-        <v>1</v>
-      </c>
-      <c r="G272" s="20">
-        <v>0</v>
-      </c>
-      <c r="H272" s="35"/>
+        <v>440</v>
+      </c>
+      <c r="D272" s="37"/>
+      <c r="E272" s="31"/>
+      <c r="F272" s="19"/>
+      <c r="G272" s="20"/>
+      <c r="H272" s="37"/>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="35"/>
       <c r="B273" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C273" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D273" s="35"/>
       <c r="E273" s="29"/>
@@ -6921,10 +6943,10 @@
     <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="35"/>
       <c r="B274" s="7" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="C274" s="4" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="D274" s="35"/>
       <c r="E274" s="29"/>
@@ -6939,10 +6961,10 @@
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="35"/>
       <c r="B275" s="7" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="C275" s="4" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="D275" s="35"/>
       <c r="E275" s="29"/>
@@ -6957,10 +6979,10 @@
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="35"/>
       <c r="B276" s="7" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C276" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D276" s="35"/>
       <c r="E276" s="29"/>
@@ -6975,10 +6997,10 @@
     <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="35"/>
       <c r="B277" s="7" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
       <c r="C277" s="4" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
       <c r="D277" s="35"/>
       <c r="E277" s="29"/>
@@ -6993,10 +7015,10 @@
     <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="35"/>
       <c r="B278" s="7" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="C278" s="4" t="s">
-        <v>336</v>
+        <v>352</v>
       </c>
       <c r="D278" s="35"/>
       <c r="E278" s="29"/>
@@ -7011,10 +7033,10 @@
     <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="35"/>
       <c r="B279" s="7" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="C279" s="4" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="D279" s="35"/>
       <c r="E279" s="29"/>
@@ -7026,51 +7048,59 @@
       </c>
       <c r="H279" s="35"/>
     </row>
-    <row r="280" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" s="35"/>
-      <c r="B280" s="11"/>
-      <c r="C280" s="12"/>
+      <c r="B280" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="C280" s="4" t="s">
+        <v>336</v>
+      </c>
       <c r="D280" s="35"/>
-      <c r="E280" s="32"/>
-      <c r="F280" s="23"/>
-      <c r="G280" s="24"/>
+      <c r="E280" s="29"/>
+      <c r="F280" s="19">
+        <v>1</v>
+      </c>
+      <c r="G280" s="20">
+        <v>0</v>
+      </c>
       <c r="H280" s="35"/>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="35"/>
       <c r="B281" s="7" t="s">
-        <v>442</v>
+        <v>329</v>
       </c>
       <c r="C281" s="4" t="s">
-        <v>443</v>
+        <v>330</v>
       </c>
       <c r="D281" s="35"/>
       <c r="E281" s="29"/>
-      <c r="F281" s="19"/>
-      <c r="G281" s="20"/>
+      <c r="F281" s="19">
+        <v>1</v>
+      </c>
+      <c r="G281" s="20">
+        <v>0</v>
+      </c>
       <c r="H281" s="35"/>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="35"/>
-      <c r="B282" s="7" t="s">
-        <v>452</v>
-      </c>
-      <c r="C282" s="4" t="s">
-        <v>453</v>
-      </c>
+      <c r="B282" s="11"/>
+      <c r="C282" s="12"/>
       <c r="D282" s="35"/>
-      <c r="E282" s="29"/>
-      <c r="F282" s="19"/>
-      <c r="G282" s="20"/>
+      <c r="E282" s="32"/>
+      <c r="F282" s="23"/>
+      <c r="G282" s="24"/>
       <c r="H282" s="35"/>
     </row>
     <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283" s="35"/>
       <c r="B283" s="7" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C283" s="4" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D283" s="35"/>
       <c r="E283" s="29"/>
@@ -7078,25 +7108,53 @@
       <c r="G283" s="20"/>
       <c r="H283" s="35"/>
     </row>
-    <row r="284" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284" s="35"/>
-      <c r="B284" s="8"/>
-      <c r="C284" s="6"/>
+      <c r="B284" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="C284" s="4" t="s">
+        <v>453</v>
+      </c>
       <c r="D284" s="35"/>
-      <c r="E284" s="33"/>
-      <c r="F284" s="25"/>
-      <c r="G284" s="26"/>
+      <c r="E284" s="29"/>
+      <c r="F284" s="19"/>
+      <c r="G284" s="20"/>
       <c r="H284" s="35"/>
     </row>
-    <row r="285" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285" s="35"/>
-      <c r="B285" s="38"/>
-      <c r="C285" s="39"/>
+      <c r="B285" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="C285" s="4" t="s">
+        <v>445</v>
+      </c>
       <c r="D285" s="35"/>
-      <c r="E285" s="40"/>
-      <c r="F285" s="41"/>
-      <c r="G285" s="41"/>
+      <c r="E285" s="29"/>
+      <c r="F285" s="19"/>
+      <c r="G285" s="20"/>
       <c r="H285" s="35"/>
+    </row>
+    <row r="286" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A286" s="35"/>
+      <c r="B286" s="8"/>
+      <c r="C286" s="6"/>
+      <c r="D286" s="35"/>
+      <c r="E286" s="33"/>
+      <c r="F286" s="25"/>
+      <c r="G286" s="26"/>
+      <c r="H286" s="35"/>
+    </row>
+    <row r="287" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A287" s="35"/>
+      <c r="B287" s="38"/>
+      <c r="C287" s="39"/>
+      <c r="D287" s="35"/>
+      <c r="E287" s="40"/>
+      <c r="F287" s="41"/>
+      <c r="G287" s="41"/>
+      <c r="H287" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Penambahan API untuk schBudgeting.tblBudgetExpenseGroup
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="502">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -1604,6 +1604,30 @@
   </si>
   <si>
     <t>Mendapatkan Daftar Objek Pagu Anggaran</t>
+  </si>
+  <si>
+    <t>transaction.create.budgeting.setBudget</t>
+  </si>
+  <si>
+    <t>Menyimpan Data Baru Anggaran</t>
+  </si>
+  <si>
+    <t>transaction.create.budgeting.setBudgetExpenseGroup</t>
+  </si>
+  <si>
+    <t>Menyimpan Data Baru Kelompok Anggaran Belanja</t>
+  </si>
+  <si>
+    <t>transaction.update.budgeting.setBudgetExpenseGroup</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Kelompok Anggaran Belanja</t>
+  </si>
+  <si>
+    <t>transaction.read.budgeting.getDataListBudgetExpenseGroup</t>
+  </si>
+  <si>
+    <t>Mendapatkan Daftar Kelompok Anggaran Belanja</t>
   </si>
 </sst>
 </file>
@@ -2432,13 +2456,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H300"/>
+  <dimension ref="A1:H306"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B196" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B193" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C201" sqref="C201"/>
+      <selection pane="bottomRight" activeCell="C203" sqref="C203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3327,10 +3351,10 @@
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="35"/>
       <c r="B57" s="7" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>448</v>
+        <v>495</v>
       </c>
       <c r="D57" s="35"/>
       <c r="E57" s="29"/>
@@ -3341,10 +3365,10 @@
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="35"/>
       <c r="B58" s="7" t="s">
-        <v>450</v>
+        <v>496</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>451</v>
+        <v>497</v>
       </c>
       <c r="D58" s="35"/>
       <c r="E58" s="29"/>
@@ -3352,101 +3376,85 @@
       <c r="G58" s="20"/>
       <c r="H58" s="35"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="35"/>
-      <c r="B59" s="7" t="s">
-        <v>447</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>449</v>
-      </c>
+      <c r="B59" s="11"/>
+      <c r="C59" s="12"/>
       <c r="D59" s="35"/>
-      <c r="E59" s="29"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="20"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="24"/>
       <c r="H59" s="35"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="35"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="4"/>
+      <c r="B60" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>448</v>
+      </c>
       <c r="D60" s="35"/>
       <c r="E60" s="29"/>
       <c r="F60" s="19"/>
       <c r="G60" s="20"/>
       <c r="H60" s="35"/>
     </row>
-    <row r="61" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="35"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="10"/>
+      <c r="B61" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>451</v>
+      </c>
       <c r="D61" s="35"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="22"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="20"/>
       <c r="H61" s="35"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="35"/>
       <c r="B62" s="7" t="s">
-        <v>300</v>
+        <v>447</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>302</v>
+        <v>449</v>
       </c>
       <c r="D62" s="35"/>
       <c r="E62" s="29"/>
-      <c r="F62" s="19">
-        <v>1</v>
-      </c>
-      <c r="G62" s="20">
-        <v>0</v>
-      </c>
+      <c r="F62" s="19"/>
+      <c r="G62" s="20"/>
       <c r="H62" s="35"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="35"/>
-      <c r="B63" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>303</v>
-      </c>
+      <c r="B63" s="7"/>
+      <c r="C63" s="4"/>
       <c r="D63" s="35"/>
       <c r="E63" s="29"/>
-      <c r="F63" s="19">
-        <v>1</v>
-      </c>
-      <c r="G63" s="20">
-        <v>0</v>
-      </c>
+      <c r="F63" s="19"/>
+      <c r="G63" s="20"/>
       <c r="H63" s="35"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="35"/>
-      <c r="B64" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>299</v>
-      </c>
+      <c r="B64" s="9"/>
+      <c r="C64" s="10"/>
       <c r="D64" s="35"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="19">
-        <v>1</v>
-      </c>
-      <c r="G64" s="20">
-        <v>0</v>
-      </c>
+      <c r="E64" s="30"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="22"/>
       <c r="H64" s="35"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="35"/>
       <c r="B65" s="7" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D65" s="35"/>
       <c r="E65" s="29"/>
@@ -3461,10 +3469,10 @@
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="35"/>
       <c r="B66" s="7" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D66" s="35"/>
       <c r="E66" s="29"/>
@@ -3476,23 +3484,31 @@
       </c>
       <c r="H66" s="35"/>
     </row>
-    <row r="67" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="35"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="12"/>
+      <c r="B67" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>299</v>
+      </c>
       <c r="D67" s="35"/>
-      <c r="E67" s="32"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="24"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="19">
+        <v>1</v>
+      </c>
+      <c r="G67" s="20">
+        <v>0</v>
+      </c>
       <c r="H67" s="35"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="35"/>
       <c r="B68" s="7" t="s">
-        <v>50</v>
+        <v>305</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>92</v>
+        <v>306</v>
       </c>
       <c r="D68" s="35"/>
       <c r="E68" s="29"/>
@@ -3507,10 +3523,10 @@
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="35"/>
       <c r="B69" s="7" t="s">
-        <v>94</v>
+        <v>304</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>95</v>
+        <v>307</v>
       </c>
       <c r="D69" s="35"/>
       <c r="E69" s="29"/>
@@ -3522,31 +3538,23 @@
       </c>
       <c r="H69" s="35"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="35"/>
-      <c r="B70" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>312</v>
-      </c>
+      <c r="B70" s="11"/>
+      <c r="C70" s="12"/>
       <c r="D70" s="35"/>
-      <c r="E70" s="29"/>
-      <c r="F70" s="19">
-        <v>1</v>
-      </c>
-      <c r="G70" s="20">
-        <v>0</v>
-      </c>
+      <c r="E70" s="32"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="24"/>
       <c r="H70" s="35"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="35"/>
       <c r="B71" s="7" t="s">
-        <v>313</v>
+        <v>50</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>314</v>
+        <v>92</v>
       </c>
       <c r="D71" s="35"/>
       <c r="E71" s="29"/>
@@ -3561,10 +3569,10 @@
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="35"/>
       <c r="B72" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D72" s="35"/>
       <c r="E72" s="29"/>
@@ -3579,10 +3587,10 @@
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="35"/>
       <c r="B73" s="7" t="s">
-        <v>109</v>
+        <v>311</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>110</v>
+        <v>312</v>
       </c>
       <c r="D73" s="35"/>
       <c r="E73" s="29"/>
@@ -3597,10 +3605,10 @@
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="35"/>
       <c r="B74" s="7" t="s">
-        <v>123</v>
+        <v>313</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>126</v>
+        <v>314</v>
       </c>
       <c r="D74" s="35"/>
       <c r="E74" s="29"/>
@@ -3615,10 +3623,10 @@
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="35"/>
       <c r="B75" s="7" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="D75" s="35"/>
       <c r="E75" s="29"/>
@@ -3633,10 +3641,10 @@
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="35"/>
       <c r="B76" s="7" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D76" s="35"/>
       <c r="E76" s="29"/>
@@ -3651,10 +3659,10 @@
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="35"/>
       <c r="B77" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D77" s="35"/>
       <c r="E77" s="29"/>
@@ -3669,10 +3677,10 @@
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="35"/>
       <c r="B78" s="7" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="D78" s="35"/>
       <c r="E78" s="29"/>
@@ -3687,10 +3695,10 @@
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="35"/>
       <c r="B79" s="7" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>381</v>
+        <v>100</v>
       </c>
       <c r="D79" s="35"/>
       <c r="E79" s="29"/>
@@ -3705,10 +3713,10 @@
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="35"/>
       <c r="B80" s="7" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>382</v>
+        <v>128</v>
       </c>
       <c r="D80" s="35"/>
       <c r="E80" s="29"/>
@@ -3723,10 +3731,10 @@
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="35"/>
       <c r="B81" s="7" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>383</v>
+        <v>101</v>
       </c>
       <c r="D81" s="35"/>
       <c r="E81" s="29"/>
@@ -3741,10 +3749,10 @@
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="35"/>
       <c r="B82" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D82" s="35"/>
       <c r="E82" s="29"/>
@@ -3759,10 +3767,10 @@
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="35"/>
       <c r="B83" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>114</v>
+        <v>382</v>
       </c>
       <c r="D83" s="35"/>
       <c r="E83" s="29"/>
@@ -3777,10 +3785,10 @@
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="35"/>
       <c r="B84" s="7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>115</v>
+        <v>383</v>
       </c>
       <c r="D84" s="35"/>
       <c r="E84" s="29"/>
@@ -3795,10 +3803,10 @@
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="35"/>
       <c r="B85" s="7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>116</v>
+        <v>384</v>
       </c>
       <c r="D85" s="35"/>
       <c r="E85" s="29"/>
@@ -3813,10 +3821,10 @@
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="35"/>
       <c r="B86" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D86" s="35"/>
       <c r="E86" s="29"/>
@@ -3831,10 +3839,10 @@
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="35"/>
       <c r="B87" s="7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D87" s="35"/>
       <c r="E87" s="29"/>
@@ -3849,10 +3857,10 @@
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="35"/>
       <c r="B88" s="7" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D88" s="35"/>
       <c r="E88" s="29"/>
@@ -3867,10 +3875,10 @@
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="35"/>
       <c r="B89" s="7" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>198</v>
+        <v>119</v>
       </c>
       <c r="D89" s="35"/>
       <c r="E89" s="29"/>
@@ -3885,10 +3893,10 @@
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="35"/>
       <c r="B90" s="7" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>199</v>
+        <v>120</v>
       </c>
       <c r="D90" s="35"/>
       <c r="E90" s="29"/>
@@ -3903,10 +3911,10 @@
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="35"/>
       <c r="B91" s="7" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>200</v>
+        <v>122</v>
       </c>
       <c r="D91" s="35"/>
       <c r="E91" s="29"/>
@@ -3921,10 +3929,10 @@
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="35"/>
       <c r="B92" s="7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D92" s="35"/>
       <c r="E92" s="29"/>
@@ -3939,10 +3947,10 @@
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="35"/>
       <c r="B93" s="7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D93" s="35"/>
       <c r="E93" s="29"/>
@@ -3957,10 +3965,10 @@
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="35"/>
       <c r="B94" s="7" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D94" s="35"/>
       <c r="E94" s="29"/>
@@ -3975,10 +3983,10 @@
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="35"/>
       <c r="B95" s="7" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D95" s="35"/>
       <c r="E95" s="29"/>
@@ -3993,10 +4001,10 @@
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="35"/>
       <c r="B96" s="7" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D96" s="35"/>
       <c r="E96" s="29"/>
@@ -4011,10 +4019,10 @@
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="35"/>
       <c r="B97" s="7" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D97" s="35"/>
       <c r="E97" s="29"/>
@@ -4029,10 +4037,10 @@
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="35"/>
       <c r="B98" s="7" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D98" s="35"/>
       <c r="E98" s="29"/>
@@ -4047,10 +4055,10 @@
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="35"/>
       <c r="B99" s="7" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D99" s="35"/>
       <c r="E99" s="29"/>
@@ -4065,10 +4073,10 @@
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="35"/>
       <c r="B100" s="7" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D100" s="35"/>
       <c r="E100" s="29"/>
@@ -4083,10 +4091,10 @@
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="35"/>
       <c r="B101" s="7" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D101" s="35"/>
       <c r="E101" s="29"/>
@@ -4101,10 +4109,10 @@
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="35"/>
       <c r="B102" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D102" s="35"/>
       <c r="E102" s="29"/>
@@ -4119,10 +4127,10 @@
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="35"/>
       <c r="B103" s="7" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D103" s="35"/>
       <c r="E103" s="29"/>
@@ -4134,43 +4142,49 @@
       </c>
       <c r="H103" s="35"/>
     </row>
-    <row r="104" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
-      <c r="B104" s="11"/>
-      <c r="C104" s="12"/>
+      <c r="B104" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>211</v>
+      </c>
       <c r="D104" s="35"/>
-      <c r="E104" s="32"/>
-      <c r="F104" s="23"/>
-      <c r="G104" s="24"/>
+      <c r="E104" s="29"/>
+      <c r="F104" s="19">
+        <v>1</v>
+      </c>
+      <c r="G104" s="20">
+        <v>0</v>
+      </c>
       <c r="H104" s="35"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="35"/>
       <c r="B105" s="7" t="s">
-        <v>234</v>
+        <v>130</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="D105" s="35"/>
-      <c r="E105" s="29">
-        <v>44188</v>
-      </c>
+      <c r="E105" s="29"/>
       <c r="F105" s="19">
         <v>1</v>
       </c>
       <c r="G105" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H105" s="35"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="35"/>
       <c r="B106" s="7" t="s">
-        <v>235</v>
+        <v>129</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>239</v>
+        <v>213</v>
       </c>
       <c r="D106" s="35"/>
       <c r="E106" s="29"/>
@@ -4182,49 +4196,43 @@
       </c>
       <c r="H106" s="35"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="35"/>
-      <c r="B107" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>240</v>
-      </c>
+      <c r="B107" s="11"/>
+      <c r="C107" s="12"/>
       <c r="D107" s="35"/>
-      <c r="E107" s="29"/>
-      <c r="F107" s="19">
-        <v>1</v>
-      </c>
-      <c r="G107" s="20">
-        <v>0</v>
-      </c>
+      <c r="E107" s="32"/>
+      <c r="F107" s="23"/>
+      <c r="G107" s="24"/>
       <c r="H107" s="35"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="35"/>
       <c r="B108" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D108" s="35"/>
-      <c r="E108" s="29"/>
+      <c r="E108" s="29">
+        <v>44188</v>
+      </c>
       <c r="F108" s="19">
         <v>1</v>
       </c>
       <c r="G108" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H108" s="35"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="35"/>
       <c r="B109" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D109" s="35"/>
       <c r="E109" s="29"/>
@@ -4236,23 +4244,31 @@
       </c>
       <c r="H109" s="35"/>
     </row>
-    <row r="110" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="35"/>
-      <c r="B110" s="11"/>
-      <c r="C110" s="12"/>
+      <c r="B110" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="D110" s="35"/>
-      <c r="E110" s="32"/>
-      <c r="F110" s="23"/>
-      <c r="G110" s="24"/>
+      <c r="E110" s="29"/>
+      <c r="F110" s="19">
+        <v>1</v>
+      </c>
+      <c r="G110" s="20">
+        <v>0</v>
+      </c>
       <c r="H110" s="35"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="35"/>
       <c r="B111" s="7" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="D111" s="35"/>
       <c r="E111" s="29"/>
@@ -4267,10 +4283,10 @@
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="35"/>
       <c r="B112" s="7" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="D112" s="35"/>
       <c r="E112" s="29"/>
@@ -4282,31 +4298,23 @@
       </c>
       <c r="H112" s="35"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="35"/>
-      <c r="B113" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C113" s="4" t="s">
-        <v>225</v>
-      </c>
+      <c r="B113" s="11"/>
+      <c r="C113" s="12"/>
       <c r="D113" s="35"/>
-      <c r="E113" s="29"/>
-      <c r="F113" s="19">
-        <v>1</v>
-      </c>
-      <c r="G113" s="20">
-        <v>0</v>
-      </c>
+      <c r="E113" s="32"/>
+      <c r="F113" s="23"/>
+      <c r="G113" s="24"/>
       <c r="H113" s="35"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="35"/>
       <c r="B114" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D114" s="35"/>
       <c r="E114" s="29"/>
@@ -4321,10 +4329,10 @@
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="35"/>
       <c r="B115" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D115" s="35"/>
       <c r="E115" s="29"/>
@@ -4336,23 +4344,31 @@
       </c>
       <c r="H115" s="35"/>
     </row>
-    <row r="116" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="35"/>
-      <c r="B116" s="11"/>
-      <c r="C116" s="12"/>
+      <c r="B116" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>225</v>
+      </c>
       <c r="D116" s="35"/>
-      <c r="E116" s="32"/>
-      <c r="F116" s="23"/>
-      <c r="G116" s="24"/>
+      <c r="E116" s="29"/>
+      <c r="F116" s="19">
+        <v>1</v>
+      </c>
+      <c r="G116" s="20">
+        <v>0</v>
+      </c>
       <c r="H116" s="35"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="35"/>
       <c r="B117" s="7" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D117" s="35"/>
       <c r="E117" s="29"/>
@@ -4364,41 +4380,41 @@
       </c>
       <c r="H117" s="35"/>
     </row>
-    <row r="118" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="35"/>
-      <c r="B118" s="11"/>
-      <c r="C118" s="12"/>
+      <c r="B118" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>227</v>
+      </c>
       <c r="D118" s="35"/>
-      <c r="E118" s="32"/>
-      <c r="F118" s="23"/>
-      <c r="G118" s="24"/>
+      <c r="E118" s="29"/>
+      <c r="F118" s="19">
+        <v>1</v>
+      </c>
+      <c r="G118" s="20">
+        <v>0</v>
+      </c>
       <c r="H118" s="35"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="35"/>
-      <c r="B119" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>232</v>
-      </c>
+      <c r="B119" s="11"/>
+      <c r="C119" s="12"/>
       <c r="D119" s="35"/>
-      <c r="E119" s="29"/>
-      <c r="F119" s="19">
-        <v>1</v>
-      </c>
-      <c r="G119" s="20">
-        <v>0</v>
-      </c>
+      <c r="E119" s="32"/>
+      <c r="F119" s="23"/>
+      <c r="G119" s="24"/>
       <c r="H119" s="35"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="35"/>
       <c r="B120" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D120" s="35"/>
       <c r="E120" s="29"/>
@@ -4423,10 +4439,10 @@
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="35"/>
       <c r="B122" s="7" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="D122" s="35"/>
       <c r="E122" s="29"/>
@@ -4438,41 +4454,41 @@
       </c>
       <c r="H122" s="35"/>
     </row>
-    <row r="123" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="35"/>
-      <c r="B123" s="11"/>
-      <c r="C123" s="12"/>
+      <c r="B123" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="D123" s="35"/>
-      <c r="E123" s="32"/>
-      <c r="F123" s="23"/>
-      <c r="G123" s="24"/>
+      <c r="E123" s="29"/>
+      <c r="F123" s="19">
+        <v>1</v>
+      </c>
+      <c r="G123" s="20">
+        <v>0</v>
+      </c>
       <c r="H123" s="35"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="35"/>
-      <c r="B124" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>247</v>
-      </c>
+      <c r="B124" s="11"/>
+      <c r="C124" s="12"/>
       <c r="D124" s="35"/>
-      <c r="E124" s="29"/>
-      <c r="F124" s="19">
-        <v>1</v>
-      </c>
-      <c r="G124" s="20">
-        <v>0</v>
-      </c>
+      <c r="E124" s="32"/>
+      <c r="F124" s="23"/>
+      <c r="G124" s="24"/>
       <c r="H124" s="35"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="35"/>
       <c r="B125" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="D125" s="35"/>
       <c r="E125" s="29"/>
@@ -4484,31 +4500,23 @@
       </c>
       <c r="H125" s="35"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="35"/>
-      <c r="B126" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="C126" s="4" t="s">
-        <v>284</v>
-      </c>
+      <c r="B126" s="11"/>
+      <c r="C126" s="12"/>
       <c r="D126" s="35"/>
-      <c r="E126" s="29"/>
-      <c r="F126" s="19">
-        <v>1</v>
-      </c>
-      <c r="G126" s="20">
-        <v>0</v>
-      </c>
+      <c r="E126" s="32"/>
+      <c r="F126" s="23"/>
+      <c r="G126" s="24"/>
       <c r="H126" s="35"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="35"/>
       <c r="B127" s="7" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="D127" s="35"/>
       <c r="E127" s="29"/>
@@ -4523,10 +4531,10 @@
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="35"/>
       <c r="B128" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D128" s="35"/>
       <c r="E128" s="29"/>
@@ -4541,10 +4549,10 @@
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="35"/>
       <c r="B129" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="D129" s="35"/>
       <c r="E129" s="29"/>
@@ -4559,10 +4567,10 @@
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="35"/>
       <c r="B130" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="D130" s="35"/>
       <c r="E130" s="29"/>
@@ -4577,10 +4585,10 @@
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="35"/>
       <c r="B131" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D131" s="35"/>
       <c r="E131" s="29"/>
@@ -4595,10 +4603,10 @@
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="35"/>
       <c r="B132" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
       <c r="D132" s="35"/>
       <c r="E132" s="29"/>
@@ -4613,10 +4621,10 @@
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="35"/>
       <c r="B133" s="7" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D133" s="35"/>
       <c r="E133" s="29"/>
@@ -4631,10 +4639,10 @@
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="35"/>
       <c r="B134" s="7" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>265</v>
+        <v>286</v>
       </c>
       <c r="D134" s="35"/>
       <c r="E134" s="29"/>
@@ -4649,10 +4657,10 @@
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="35"/>
       <c r="B135" s="7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="D135" s="35"/>
       <c r="E135" s="29"/>
@@ -4667,10 +4675,10 @@
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="35"/>
       <c r="B136" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="D136" s="35"/>
       <c r="E136" s="29"/>
@@ -4685,10 +4693,10 @@
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="35"/>
       <c r="B137" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D137" s="35"/>
       <c r="E137" s="29"/>
@@ -4703,10 +4711,10 @@
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="35"/>
       <c r="B138" s="7" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="D138" s="35"/>
       <c r="E138" s="29"/>
@@ -4721,10 +4729,10 @@
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="35"/>
       <c r="B139" s="7" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D139" s="35"/>
       <c r="E139" s="29"/>
@@ -4739,10 +4747,10 @@
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="35"/>
       <c r="B140" s="7" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D140" s="35"/>
       <c r="E140" s="29"/>
@@ -4757,10 +4765,10 @@
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="35"/>
       <c r="B141" s="7" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="D141" s="35"/>
       <c r="E141" s="29"/>
@@ -4775,10 +4783,10 @@
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="35"/>
       <c r="B142" s="7" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D142" s="35"/>
       <c r="E142" s="29"/>
@@ -4793,10 +4801,10 @@
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="35"/>
       <c r="B143" s="7" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="D143" s="35"/>
       <c r="E143" s="29"/>
@@ -4811,10 +4819,10 @@
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="35"/>
       <c r="B144" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D144" s="35"/>
       <c r="E144" s="29"/>
@@ -4826,23 +4834,31 @@
       </c>
       <c r="H144" s="35"/>
     </row>
-    <row r="145" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="35"/>
-      <c r="B145" s="11"/>
-      <c r="C145" s="12"/>
+      <c r="B145" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>281</v>
+      </c>
       <c r="D145" s="35"/>
-      <c r="E145" s="32"/>
-      <c r="F145" s="23"/>
-      <c r="G145" s="24"/>
+      <c r="E145" s="29"/>
+      <c r="F145" s="19">
+        <v>1</v>
+      </c>
+      <c r="G145" s="20">
+        <v>0</v>
+      </c>
       <c r="H145" s="35"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="35"/>
       <c r="B146" s="7" t="s">
-        <v>144</v>
+        <v>276</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>214</v>
+        <v>280</v>
       </c>
       <c r="D146" s="35"/>
       <c r="E146" s="29"/>
@@ -4857,10 +4873,10 @@
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="35"/>
       <c r="B147" s="7" t="s">
-        <v>215</v>
+        <v>277</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>216</v>
+        <v>279</v>
       </c>
       <c r="D147" s="35"/>
       <c r="E147" s="29"/>
@@ -4885,10 +4901,10 @@
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="35"/>
       <c r="B149" s="7" t="s">
-        <v>288</v>
+        <v>144</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>296</v>
+        <v>214</v>
       </c>
       <c r="D149" s="35"/>
       <c r="E149" s="29"/>
@@ -4903,10 +4919,10 @@
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="35"/>
       <c r="B150" s="7" t="s">
-        <v>289</v>
+        <v>215</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>290</v>
+        <v>216</v>
       </c>
       <c r="D150" s="35"/>
       <c r="E150" s="29"/>
@@ -4918,31 +4934,23 @@
       </c>
       <c r="H150" s="35"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="35"/>
-      <c r="B151" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C151" s="4" t="s">
-        <v>297</v>
-      </c>
+      <c r="B151" s="11"/>
+      <c r="C151" s="12"/>
       <c r="D151" s="35"/>
-      <c r="E151" s="29"/>
-      <c r="F151" s="19">
-        <v>1</v>
-      </c>
-      <c r="G151" s="20">
-        <v>0</v>
-      </c>
+      <c r="E151" s="32"/>
+      <c r="F151" s="23"/>
+      <c r="G151" s="24"/>
       <c r="H151" s="35"/>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="35"/>
       <c r="B152" s="7" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D152" s="35"/>
       <c r="E152" s="29"/>
@@ -4957,10 +4965,10 @@
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="35"/>
       <c r="B153" s="7" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D153" s="35"/>
       <c r="E153" s="29"/>
@@ -4974,95 +4982,89 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="35"/>
-      <c r="B154" s="7"/>
-      <c r="C154" s="4"/>
+      <c r="B154" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>297</v>
+      </c>
       <c r="D154" s="35"/>
       <c r="E154" s="29"/>
-      <c r="F154" s="19"/>
-      <c r="G154" s="20"/>
+      <c r="F154" s="19">
+        <v>1</v>
+      </c>
+      <c r="G154" s="20">
+        <v>0</v>
+      </c>
       <c r="H154" s="35"/>
     </row>
-    <row r="155" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="35"/>
-      <c r="B155" s="9"/>
-      <c r="C155" s="10"/>
+      <c r="B155" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>293</v>
+      </c>
       <c r="D155" s="35"/>
-      <c r="E155" s="30"/>
-      <c r="F155" s="21"/>
-      <c r="G155" s="22"/>
+      <c r="E155" s="29"/>
+      <c r="F155" s="19">
+        <v>1</v>
+      </c>
+      <c r="G155" s="20">
+        <v>0</v>
+      </c>
       <c r="H155" s="35"/>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="35"/>
       <c r="B156" s="7" t="s">
-        <v>52</v>
+        <v>294</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>53</v>
+        <v>295</v>
       </c>
       <c r="D156" s="35"/>
-      <c r="E156" s="29">
-        <v>44207</v>
-      </c>
+      <c r="E156" s="29"/>
       <c r="F156" s="19">
         <v>1</v>
       </c>
       <c r="G156" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H156" s="35"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="35"/>
-      <c r="B157" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C157" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="B157" s="7"/>
+      <c r="C157" s="4"/>
       <c r="D157" s="35"/>
-      <c r="E157" s="29">
-        <v>44211</v>
-      </c>
-      <c r="F157" s="19">
-        <v>1</v>
-      </c>
-      <c r="G157" s="20">
-        <v>1</v>
-      </c>
+      <c r="E157" s="29"/>
+      <c r="F157" s="19"/>
+      <c r="G157" s="20"/>
       <c r="H157" s="35"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="35"/>
-      <c r="B158" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C158" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="B158" s="9"/>
+      <c r="C158" s="10"/>
       <c r="D158" s="35"/>
-      <c r="E158" s="29">
-        <v>44211</v>
-      </c>
-      <c r="F158" s="19">
-        <v>1</v>
-      </c>
-      <c r="G158" s="20">
-        <v>1</v>
-      </c>
+      <c r="E158" s="30"/>
+      <c r="F158" s="21"/>
+      <c r="G158" s="22"/>
       <c r="H158" s="35"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="35"/>
       <c r="B159" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D159" s="35"/>
       <c r="E159" s="29">
-        <v>44211</v>
+        <v>44207</v>
       </c>
       <c r="F159" s="19">
         <v>1</v>
@@ -5075,10 +5077,10 @@
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="35"/>
       <c r="B160" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D160" s="35"/>
       <c r="E160" s="29">
@@ -5095,10 +5097,10 @@
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="35"/>
       <c r="B161" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D161" s="35"/>
       <c r="E161" s="29">
@@ -5115,10 +5117,10 @@
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="35"/>
       <c r="B162" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D162" s="35"/>
       <c r="E162" s="29">
@@ -5135,10 +5137,10 @@
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="35"/>
       <c r="B163" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D163" s="35"/>
       <c r="E163" s="29">
@@ -5155,10 +5157,10 @@
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="35"/>
       <c r="B164" s="7" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D164" s="35"/>
       <c r="E164" s="29">
@@ -5175,10 +5177,10 @@
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="35"/>
       <c r="B165" s="7" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D165" s="35"/>
       <c r="E165" s="29">
@@ -5195,10 +5197,10 @@
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="35"/>
       <c r="B166" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D166" s="35"/>
       <c r="E166" s="29">
@@ -5215,10 +5217,10 @@
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="35"/>
       <c r="B167" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D167" s="35"/>
       <c r="E167" s="29">
@@ -5235,10 +5237,10 @@
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="35"/>
       <c r="B168" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D168" s="35"/>
       <c r="E168" s="29">
@@ -5255,10 +5257,10 @@
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="35"/>
       <c r="B169" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D169" s="35"/>
       <c r="E169" s="29">
@@ -5275,10 +5277,10 @@
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="35"/>
       <c r="B170" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D170" s="35"/>
       <c r="E170" s="29">
@@ -5295,10 +5297,10 @@
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="35"/>
       <c r="B171" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>207</v>
+        <v>84</v>
       </c>
       <c r="D171" s="35"/>
       <c r="E171" s="29">
@@ -5315,10 +5317,10 @@
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="35"/>
       <c r="B172" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D172" s="35"/>
       <c r="E172" s="29">
@@ -5335,10 +5337,10 @@
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="35"/>
       <c r="B173" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D173" s="35"/>
       <c r="E173" s="29">
@@ -5355,10 +5357,10 @@
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="35"/>
       <c r="B174" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>90</v>
+        <v>207</v>
       </c>
       <c r="D174" s="35"/>
       <c r="E174" s="29">
@@ -5375,10 +5377,10 @@
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="35"/>
       <c r="B175" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D175" s="35"/>
       <c r="E175" s="29">
@@ -5394,99 +5396,105 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="35"/>
-      <c r="B176" s="7"/>
-      <c r="C176" s="4"/>
+      <c r="B176" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C176" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="D176" s="35"/>
-      <c r="E176" s="29"/>
-      <c r="F176" s="19"/>
-      <c r="G176" s="20"/>
+      <c r="E176" s="29">
+        <v>44211</v>
+      </c>
+      <c r="F176" s="19">
+        <v>1</v>
+      </c>
+      <c r="G176" s="20">
+        <v>1</v>
+      </c>
       <c r="H176" s="35"/>
     </row>
-    <row r="177" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="35"/>
-      <c r="B177" s="9"/>
-      <c r="C177" s="10"/>
+      <c r="B177" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="D177" s="35"/>
-      <c r="E177" s="30"/>
-      <c r="F177" s="21"/>
-      <c r="G177" s="22"/>
+      <c r="E177" s="29">
+        <v>44211</v>
+      </c>
+      <c r="F177" s="19">
+        <v>1</v>
+      </c>
+      <c r="G177" s="20">
+        <v>1</v>
+      </c>
       <c r="H177" s="35"/>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="35"/>
       <c r="B178" s="7" t="s">
-        <v>422</v>
+        <v>79</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>423</v>
+        <v>91</v>
       </c>
       <c r="D178" s="35"/>
-      <c r="E178" s="29"/>
-      <c r="F178" s="19"/>
-      <c r="G178" s="20"/>
+      <c r="E178" s="29">
+        <v>44211</v>
+      </c>
+      <c r="F178" s="19">
+        <v>1</v>
+      </c>
+      <c r="G178" s="20">
+        <v>1</v>
+      </c>
       <c r="H178" s="35"/>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="35"/>
-      <c r="B179" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C179" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="B179" s="7"/>
+      <c r="C179" s="4"/>
       <c r="D179" s="35"/>
       <c r="E179" s="29"/>
-      <c r="F179" s="19">
-        <v>1</v>
-      </c>
-      <c r="G179" s="20">
-        <v>0</v>
-      </c>
+      <c r="F179" s="19"/>
+      <c r="G179" s="20"/>
       <c r="H179" s="35"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="35"/>
-      <c r="B180" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C180" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="B180" s="9"/>
+      <c r="C180" s="10"/>
       <c r="D180" s="35"/>
-      <c r="E180" s="29"/>
-      <c r="F180" s="19">
-        <v>1</v>
-      </c>
-      <c r="G180" s="20">
-        <v>0</v>
-      </c>
+      <c r="E180" s="30"/>
+      <c r="F180" s="21"/>
+      <c r="G180" s="22"/>
       <c r="H180" s="35"/>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="35"/>
       <c r="B181" s="7" t="s">
-        <v>16</v>
+        <v>422</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>18</v>
+        <v>423</v>
       </c>
       <c r="D181" s="35"/>
       <c r="E181" s="29"/>
-      <c r="F181" s="19">
-        <v>1</v>
-      </c>
-      <c r="G181" s="20">
-        <v>0</v>
-      </c>
+      <c r="F181" s="19"/>
+      <c r="G181" s="20"/>
       <c r="H181" s="35"/>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="35"/>
       <c r="B182" s="7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D182" s="35"/>
       <c r="E182" s="29"/>
@@ -5501,10 +5509,10 @@
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="35"/>
       <c r="B183" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D183" s="35"/>
       <c r="E183" s="29"/>
@@ -5519,10 +5527,10 @@
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="35"/>
       <c r="B184" s="7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D184" s="35"/>
       <c r="E184" s="29"/>
@@ -5537,10 +5545,10 @@
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="35"/>
       <c r="B185" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D185" s="35"/>
       <c r="E185" s="29"/>
@@ -5555,10 +5563,10 @@
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="35"/>
       <c r="B186" s="7" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D186" s="35"/>
       <c r="E186" s="29"/>
@@ -5573,10 +5581,10 @@
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="35"/>
       <c r="B187" s="7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D187" s="35"/>
       <c r="E187" s="29"/>
@@ -5591,10 +5599,10 @@
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="35"/>
       <c r="B188" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D188" s="35"/>
       <c r="E188" s="29"/>
@@ -5609,10 +5617,10 @@
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="35"/>
       <c r="B189" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D189" s="35"/>
       <c r="E189" s="29"/>
@@ -5627,10 +5635,10 @@
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="35"/>
       <c r="B190" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="D190" s="35"/>
       <c r="E190" s="29"/>
@@ -5645,10 +5653,10 @@
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="35"/>
       <c r="B191" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D191" s="35"/>
       <c r="E191" s="29"/>
@@ -5663,10 +5671,10 @@
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="35"/>
       <c r="B192" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D192" s="35"/>
       <c r="E192" s="29"/>
@@ -5681,10 +5689,10 @@
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="35"/>
       <c r="B193" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D193" s="35"/>
       <c r="E193" s="29"/>
@@ -5699,10 +5707,10 @@
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="35"/>
       <c r="B194" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C194" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
+      </c>
+      <c r="C194" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D194" s="35"/>
       <c r="E194" s="29"/>
@@ -5717,10 +5725,10 @@
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="35"/>
       <c r="B195" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D195" s="35"/>
       <c r="E195" s="29"/>
@@ -5735,10 +5743,10 @@
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="35"/>
       <c r="B196" s="7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D196" s="35"/>
       <c r="E196" s="29"/>
@@ -5753,10 +5761,10 @@
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="35"/>
       <c r="B197" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C197" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+      <c r="C197" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D197" s="35"/>
       <c r="E197" s="29"/>
@@ -5768,65 +5776,77 @@
       </c>
       <c r="H197" s="35"/>
     </row>
-    <row r="198" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="35"/>
-      <c r="B198" s="11"/>
-      <c r="C198" s="12"/>
+      <c r="B198" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="D198" s="35"/>
-      <c r="E198" s="32"/>
-      <c r="F198" s="23"/>
-      <c r="G198" s="24"/>
+      <c r="E198" s="29"/>
+      <c r="F198" s="19">
+        <v>1</v>
+      </c>
+      <c r="G198" s="20">
+        <v>0</v>
+      </c>
       <c r="H198" s="35"/>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="35"/>
       <c r="B199" s="7" t="s">
-        <v>484</v>
+        <v>47</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>487</v>
+        <v>36</v>
       </c>
       <c r="D199" s="35"/>
       <c r="E199" s="29"/>
-      <c r="F199" s="19"/>
-      <c r="G199" s="20"/>
+      <c r="F199" s="19">
+        <v>1</v>
+      </c>
+      <c r="G199" s="20">
+        <v>0</v>
+      </c>
       <c r="H199" s="35"/>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="35"/>
       <c r="B200" s="7" t="s">
-        <v>490</v>
+        <v>48</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>491</v>
+        <v>49</v>
       </c>
       <c r="D200" s="35"/>
       <c r="E200" s="29"/>
-      <c r="F200" s="19"/>
-      <c r="G200" s="20"/>
+      <c r="F200" s="19">
+        <v>1</v>
+      </c>
+      <c r="G200" s="20">
+        <v>0</v>
+      </c>
       <c r="H200" s="35"/>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="35"/>
-      <c r="B201" s="7" t="s">
-        <v>492</v>
-      </c>
-      <c r="C201" s="4" t="s">
-        <v>493</v>
-      </c>
+      <c r="B201" s="11"/>
+      <c r="C201" s="12"/>
       <c r="D201" s="35"/>
-      <c r="E201" s="29"/>
-      <c r="F201" s="19"/>
-      <c r="G201" s="20"/>
+      <c r="E201" s="32"/>
+      <c r="F201" s="23"/>
+      <c r="G201" s="24"/>
       <c r="H201" s="35"/>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="35"/>
       <c r="B202" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D202" s="35"/>
       <c r="E202" s="29"/>
@@ -5837,10 +5857,10 @@
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="35"/>
       <c r="B203" s="7" t="s">
-        <v>486</v>
+        <v>500</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>489</v>
+        <v>501</v>
       </c>
       <c r="D203" s="35"/>
       <c r="E203" s="29"/>
@@ -5848,23 +5868,27 @@
       <c r="G203" s="20"/>
       <c r="H203" s="35"/>
     </row>
-    <row r="204" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="35"/>
-      <c r="B204" s="11"/>
-      <c r="C204" s="12"/>
+      <c r="B204" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="C204" s="4" t="s">
+        <v>491</v>
+      </c>
       <c r="D204" s="35"/>
-      <c r="E204" s="32"/>
-      <c r="F204" s="23"/>
-      <c r="G204" s="24"/>
+      <c r="E204" s="29"/>
+      <c r="F204" s="19"/>
+      <c r="G204" s="20"/>
       <c r="H204" s="35"/>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="35"/>
       <c r="B205" s="7" t="s">
-        <v>424</v>
+        <v>492</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>425</v>
+        <v>493</v>
       </c>
       <c r="D205" s="35"/>
       <c r="E205" s="29"/>
@@ -5875,10 +5899,10 @@
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="35"/>
       <c r="B206" s="7" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="D206" s="35"/>
       <c r="E206" s="29"/>
@@ -5886,37 +5910,37 @@
       <c r="G206" s="20"/>
       <c r="H206" s="35"/>
     </row>
-    <row r="207" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="35"/>
-      <c r="B207" s="11"/>
-      <c r="C207" s="12"/>
+      <c r="B207" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>489</v>
+      </c>
       <c r="D207" s="35"/>
-      <c r="E207" s="32"/>
-      <c r="F207" s="23"/>
-      <c r="G207" s="24"/>
+      <c r="E207" s="29"/>
+      <c r="F207" s="19"/>
+      <c r="G207" s="20"/>
       <c r="H207" s="35"/>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="35"/>
-      <c r="B208" s="7" t="s">
-        <v>474</v>
-      </c>
-      <c r="C208" s="4" t="s">
-        <v>475</v>
-      </c>
+      <c r="B208" s="11"/>
+      <c r="C208" s="12"/>
       <c r="D208" s="35"/>
-      <c r="E208" s="29"/>
-      <c r="F208" s="19"/>
-      <c r="G208" s="20"/>
+      <c r="E208" s="32"/>
+      <c r="F208" s="23"/>
+      <c r="G208" s="24"/>
       <c r="H208" s="35"/>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="35"/>
       <c r="B209" s="7" t="s">
-        <v>480</v>
+        <v>424</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>481</v>
+        <v>425</v>
       </c>
       <c r="D209" s="35"/>
       <c r="E209" s="29"/>
@@ -5924,37 +5948,37 @@
       <c r="G209" s="20"/>
       <c r="H209" s="35"/>
     </row>
-    <row r="210" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="35"/>
-      <c r="B210" s="11"/>
-      <c r="C210" s="12"/>
+      <c r="B210" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>483</v>
+      </c>
       <c r="D210" s="35"/>
-      <c r="E210" s="32"/>
-      <c r="F210" s="23"/>
-      <c r="G210" s="24"/>
+      <c r="E210" s="29"/>
+      <c r="F210" s="19"/>
+      <c r="G210" s="20"/>
       <c r="H210" s="35"/>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="35"/>
-      <c r="B211" s="7" t="s">
-        <v>476</v>
-      </c>
-      <c r="C211" s="4" t="s">
-        <v>477</v>
-      </c>
+      <c r="B211" s="11"/>
+      <c r="C211" s="12"/>
       <c r="D211" s="35"/>
-      <c r="E211" s="29"/>
-      <c r="F211" s="19"/>
-      <c r="G211" s="20"/>
+      <c r="E211" s="32"/>
+      <c r="F211" s="23"/>
+      <c r="G211" s="24"/>
       <c r="H211" s="35"/>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="35"/>
       <c r="B212" s="7" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="D212" s="35"/>
       <c r="E212" s="29"/>
@@ -5964,164 +5988,164 @@
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="35"/>
-      <c r="B213" s="7"/>
-      <c r="C213" s="4"/>
+      <c r="B213" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="C213" s="4" t="s">
+        <v>481</v>
+      </c>
       <c r="D213" s="35"/>
       <c r="E213" s="29"/>
       <c r="F213" s="19"/>
       <c r="G213" s="20"/>
       <c r="H213" s="35"/>
     </row>
-    <row r="214" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="35"/>
-      <c r="B214" s="9"/>
-      <c r="C214" s="10"/>
+      <c r="B214" s="11"/>
+      <c r="C214" s="12"/>
       <c r="D214" s="35"/>
-      <c r="E214" s="30"/>
-      <c r="F214" s="21"/>
-      <c r="G214" s="22"/>
+      <c r="E214" s="32"/>
+      <c r="F214" s="23"/>
+      <c r="G214" s="24"/>
       <c r="H214" s="35"/>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="35"/>
       <c r="B215" s="7" t="s">
-        <v>309</v>
+        <v>476</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>310</v>
+        <v>477</v>
       </c>
       <c r="D215" s="35"/>
       <c r="E215" s="29"/>
-      <c r="F215" s="19">
-        <v>1</v>
-      </c>
-      <c r="G215" s="20">
-        <v>0</v>
-      </c>
+      <c r="F215" s="19"/>
+      <c r="G215" s="20"/>
       <c r="H215" s="35"/>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="35"/>
       <c r="B216" s="7" t="s">
-        <v>426</v>
+        <v>478</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>427</v>
+        <v>479</v>
       </c>
       <c r="D216" s="35"/>
       <c r="E216" s="29"/>
-      <c r="F216" s="19">
-        <v>1</v>
-      </c>
-      <c r="G216" s="20">
-        <v>0</v>
-      </c>
+      <c r="F216" s="19"/>
+      <c r="G216" s="20"/>
       <c r="H216" s="35"/>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="35"/>
-      <c r="B217" s="7" t="s">
-        <v>428</v>
-      </c>
-      <c r="C217" s="4" t="s">
-        <v>429</v>
-      </c>
+      <c r="B217" s="7"/>
+      <c r="C217" s="4"/>
       <c r="D217" s="35"/>
       <c r="E217" s="29"/>
-      <c r="F217" s="19">
-        <v>1</v>
-      </c>
-      <c r="G217" s="20">
-        <v>0</v>
-      </c>
+      <c r="F217" s="19"/>
+      <c r="G217" s="20"/>
       <c r="H217" s="35"/>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="35"/>
-      <c r="B218" s="7" t="s">
-        <v>410</v>
-      </c>
-      <c r="C218" s="4" t="s">
-        <v>411</v>
-      </c>
+      <c r="B218" s="9"/>
+      <c r="C218" s="10"/>
       <c r="D218" s="35"/>
-      <c r="E218" s="29"/>
-      <c r="F218" s="19">
-        <v>1</v>
-      </c>
-      <c r="G218" s="20">
-        <v>0</v>
-      </c>
+      <c r="E218" s="30"/>
+      <c r="F218" s="21"/>
+      <c r="G218" s="22"/>
       <c r="H218" s="35"/>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="35"/>
-      <c r="B219" s="48" t="s">
-        <v>462</v>
-      </c>
-      <c r="C219" s="49" t="s">
-        <v>463</v>
-      </c>
-      <c r="D219" s="50"/>
-      <c r="E219" s="51"/>
-      <c r="F219" s="52">
-        <v>1</v>
-      </c>
-      <c r="G219" s="53">
+      <c r="B219" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="C219" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="D219" s="35"/>
+      <c r="E219" s="29"/>
+      <c r="F219" s="19">
+        <v>1</v>
+      </c>
+      <c r="G219" s="20">
         <v>0</v>
       </c>
       <c r="H219" s="35"/>
     </row>
-    <row r="220" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="35"/>
-      <c r="B220" s="11"/>
-      <c r="C220" s="12"/>
+      <c r="B220" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>427</v>
+      </c>
       <c r="D220" s="35"/>
-      <c r="E220" s="32"/>
-      <c r="F220" s="23"/>
-      <c r="G220" s="24"/>
+      <c r="E220" s="29"/>
+      <c r="F220" s="19">
+        <v>1</v>
+      </c>
+      <c r="G220" s="20">
+        <v>0</v>
+      </c>
       <c r="H220" s="35"/>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="35"/>
       <c r="B221" s="7" t="s">
-        <v>458</v>
+        <v>428</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>459</v>
+        <v>429</v>
       </c>
       <c r="D221" s="35"/>
       <c r="E221" s="29"/>
-      <c r="F221" s="19"/>
-      <c r="G221" s="20"/>
+      <c r="F221" s="19">
+        <v>1</v>
+      </c>
+      <c r="G221" s="20">
+        <v>0</v>
+      </c>
       <c r="H221" s="35"/>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="35"/>
       <c r="B222" s="7" t="s">
-        <v>454</v>
+        <v>410</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>455</v>
+        <v>411</v>
       </c>
       <c r="D222" s="35"/>
       <c r="E222" s="29"/>
-      <c r="F222" s="19"/>
-      <c r="G222" s="20"/>
+      <c r="F222" s="19">
+        <v>1</v>
+      </c>
+      <c r="G222" s="20">
+        <v>0</v>
+      </c>
       <c r="H222" s="35"/>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="35"/>
-      <c r="B223" s="7" t="s">
-        <v>456</v>
-      </c>
-      <c r="C223" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="D223" s="35"/>
-      <c r="E223" s="29"/>
-      <c r="F223" s="19"/>
-      <c r="G223" s="20"/>
+      <c r="B223" s="48" t="s">
+        <v>462</v>
+      </c>
+      <c r="C223" s="49" t="s">
+        <v>463</v>
+      </c>
+      <c r="D223" s="50"/>
+      <c r="E223" s="51"/>
+      <c r="F223" s="52">
+        <v>1</v>
+      </c>
+      <c r="G223" s="53">
+        <v>0</v>
+      </c>
       <c r="H223" s="35"/>
     </row>
     <row r="224" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6137,28 +6161,24 @@
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="35"/>
       <c r="B225" s="7" t="s">
-        <v>102</v>
+        <v>458</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>103</v>
+        <v>459</v>
       </c>
       <c r="D225" s="35"/>
       <c r="E225" s="29"/>
-      <c r="F225" s="19">
-        <v>1</v>
-      </c>
-      <c r="G225" s="20">
-        <v>0</v>
-      </c>
+      <c r="F225" s="19"/>
+      <c r="G225" s="20"/>
       <c r="H225" s="35"/>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="35"/>
       <c r="B226" s="7" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="D226" s="35"/>
       <c r="E226" s="29"/>
@@ -6166,51 +6186,55 @@
       <c r="G226" s="20"/>
       <c r="H226" s="35"/>
     </row>
-    <row r="227" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="35"/>
-      <c r="B227" s="11"/>
-      <c r="C227" s="12"/>
+      <c r="B227" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="C227" s="4" t="s">
+        <v>457</v>
+      </c>
       <c r="D227" s="35"/>
-      <c r="E227" s="32"/>
-      <c r="F227" s="23"/>
-      <c r="G227" s="24"/>
+      <c r="E227" s="29"/>
+      <c r="F227" s="19"/>
+      <c r="G227" s="20"/>
       <c r="H227" s="35"/>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="35"/>
-      <c r="B228" s="7" t="s">
-        <v>464</v>
-      </c>
-      <c r="C228" s="4" t="s">
-        <v>465</v>
-      </c>
+      <c r="B228" s="11"/>
+      <c r="C228" s="12"/>
       <c r="D228" s="35"/>
-      <c r="E228" s="29"/>
-      <c r="F228" s="19"/>
-      <c r="G228" s="20"/>
+      <c r="E228" s="32"/>
+      <c r="F228" s="23"/>
+      <c r="G228" s="24"/>
       <c r="H228" s="35"/>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="35"/>
       <c r="B229" s="7" t="s">
-        <v>470</v>
+        <v>102</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>471</v>
+        <v>103</v>
       </c>
       <c r="D229" s="35"/>
       <c r="E229" s="29"/>
-      <c r="F229" s="19"/>
-      <c r="G229" s="20"/>
+      <c r="F229" s="19">
+        <v>1</v>
+      </c>
+      <c r="G229" s="20">
+        <v>0</v>
+      </c>
       <c r="H229" s="35"/>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="35"/>
       <c r="B230" s="7" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="D230" s="35"/>
       <c r="E230" s="29"/>
@@ -6218,93 +6242,89 @@
       <c r="G230" s="20"/>
       <c r="H230" s="35"/>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="35"/>
-      <c r="B231" s="7" t="s">
-        <v>468</v>
-      </c>
-      <c r="C231" s="4" t="s">
-        <v>469</v>
-      </c>
+      <c r="B231" s="11"/>
+      <c r="C231" s="12"/>
       <c r="D231" s="35"/>
-      <c r="E231" s="29"/>
-      <c r="F231" s="19"/>
-      <c r="G231" s="20"/>
+      <c r="E231" s="32"/>
+      <c r="F231" s="23"/>
+      <c r="G231" s="24"/>
       <c r="H231" s="35"/>
     </row>
-    <row r="232" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="35"/>
-      <c r="B232" s="11"/>
-      <c r="C232" s="12"/>
+      <c r="B232" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="C232" s="4" t="s">
+        <v>465</v>
+      </c>
       <c r="D232" s="35"/>
-      <c r="E232" s="32"/>
-      <c r="F232" s="23"/>
-      <c r="G232" s="24"/>
+      <c r="E232" s="29"/>
+      <c r="F232" s="19"/>
+      <c r="G232" s="20"/>
       <c r="H232" s="35"/>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="35"/>
       <c r="B233" s="7" t="s">
-        <v>412</v>
+        <v>470</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>413</v>
+        <v>471</v>
       </c>
       <c r="D233" s="35"/>
       <c r="E233" s="29"/>
-      <c r="F233" s="19">
-        <v>1</v>
-      </c>
-      <c r="G233" s="20">
-        <v>0</v>
-      </c>
+      <c r="F233" s="19"/>
+      <c r="G233" s="20"/>
       <c r="H233" s="35"/>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="35"/>
-      <c r="B234" s="7"/>
-      <c r="C234" s="4"/>
+      <c r="B234" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="C234" s="4" t="s">
+        <v>467</v>
+      </c>
       <c r="D234" s="35"/>
       <c r="E234" s="29"/>
       <c r="F234" s="19"/>
       <c r="G234" s="20"/>
       <c r="H234" s="35"/>
     </row>
-    <row r="235" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="35"/>
-      <c r="B235" s="9"/>
-      <c r="C235" s="10"/>
+      <c r="B235" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="C235" s="4" t="s">
+        <v>469</v>
+      </c>
       <c r="D235" s="35"/>
-      <c r="E235" s="30"/>
-      <c r="F235" s="21"/>
-      <c r="G235" s="22"/>
+      <c r="E235" s="29"/>
+      <c r="F235" s="19"/>
+      <c r="G235" s="20"/>
       <c r="H235" s="35"/>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="35"/>
-      <c r="B236" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C236" s="4" t="s">
-        <v>93</v>
-      </c>
+      <c r="B236" s="11"/>
+      <c r="C236" s="12"/>
       <c r="D236" s="35"/>
-      <c r="E236" s="29"/>
-      <c r="F236" s="19">
-        <v>1</v>
-      </c>
-      <c r="G236" s="20">
-        <v>0</v>
-      </c>
+      <c r="E236" s="32"/>
+      <c r="F236" s="23"/>
+      <c r="G236" s="24"/>
       <c r="H236" s="35"/>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="35"/>
       <c r="B237" s="7" t="s">
-        <v>164</v>
+        <v>412</v>
       </c>
       <c r="C237" s="4" t="s">
-        <v>145</v>
+        <v>413</v>
       </c>
       <c r="D237" s="35"/>
       <c r="E237" s="29"/>
@@ -6318,47 +6338,31 @@
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="35"/>
-      <c r="B238" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="C238" s="4" t="s">
-        <v>316</v>
-      </c>
+      <c r="B238" s="7"/>
+      <c r="C238" s="4"/>
       <c r="D238" s="35"/>
       <c r="E238" s="29"/>
-      <c r="F238" s="19">
-        <v>1</v>
-      </c>
-      <c r="G238" s="20">
-        <v>0</v>
-      </c>
+      <c r="F238" s="19"/>
+      <c r="G238" s="20"/>
       <c r="H238" s="35"/>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="35"/>
-      <c r="B239" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C239" s="4" t="s">
-        <v>146</v>
-      </c>
+      <c r="B239" s="9"/>
+      <c r="C239" s="10"/>
       <c r="D239" s="35"/>
-      <c r="E239" s="29"/>
-      <c r="F239" s="19">
-        <v>1</v>
-      </c>
-      <c r="G239" s="20">
-        <v>0</v>
-      </c>
+      <c r="E239" s="30"/>
+      <c r="F239" s="21"/>
+      <c r="G239" s="22"/>
       <c r="H239" s="35"/>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="35"/>
       <c r="B240" s="7" t="s">
-        <v>166</v>
+        <v>51</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>147</v>
+        <v>93</v>
       </c>
       <c r="D240" s="35"/>
       <c r="E240" s="29"/>
@@ -6373,10 +6377,10 @@
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="35"/>
       <c r="B241" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D241" s="35"/>
       <c r="E241" s="29"/>
@@ -6391,10 +6395,10 @@
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="35"/>
       <c r="B242" s="7" t="s">
-        <v>168</v>
+        <v>315</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>149</v>
+        <v>316</v>
       </c>
       <c r="D242" s="35"/>
       <c r="E242" s="29"/>
@@ -6409,10 +6413,10 @@
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="35"/>
       <c r="B243" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D243" s="35"/>
       <c r="E243" s="29"/>
@@ -6427,10 +6431,10 @@
     <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="35"/>
       <c r="B244" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D244" s="35"/>
       <c r="E244" s="29"/>
@@ -6445,10 +6449,10 @@
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="35"/>
       <c r="B245" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D245" s="35"/>
       <c r="E245" s="29"/>
@@ -6463,10 +6467,10 @@
     <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="35"/>
       <c r="B246" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D246" s="35"/>
       <c r="E246" s="29"/>
@@ -6481,10 +6485,10 @@
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="35"/>
       <c r="B247" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D247" s="35"/>
       <c r="E247" s="29"/>
@@ -6499,10 +6503,10 @@
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="35"/>
       <c r="B248" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C248" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D248" s="35"/>
       <c r="E248" s="29"/>
@@ -6517,10 +6521,10 @@
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="35"/>
       <c r="B249" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D249" s="35"/>
       <c r="E249" s="29"/>
@@ -6535,10 +6539,10 @@
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="35"/>
       <c r="B250" s="7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D250" s="35"/>
       <c r="E250" s="29"/>
@@ -6553,10 +6557,10 @@
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="35"/>
       <c r="B251" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D251" s="35"/>
       <c r="E251" s="29"/>
@@ -6571,10 +6575,10 @@
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="35"/>
       <c r="B252" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D252" s="35"/>
       <c r="E252" s="29"/>
@@ -6589,10 +6593,10 @@
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="35"/>
       <c r="B253" s="7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D253" s="35"/>
       <c r="E253" s="29"/>
@@ -6607,10 +6611,10 @@
     <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="35"/>
       <c r="B254" s="7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D254" s="35"/>
       <c r="E254" s="29"/>
@@ -6625,10 +6629,10 @@
     <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="35"/>
       <c r="B255" s="7" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D255" s="35"/>
       <c r="E255" s="29"/>
@@ -6643,10 +6647,10 @@
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="35"/>
       <c r="B256" s="7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D256" s="35"/>
       <c r="E256" s="29"/>
@@ -6661,10 +6665,10 @@
     <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="35"/>
       <c r="B257" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D257" s="35"/>
       <c r="E257" s="29"/>
@@ -6679,10 +6683,10 @@
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="35"/>
       <c r="B258" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D258" s="35"/>
       <c r="E258" s="29"/>
@@ -6697,10 +6701,10 @@
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="35"/>
       <c r="B259" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C259" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D259" s="35"/>
       <c r="E259" s="29"/>
@@ -6715,7 +6719,7 @@
     <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="35"/>
       <c r="B260" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C260" s="4" t="s">
         <v>163</v>
@@ -6733,7 +6737,7 @@
     <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="35"/>
       <c r="B261" s="7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C261" s="4" t="s">
         <v>163</v>
@@ -6751,7 +6755,7 @@
     <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" s="35"/>
       <c r="B262" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C262" s="4" t="s">
         <v>163</v>
@@ -6769,7 +6773,7 @@
     <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="35"/>
       <c r="B263" s="7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C263" s="4" t="s">
         <v>163</v>
@@ -6787,7 +6791,7 @@
     <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" s="35"/>
       <c r="B264" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C264" s="4" t="s">
         <v>163</v>
@@ -6805,7 +6809,7 @@
     <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" s="35"/>
       <c r="B265" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C265" s="4" t="s">
         <v>163</v>
@@ -6823,7 +6827,7 @@
     <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" s="35"/>
       <c r="B266" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C266" s="4" t="s">
         <v>163</v>
@@ -6841,7 +6845,7 @@
     <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" s="35"/>
       <c r="B267" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C267" s="4" t="s">
         <v>163</v>
@@ -6859,7 +6863,7 @@
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" s="35"/>
       <c r="B268" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C268" s="4" t="s">
         <v>163</v>
@@ -6877,7 +6881,7 @@
     <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" s="35"/>
       <c r="B269" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C269" s="4" t="s">
         <v>163</v>
@@ -6895,7 +6899,7 @@
     <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270" s="35"/>
       <c r="B270" s="7" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C270" s="4" t="s">
         <v>163</v>
@@ -6913,7 +6917,7 @@
     <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" s="35"/>
       <c r="B271" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C271" s="4" t="s">
         <v>163</v>
@@ -6931,7 +6935,7 @@
     <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" s="35"/>
       <c r="B272" s="7" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="C272" s="4" t="s">
         <v>163</v>
@@ -6948,31 +6952,47 @@
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="35"/>
-      <c r="B273" s="7"/>
-      <c r="C273" s="4"/>
+      <c r="B273" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C273" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="D273" s="35"/>
       <c r="E273" s="29"/>
-      <c r="F273" s="19"/>
-      <c r="G273" s="20"/>
+      <c r="F273" s="19">
+        <v>1</v>
+      </c>
+      <c r="G273" s="20">
+        <v>0</v>
+      </c>
       <c r="H273" s="35"/>
     </row>
-    <row r="274" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="35"/>
-      <c r="B274" s="9"/>
-      <c r="C274" s="10"/>
+      <c r="B274" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C274" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="D274" s="35"/>
-      <c r="E274" s="30"/>
-      <c r="F274" s="21"/>
-      <c r="G274" s="22"/>
+      <c r="E274" s="29"/>
+      <c r="F274" s="19">
+        <v>1</v>
+      </c>
+      <c r="G274" s="20">
+        <v>0</v>
+      </c>
       <c r="H274" s="35"/>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="35"/>
       <c r="B275" s="7" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="C275" s="4" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="D275" s="35"/>
       <c r="E275" s="29"/>
@@ -6987,10 +7007,10 @@
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="35"/>
       <c r="B276" s="7" t="s">
-        <v>325</v>
+        <v>217</v>
       </c>
       <c r="C276" s="4" t="s">
-        <v>327</v>
+        <v>163</v>
       </c>
       <c r="D276" s="35"/>
       <c r="E276" s="29"/>
@@ -7004,233 +7024,217 @@
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="35"/>
-      <c r="B277" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="C277" s="4" t="s">
-        <v>328</v>
-      </c>
+      <c r="B277" s="7"/>
+      <c r="C277" s="4"/>
       <c r="D277" s="35"/>
       <c r="E277" s="29"/>
-      <c r="F277" s="19">
-        <v>1</v>
-      </c>
-      <c r="G277" s="20">
-        <v>0</v>
-      </c>
+      <c r="F277" s="19"/>
+      <c r="G277" s="20"/>
       <c r="H277" s="35"/>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="35"/>
-      <c r="B278" s="7" t="s">
+      <c r="B278" s="9"/>
+      <c r="C278" s="10"/>
+      <c r="D278" s="35"/>
+      <c r="E278" s="30"/>
+      <c r="F278" s="21"/>
+      <c r="G278" s="22"/>
+      <c r="H278" s="35"/>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A279" s="35"/>
+      <c r="B279" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C279" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D279" s="35"/>
+      <c r="E279" s="29"/>
+      <c r="F279" s="19">
+        <v>1</v>
+      </c>
+      <c r="G279" s="20">
+        <v>0</v>
+      </c>
+      <c r="H279" s="35"/>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A280" s="35"/>
+      <c r="B280" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="C280" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D280" s="35"/>
+      <c r="E280" s="29"/>
+      <c r="F280" s="19">
+        <v>1</v>
+      </c>
+      <c r="G280" s="20">
+        <v>0</v>
+      </c>
+      <c r="H280" s="35"/>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A281" s="35"/>
+      <c r="B281" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C281" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="D281" s="35"/>
+      <c r="E281" s="29"/>
+      <c r="F281" s="19">
+        <v>1</v>
+      </c>
+      <c r="G281" s="20">
+        <v>0</v>
+      </c>
+      <c r="H281" s="35"/>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A282" s="35"/>
+      <c r="B282" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="C278" s="4" t="s">
+      <c r="C282" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="D278" s="35"/>
-      <c r="E278" s="29"/>
-      <c r="F278" s="19">
-        <v>1</v>
-      </c>
-      <c r="G278" s="20">
-        <v>0</v>
-      </c>
-      <c r="H278" s="35"/>
-    </row>
-    <row r="279" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A279" s="37"/>
-      <c r="B279" s="13" t="s">
-        <v>369</v>
-      </c>
-      <c r="C279" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="D279" s="37"/>
-      <c r="E279" s="31"/>
-      <c r="F279" s="19">
-        <v>1</v>
-      </c>
-      <c r="G279" s="20">
-        <v>0</v>
-      </c>
-      <c r="H279" s="37"/>
-    </row>
-    <row r="280" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A280" s="37"/>
-      <c r="B280" s="13" t="s">
-        <v>370</v>
-      </c>
-      <c r="C280" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="D280" s="37"/>
-      <c r="E280" s="31"/>
-      <c r="F280" s="19">
-        <v>1</v>
-      </c>
-      <c r="G280" s="20">
-        <v>0</v>
-      </c>
-      <c r="H280" s="37"/>
-    </row>
-    <row r="281" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A281" s="37"/>
-      <c r="B281" s="13" t="s">
-        <v>371</v>
-      </c>
-      <c r="C281" s="14" t="s">
-        <v>375</v>
-      </c>
-      <c r="D281" s="37"/>
-      <c r="E281" s="31"/>
-      <c r="F281" s="19">
-        <v>1</v>
-      </c>
-      <c r="G281" s="20">
-        <v>0</v>
-      </c>
-      <c r="H281" s="37"/>
-    </row>
-    <row r="282" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A282" s="37"/>
-      <c r="B282" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="C282" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="D282" s="37"/>
-      <c r="E282" s="31"/>
+      <c r="D282" s="35"/>
+      <c r="E282" s="29"/>
       <c r="F282" s="19">
         <v>1</v>
       </c>
       <c r="G282" s="20">
         <v>0</v>
       </c>
-      <c r="H282" s="37"/>
+      <c r="H282" s="35"/>
     </row>
     <row r="283" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A283" s="37"/>
-      <c r="B283" s="7" t="s">
-        <v>436</v>
-      </c>
-      <c r="C283" s="4" t="s">
-        <v>437</v>
+      <c r="B283" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="C283" s="14" t="s">
+        <v>373</v>
       </c>
       <c r="D283" s="37"/>
       <c r="E283" s="31"/>
-      <c r="F283" s="19"/>
-      <c r="G283" s="20"/>
+      <c r="F283" s="19">
+        <v>1</v>
+      </c>
+      <c r="G283" s="20">
+        <v>0</v>
+      </c>
       <c r="H283" s="37"/>
     </row>
     <row r="284" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A284" s="37"/>
-      <c r="B284" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="C284" s="4" t="s">
-        <v>441</v>
+      <c r="B284" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="C284" s="14" t="s">
+        <v>374</v>
       </c>
       <c r="D284" s="37"/>
       <c r="E284" s="31"/>
-      <c r="F284" s="19"/>
-      <c r="G284" s="20"/>
+      <c r="F284" s="19">
+        <v>1</v>
+      </c>
+      <c r="G284" s="20">
+        <v>0</v>
+      </c>
       <c r="H284" s="37"/>
     </row>
     <row r="285" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A285" s="37"/>
-      <c r="B285" s="7" t="s">
-        <v>439</v>
-      </c>
-      <c r="C285" s="4" t="s">
-        <v>440</v>
+      <c r="B285" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="C285" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="D285" s="37"/>
       <c r="E285" s="31"/>
-      <c r="F285" s="19"/>
-      <c r="G285" s="20"/>
+      <c r="F285" s="19">
+        <v>1</v>
+      </c>
+      <c r="G285" s="20">
+        <v>0</v>
+      </c>
       <c r="H285" s="37"/>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A286" s="35"/>
-      <c r="B286" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="C286" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D286" s="35"/>
-      <c r="E286" s="29"/>
+    <row r="286" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A286" s="37"/>
+      <c r="B286" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="C286" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="D286" s="37"/>
+      <c r="E286" s="31"/>
       <c r="F286" s="19">
         <v>1</v>
       </c>
       <c r="G286" s="20">
         <v>0</v>
       </c>
-      <c r="H286" s="35"/>
-    </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A287" s="35"/>
+      <c r="H286" s="37"/>
+    </row>
+    <row r="287" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A287" s="37"/>
       <c r="B287" s="7" t="s">
-        <v>354</v>
+        <v>436</v>
       </c>
       <c r="C287" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D287" s="35"/>
-      <c r="E287" s="29"/>
-      <c r="F287" s="19">
-        <v>1</v>
-      </c>
-      <c r="G287" s="20">
-        <v>0</v>
-      </c>
-      <c r="H287" s="35"/>
-    </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A288" s="35"/>
+        <v>437</v>
+      </c>
+      <c r="D287" s="37"/>
+      <c r="E287" s="31"/>
+      <c r="F287" s="19"/>
+      <c r="G287" s="20"/>
+      <c r="H287" s="37"/>
+    </row>
+    <row r="288" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A288" s="37"/>
       <c r="B288" s="7" t="s">
-        <v>355</v>
+        <v>438</v>
       </c>
       <c r="C288" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="D288" s="35"/>
-      <c r="E288" s="29"/>
-      <c r="F288" s="19">
-        <v>1</v>
-      </c>
-      <c r="G288" s="20">
-        <v>0</v>
-      </c>
-      <c r="H288" s="35"/>
-    </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A289" s="35"/>
+        <v>441</v>
+      </c>
+      <c r="D288" s="37"/>
+      <c r="E288" s="31"/>
+      <c r="F288" s="19"/>
+      <c r="G288" s="20"/>
+      <c r="H288" s="37"/>
+    </row>
+    <row r="289" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="37"/>
       <c r="B289" s="7" t="s">
-        <v>349</v>
+        <v>439</v>
       </c>
       <c r="C289" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="D289" s="35"/>
-      <c r="E289" s="29"/>
-      <c r="F289" s="19">
-        <v>1</v>
-      </c>
-      <c r="G289" s="20">
-        <v>0</v>
-      </c>
-      <c r="H289" s="35"/>
+        <v>440</v>
+      </c>
+      <c r="D289" s="37"/>
+      <c r="E289" s="31"/>
+      <c r="F289" s="19"/>
+      <c r="G289" s="20"/>
+      <c r="H289" s="37"/>
     </row>
     <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290" s="35"/>
       <c r="B290" s="7" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="C290" s="4" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="D290" s="35"/>
       <c r="E290" s="29"/>
@@ -7245,10 +7249,10 @@
     <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291" s="35"/>
       <c r="B291" s="7" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="C291" s="4" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="D291" s="35"/>
       <c r="E291" s="29"/>
@@ -7263,10 +7267,10 @@
     <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292" s="35"/>
       <c r="B292" s="7" t="s">
-        <v>337</v>
+        <v>355</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>338</v>
+        <v>358</v>
       </c>
       <c r="D292" s="35"/>
       <c r="E292" s="29"/>
@@ -7281,10 +7285,10 @@
     <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293" s="35"/>
       <c r="B293" s="7" t="s">
-        <v>335</v>
+        <v>349</v>
       </c>
       <c r="C293" s="4" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="D293" s="35"/>
       <c r="E293" s="29"/>
@@ -7299,10 +7303,10 @@
     <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294" s="35"/>
       <c r="B294" s="7" t="s">
-        <v>329</v>
+        <v>348</v>
       </c>
       <c r="C294" s="4" t="s">
-        <v>330</v>
+        <v>351</v>
       </c>
       <c r="D294" s="35"/>
       <c r="E294" s="29"/>
@@ -7314,77 +7318,173 @@
       </c>
       <c r="H294" s="35"/>
     </row>
-    <row r="295" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295" s="35"/>
-      <c r="B295" s="11"/>
-      <c r="C295" s="12"/>
+      <c r="B295" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C295" s="4" t="s">
+        <v>352</v>
+      </c>
       <c r="D295" s="35"/>
-      <c r="E295" s="32"/>
-      <c r="F295" s="23"/>
-      <c r="G295" s="24"/>
+      <c r="E295" s="29"/>
+      <c r="F295" s="19">
+        <v>1</v>
+      </c>
+      <c r="G295" s="20">
+        <v>0</v>
+      </c>
       <c r="H295" s="35"/>
     </row>
     <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296" s="35"/>
       <c r="B296" s="7" t="s">
-        <v>442</v>
+        <v>337</v>
       </c>
       <c r="C296" s="4" t="s">
-        <v>443</v>
+        <v>338</v>
       </c>
       <c r="D296" s="35"/>
       <c r="E296" s="29"/>
-      <c r="F296" s="19"/>
-      <c r="G296" s="20"/>
+      <c r="F296" s="19">
+        <v>1</v>
+      </c>
+      <c r="G296" s="20">
+        <v>0</v>
+      </c>
       <c r="H296" s="35"/>
     </row>
     <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297" s="35"/>
       <c r="B297" s="7" t="s">
-        <v>452</v>
+        <v>335</v>
       </c>
       <c r="C297" s="4" t="s">
-        <v>453</v>
+        <v>336</v>
       </c>
       <c r="D297" s="35"/>
       <c r="E297" s="29"/>
-      <c r="F297" s="19"/>
-      <c r="G297" s="20"/>
+      <c r="F297" s="19">
+        <v>1</v>
+      </c>
+      <c r="G297" s="20">
+        <v>0</v>
+      </c>
       <c r="H297" s="35"/>
     </row>
     <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298" s="35"/>
       <c r="B298" s="7" t="s">
-        <v>444</v>
+        <v>329</v>
       </c>
       <c r="C298" s="4" t="s">
-        <v>445</v>
+        <v>330</v>
       </c>
       <c r="D298" s="35"/>
       <c r="E298" s="29"/>
-      <c r="F298" s="19"/>
-      <c r="G298" s="20"/>
+      <c r="F298" s="19">
+        <v>1</v>
+      </c>
+      <c r="G298" s="20">
+        <v>0</v>
+      </c>
       <c r="H298" s="35"/>
     </row>
-    <row r="299" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="35"/>
-      <c r="B299" s="8"/>
-      <c r="C299" s="6"/>
+      <c r="B299" s="11"/>
+      <c r="C299" s="12"/>
       <c r="D299" s="35"/>
-      <c r="E299" s="33"/>
-      <c r="F299" s="25"/>
-      <c r="G299" s="26"/>
+      <c r="E299" s="32"/>
+      <c r="F299" s="23"/>
+      <c r="G299" s="24"/>
       <c r="H299" s="35"/>
     </row>
-    <row r="300" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300" s="35"/>
-      <c r="B300" s="38"/>
-      <c r="C300" s="39"/>
+      <c r="B300" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="C300" s="4" t="s">
+        <v>499</v>
+      </c>
       <c r="D300" s="35"/>
-      <c r="E300" s="40"/>
-      <c r="F300" s="41"/>
-      <c r="G300" s="41"/>
+      <c r="E300" s="29"/>
+      <c r="F300" s="19"/>
+      <c r="G300" s="20"/>
       <c r="H300" s="35"/>
+    </row>
+    <row r="301" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="35"/>
+      <c r="B301" s="11"/>
+      <c r="C301" s="12"/>
+      <c r="D301" s="35"/>
+      <c r="E301" s="32"/>
+      <c r="F301" s="23"/>
+      <c r="G301" s="24"/>
+      <c r="H301" s="35"/>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A302" s="35"/>
+      <c r="B302" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="C302" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="D302" s="35"/>
+      <c r="E302" s="29"/>
+      <c r="F302" s="19"/>
+      <c r="G302" s="20"/>
+      <c r="H302" s="35"/>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A303" s="35"/>
+      <c r="B303" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="C303" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="D303" s="35"/>
+      <c r="E303" s="29"/>
+      <c r="F303" s="19"/>
+      <c r="G303" s="20"/>
+      <c r="H303" s="35"/>
+    </row>
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A304" s="35"/>
+      <c r="B304" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="C304" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D304" s="35"/>
+      <c r="E304" s="29"/>
+      <c r="F304" s="19"/>
+      <c r="G304" s="20"/>
+      <c r="H304" s="35"/>
+    </row>
+    <row r="305" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A305" s="35"/>
+      <c r="B305" s="8"/>
+      <c r="C305" s="6"/>
+      <c r="D305" s="35"/>
+      <c r="E305" s="33"/>
+      <c r="F305" s="25"/>
+      <c r="G305" s="26"/>
+      <c r="H305" s="35"/>
+    </row>
+    <row r="306" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A306" s="35"/>
+      <c r="B306" s="38"/>
+      <c r="C306" s="39"/>
+      <c r="D306" s="35"/>
+      <c r="E306" s="40"/>
+      <c r="F306" s="41"/>
+      <c r="G306" s="41"/>
+      <c r="H306" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Penambahan API untuk schBudgeting.tblBudgetExpenseLine
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="512">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -1628,6 +1628,36 @@
   </si>
   <si>
     <t>Mendapatkan Daftar Kelompok Anggaran Belanja</t>
+  </si>
+  <si>
+    <t>transaction.undelete.project.setBudgetExpenseGroup</t>
+  </si>
+  <si>
+    <t>Membatalkan Penghapusan Data Kelompok Anggaran Belanja</t>
+  </si>
+  <si>
+    <t>transaction.delete.budgeting.setBudgetExpenseGroup</t>
+  </si>
+  <si>
+    <t>Menghapus Data Kelompok Anggaran Belanja</t>
+  </si>
+  <si>
+    <t>transaction.create.budgeting.setBudgetExpense</t>
+  </si>
+  <si>
+    <t>Menyimpan Data Baru Anggaran Belanja</t>
+  </si>
+  <si>
+    <t>transaction.delete.budgeting.setBudgetExpense</t>
+  </si>
+  <si>
+    <t>Menghapus Data Anggaran Belanja</t>
+  </si>
+  <si>
+    <t>transaction.undelete.project.setBudgetExpense</t>
+  </si>
+  <si>
+    <t>Membatalkan Penghapusan Data Anggaran Belanja</t>
   </si>
 </sst>
 </file>
@@ -2456,13 +2486,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H306"/>
+  <dimension ref="A1:H312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B193" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B278" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C203" sqref="C203"/>
+      <selection pane="bottomRight" activeCell="C282" sqref="C282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3365,10 +3395,10 @@
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="35"/>
       <c r="B58" s="7" t="s">
-        <v>496</v>
+        <v>506</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
       <c r="D58" s="35"/>
       <c r="E58" s="29"/>
@@ -3376,37 +3406,37 @@
       <c r="G58" s="20"/>
       <c r="H58" s="35"/>
     </row>
-    <row r="59" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="35"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="12"/>
+      <c r="B59" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>497</v>
+      </c>
       <c r="D59" s="35"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="24"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="20"/>
       <c r="H59" s="35"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="35"/>
-      <c r="B60" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>448</v>
-      </c>
+      <c r="B60" s="11"/>
+      <c r="C60" s="12"/>
       <c r="D60" s="35"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="20"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="24"/>
       <c r="H60" s="35"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="35"/>
       <c r="B61" s="7" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D61" s="35"/>
       <c r="E61" s="29"/>
@@ -3417,10 +3447,10 @@
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="35"/>
       <c r="B62" s="7" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D62" s="35"/>
       <c r="E62" s="29"/>
@@ -3430,49 +3460,45 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="35"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="4"/>
+      <c r="B63" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>449</v>
+      </c>
       <c r="D63" s="35"/>
       <c r="E63" s="29"/>
       <c r="F63" s="19"/>
       <c r="G63" s="20"/>
       <c r="H63" s="35"/>
     </row>
-    <row r="64" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="35"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="10"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="4"/>
       <c r="D64" s="35"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="22"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="20"/>
       <c r="H64" s="35"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="35"/>
-      <c r="B65" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>302</v>
-      </c>
+      <c r="B65" s="9"/>
+      <c r="C65" s="10"/>
       <c r="D65" s="35"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="19">
-        <v>1</v>
-      </c>
-      <c r="G65" s="20">
-        <v>0</v>
-      </c>
+      <c r="E65" s="30"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="22"/>
       <c r="H65" s="35"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="35"/>
       <c r="B66" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D66" s="35"/>
       <c r="E66" s="29"/>
@@ -3487,10 +3513,10 @@
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="35"/>
       <c r="B67" s="7" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D67" s="35"/>
       <c r="E67" s="29"/>
@@ -3505,10 +3531,10 @@
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="35"/>
       <c r="B68" s="7" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="D68" s="35"/>
       <c r="E68" s="29"/>
@@ -3523,10 +3549,10 @@
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="35"/>
       <c r="B69" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D69" s="35"/>
       <c r="E69" s="29"/>
@@ -3538,41 +3564,41 @@
       </c>
       <c r="H69" s="35"/>
     </row>
-    <row r="70" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="35"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="12"/>
+      <c r="B70" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>307</v>
+      </c>
       <c r="D70" s="35"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="23"/>
-      <c r="G70" s="24"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="19">
+        <v>1</v>
+      </c>
+      <c r="G70" s="20">
+        <v>0</v>
+      </c>
       <c r="H70" s="35"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="35"/>
-      <c r="B71" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="B71" s="11"/>
+      <c r="C71" s="12"/>
       <c r="D71" s="35"/>
-      <c r="E71" s="29"/>
-      <c r="F71" s="19">
-        <v>1</v>
-      </c>
-      <c r="G71" s="20">
-        <v>0</v>
-      </c>
+      <c r="E71" s="32"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="24"/>
       <c r="H71" s="35"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="35"/>
       <c r="B72" s="7" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D72" s="35"/>
       <c r="E72" s="29"/>
@@ -3587,10 +3613,10 @@
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="35"/>
       <c r="B73" s="7" t="s">
-        <v>311</v>
+        <v>94</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>312</v>
+        <v>95</v>
       </c>
       <c r="D73" s="35"/>
       <c r="E73" s="29"/>
@@ -3605,10 +3631,10 @@
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="35"/>
       <c r="B74" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D74" s="35"/>
       <c r="E74" s="29"/>
@@ -3623,10 +3649,10 @@
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="35"/>
       <c r="B75" s="7" t="s">
-        <v>96</v>
+        <v>313</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>99</v>
+        <v>314</v>
       </c>
       <c r="D75" s="35"/>
       <c r="E75" s="29"/>
@@ -3641,10 +3667,10 @@
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="35"/>
       <c r="B76" s="7" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D76" s="35"/>
       <c r="E76" s="29"/>
@@ -3659,10 +3685,10 @@
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="35"/>
       <c r="B77" s="7" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D77" s="35"/>
       <c r="E77" s="29"/>
@@ -3677,10 +3703,10 @@
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="35"/>
       <c r="B78" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D78" s="35"/>
       <c r="E78" s="29"/>
@@ -3695,10 +3721,10 @@
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="35"/>
       <c r="B79" s="7" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="D79" s="35"/>
       <c r="E79" s="29"/>
@@ -3713,10 +3739,10 @@
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="35"/>
       <c r="B80" s="7" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="D80" s="35"/>
       <c r="E80" s="29"/>
@@ -3731,10 +3757,10 @@
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="35"/>
       <c r="B81" s="7" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="D81" s="35"/>
       <c r="E81" s="29"/>
@@ -3749,10 +3775,10 @@
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="35"/>
       <c r="B82" s="7" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>381</v>
+        <v>101</v>
       </c>
       <c r="D82" s="35"/>
       <c r="E82" s="29"/>
@@ -3767,10 +3793,10 @@
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="35"/>
       <c r="B83" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D83" s="35"/>
       <c r="E83" s="29"/>
@@ -3785,10 +3811,10 @@
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="35"/>
       <c r="B84" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D84" s="35"/>
       <c r="E84" s="29"/>
@@ -3803,10 +3829,10 @@
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="35"/>
       <c r="B85" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D85" s="35"/>
       <c r="E85" s="29"/>
@@ -3821,10 +3847,10 @@
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="35"/>
       <c r="B86" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>114</v>
+        <v>384</v>
       </c>
       <c r="D86" s="35"/>
       <c r="E86" s="29"/>
@@ -3839,10 +3865,10 @@
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="35"/>
       <c r="B87" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D87" s="35"/>
       <c r="E87" s="29"/>
@@ -3857,10 +3883,10 @@
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="35"/>
       <c r="B88" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D88" s="35"/>
       <c r="E88" s="29"/>
@@ -3875,10 +3901,10 @@
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="35"/>
       <c r="B89" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D89" s="35"/>
       <c r="E89" s="29"/>
@@ -3893,10 +3919,10 @@
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="35"/>
       <c r="B90" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D90" s="35"/>
       <c r="E90" s="29"/>
@@ -3911,10 +3937,10 @@
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="35"/>
       <c r="B91" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D91" s="35"/>
       <c r="E91" s="29"/>
@@ -3929,10 +3955,10 @@
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="35"/>
       <c r="B92" s="7" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>198</v>
+        <v>122</v>
       </c>
       <c r="D92" s="35"/>
       <c r="E92" s="29"/>
@@ -3947,10 +3973,10 @@
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="35"/>
       <c r="B93" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D93" s="35"/>
       <c r="E93" s="29"/>
@@ -3965,10 +3991,10 @@
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="35"/>
       <c r="B94" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D94" s="35"/>
       <c r="E94" s="29"/>
@@ -3983,10 +4009,10 @@
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="35"/>
       <c r="B95" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D95" s="35"/>
       <c r="E95" s="29"/>
@@ -4001,10 +4027,10 @@
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="35"/>
       <c r="B96" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D96" s="35"/>
       <c r="E96" s="29"/>
@@ -4019,10 +4045,10 @@
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="35"/>
       <c r="B97" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D97" s="35"/>
       <c r="E97" s="29"/>
@@ -4037,10 +4063,10 @@
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="35"/>
       <c r="B98" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D98" s="35"/>
       <c r="E98" s="29"/>
@@ -4055,10 +4081,10 @@
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="35"/>
       <c r="B99" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D99" s="35"/>
       <c r="E99" s="29"/>
@@ -4073,10 +4099,10 @@
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="35"/>
       <c r="B100" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D100" s="35"/>
       <c r="E100" s="29"/>
@@ -4091,10 +4117,10 @@
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="35"/>
       <c r="B101" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D101" s="35"/>
       <c r="E101" s="29"/>
@@ -4109,10 +4135,10 @@
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="35"/>
       <c r="B102" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D102" s="35"/>
       <c r="E102" s="29"/>
@@ -4127,10 +4153,10 @@
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="35"/>
       <c r="B103" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D103" s="35"/>
       <c r="E103" s="29"/>
@@ -4145,10 +4171,10 @@
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
       <c r="B104" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D104" s="35"/>
       <c r="E104" s="29"/>
@@ -4163,10 +4189,10 @@
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="35"/>
       <c r="B105" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D105" s="35"/>
       <c r="E105" s="29"/>
@@ -4181,10 +4207,10 @@
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="35"/>
       <c r="B106" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D106" s="35"/>
       <c r="E106" s="29"/>
@@ -4196,61 +4222,61 @@
       </c>
       <c r="H106" s="35"/>
     </row>
-    <row r="107" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="35"/>
-      <c r="B107" s="11"/>
-      <c r="C107" s="12"/>
+      <c r="B107" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>213</v>
+      </c>
       <c r="D107" s="35"/>
-      <c r="E107" s="32"/>
-      <c r="F107" s="23"/>
-      <c r="G107" s="24"/>
+      <c r="E107" s="29"/>
+      <c r="F107" s="19">
+        <v>1</v>
+      </c>
+      <c r="G107" s="20">
+        <v>0</v>
+      </c>
       <c r="H107" s="35"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="35"/>
-      <c r="B108" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>242</v>
-      </c>
+      <c r="B108" s="11"/>
+      <c r="C108" s="12"/>
       <c r="D108" s="35"/>
-      <c r="E108" s="29">
-        <v>44188</v>
-      </c>
-      <c r="F108" s="19">
-        <v>1</v>
-      </c>
-      <c r="G108" s="20">
-        <v>1</v>
-      </c>
+      <c r="E108" s="32"/>
+      <c r="F108" s="23"/>
+      <c r="G108" s="24"/>
       <c r="H108" s="35"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="35"/>
       <c r="B109" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D109" s="35"/>
-      <c r="E109" s="29"/>
+      <c r="E109" s="29">
+        <v>44188</v>
+      </c>
       <c r="F109" s="19">
         <v>1</v>
       </c>
       <c r="G109" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H109" s="35"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="35"/>
       <c r="B110" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D110" s="35"/>
       <c r="E110" s="29"/>
@@ -4265,10 +4291,10 @@
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="35"/>
       <c r="B111" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D111" s="35"/>
       <c r="E111" s="29"/>
@@ -4283,10 +4309,10 @@
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="35"/>
       <c r="B112" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D112" s="35"/>
       <c r="E112" s="29"/>
@@ -4298,95 +4324,83 @@
       </c>
       <c r="H112" s="35"/>
     </row>
-    <row r="113" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="35"/>
-      <c r="B113" s="11"/>
-      <c r="C113" s="12"/>
+      <c r="B113" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>243</v>
+      </c>
       <c r="D113" s="35"/>
-      <c r="E113" s="32"/>
-      <c r="F113" s="23"/>
-      <c r="G113" s="24"/>
+      <c r="E113" s="29"/>
+      <c r="F113" s="19">
+        <v>1</v>
+      </c>
+      <c r="G113" s="20">
+        <v>0</v>
+      </c>
       <c r="H113" s="35"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="35"/>
-      <c r="B114" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>223</v>
-      </c>
+      <c r="B114" s="11"/>
+      <c r="C114" s="12"/>
       <c r="D114" s="35"/>
-      <c r="E114" s="29"/>
-      <c r="F114" s="19">
-        <v>1</v>
-      </c>
-      <c r="G114" s="20">
-        <v>0</v>
-      </c>
+      <c r="E114" s="32"/>
+      <c r="F114" s="23"/>
+      <c r="G114" s="24"/>
       <c r="H114" s="35"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="35"/>
       <c r="B115" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D115" s="35"/>
       <c r="E115" s="29"/>
-      <c r="F115" s="19">
-        <v>1</v>
-      </c>
-      <c r="G115" s="20">
-        <v>0</v>
-      </c>
+      <c r="F115" s="19"/>
+      <c r="G115" s="20"/>
       <c r="H115" s="35"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="35"/>
       <c r="B116" s="7" t="s">
-        <v>220</v>
+        <v>508</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>225</v>
+        <v>509</v>
       </c>
       <c r="D116" s="35"/>
       <c r="E116" s="29"/>
-      <c r="F116" s="19">
-        <v>1</v>
-      </c>
-      <c r="G116" s="20">
-        <v>0</v>
-      </c>
+      <c r="F116" s="19"/>
+      <c r="G116" s="20"/>
       <c r="H116" s="35"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="35"/>
       <c r="B117" s="7" t="s">
-        <v>221</v>
+        <v>504</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>226</v>
+        <v>505</v>
       </c>
       <c r="D117" s="35"/>
       <c r="E117" s="29"/>
-      <c r="F117" s="19">
-        <v>1</v>
-      </c>
-      <c r="G117" s="20">
-        <v>0</v>
-      </c>
+      <c r="F117" s="19"/>
+      <c r="G117" s="20"/>
       <c r="H117" s="35"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="35"/>
       <c r="B118" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D118" s="35"/>
       <c r="E118" s="29"/>
@@ -4398,23 +4412,31 @@
       </c>
       <c r="H118" s="35"/>
     </row>
-    <row r="119" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="35"/>
-      <c r="B119" s="11"/>
-      <c r="C119" s="12"/>
+      <c r="B119" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>225</v>
+      </c>
       <c r="D119" s="35"/>
-      <c r="E119" s="32"/>
-      <c r="F119" s="23"/>
-      <c r="G119" s="24"/>
+      <c r="E119" s="29"/>
+      <c r="F119" s="19">
+        <v>1</v>
+      </c>
+      <c r="G119" s="20">
+        <v>0</v>
+      </c>
       <c r="H119" s="35"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="35"/>
-      <c r="B120" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C120" s="4" t="s">
-        <v>229</v>
+      <c r="B120" s="48" t="s">
+        <v>221</v>
+      </c>
+      <c r="C120" s="49" t="s">
+        <v>226</v>
       </c>
       <c r="D120" s="35"/>
       <c r="E120" s="29"/>
@@ -4426,41 +4448,41 @@
       </c>
       <c r="H120" s="35"/>
     </row>
-    <row r="121" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="35"/>
-      <c r="B121" s="11"/>
-      <c r="C121" s="12"/>
+      <c r="B121" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>227</v>
+      </c>
       <c r="D121" s="35"/>
-      <c r="E121" s="32"/>
-      <c r="F121" s="23"/>
-      <c r="G121" s="24"/>
+      <c r="E121" s="29"/>
+      <c r="F121" s="19">
+        <v>1</v>
+      </c>
+      <c r="G121" s="20">
+        <v>0</v>
+      </c>
       <c r="H121" s="35"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="35"/>
-      <c r="B122" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>232</v>
-      </c>
+      <c r="B122" s="11"/>
+      <c r="C122" s="12"/>
       <c r="D122" s="35"/>
-      <c r="E122" s="29"/>
-      <c r="F122" s="19">
-        <v>1</v>
-      </c>
-      <c r="G122" s="20">
-        <v>0</v>
-      </c>
+      <c r="E122" s="32"/>
+      <c r="F122" s="23"/>
+      <c r="G122" s="24"/>
       <c r="H122" s="35"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="35"/>
       <c r="B123" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D123" s="35"/>
       <c r="E123" s="29"/>
@@ -4485,10 +4507,10 @@
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="35"/>
       <c r="B125" s="7" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="D125" s="35"/>
       <c r="E125" s="29"/>
@@ -4500,41 +4522,41 @@
       </c>
       <c r="H125" s="35"/>
     </row>
-    <row r="126" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="35"/>
-      <c r="B126" s="11"/>
-      <c r="C126" s="12"/>
+      <c r="B126" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="D126" s="35"/>
-      <c r="E126" s="32"/>
-      <c r="F126" s="23"/>
-      <c r="G126" s="24"/>
+      <c r="E126" s="29"/>
+      <c r="F126" s="19">
+        <v>1</v>
+      </c>
+      <c r="G126" s="20">
+        <v>0</v>
+      </c>
       <c r="H126" s="35"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="35"/>
-      <c r="B127" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="C127" s="4" t="s">
-        <v>247</v>
-      </c>
+      <c r="B127" s="11"/>
+      <c r="C127" s="12"/>
       <c r="D127" s="35"/>
-      <c r="E127" s="29"/>
-      <c r="F127" s="19">
-        <v>1</v>
-      </c>
-      <c r="G127" s="20">
-        <v>0</v>
-      </c>
+      <c r="E127" s="32"/>
+      <c r="F127" s="23"/>
+      <c r="G127" s="24"/>
       <c r="H127" s="35"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="35"/>
       <c r="B128" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="D128" s="35"/>
       <c r="E128" s="29"/>
@@ -4546,31 +4568,23 @@
       </c>
       <c r="H128" s="35"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="35"/>
-      <c r="B129" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="C129" s="4" t="s">
-        <v>284</v>
-      </c>
+      <c r="B129" s="11"/>
+      <c r="C129" s="12"/>
       <c r="D129" s="35"/>
-      <c r="E129" s="29"/>
-      <c r="F129" s="19">
-        <v>1</v>
-      </c>
-      <c r="G129" s="20">
-        <v>0</v>
-      </c>
+      <c r="E129" s="32"/>
+      <c r="F129" s="23"/>
+      <c r="G129" s="24"/>
       <c r="H129" s="35"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="35"/>
       <c r="B130" s="7" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="D130" s="35"/>
       <c r="E130" s="29"/>
@@ -4585,10 +4599,10 @@
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="35"/>
       <c r="B131" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D131" s="35"/>
       <c r="E131" s="29"/>
@@ -4603,10 +4617,10 @@
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="35"/>
       <c r="B132" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="D132" s="35"/>
       <c r="E132" s="29"/>
@@ -4621,10 +4635,10 @@
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="35"/>
       <c r="B133" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="D133" s="35"/>
       <c r="E133" s="29"/>
@@ -4639,10 +4653,10 @@
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="35"/>
       <c r="B134" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D134" s="35"/>
       <c r="E134" s="29"/>
@@ -4657,10 +4671,10 @@
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="35"/>
       <c r="B135" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
       <c r="D135" s="35"/>
       <c r="E135" s="29"/>
@@ -4675,10 +4689,10 @@
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="35"/>
       <c r="B136" s="7" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D136" s="35"/>
       <c r="E136" s="29"/>
@@ -4693,10 +4707,10 @@
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="35"/>
       <c r="B137" s="7" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>265</v>
+        <v>286</v>
       </c>
       <c r="D137" s="35"/>
       <c r="E137" s="29"/>
@@ -4711,10 +4725,10 @@
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="35"/>
       <c r="B138" s="7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="D138" s="35"/>
       <c r="E138" s="29"/>
@@ -4729,10 +4743,10 @@
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="35"/>
       <c r="B139" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="D139" s="35"/>
       <c r="E139" s="29"/>
@@ -4747,10 +4761,10 @@
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="35"/>
       <c r="B140" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D140" s="35"/>
       <c r="E140" s="29"/>
@@ -4765,10 +4779,10 @@
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="35"/>
       <c r="B141" s="7" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="D141" s="35"/>
       <c r="E141" s="29"/>
@@ -4783,10 +4797,10 @@
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="35"/>
       <c r="B142" s="7" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D142" s="35"/>
       <c r="E142" s="29"/>
@@ -4801,10 +4815,10 @@
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="35"/>
       <c r="B143" s="7" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D143" s="35"/>
       <c r="E143" s="29"/>
@@ -4819,10 +4833,10 @@
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="35"/>
       <c r="B144" s="7" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="D144" s="35"/>
       <c r="E144" s="29"/>
@@ -4837,10 +4851,10 @@
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="35"/>
       <c r="B145" s="7" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D145" s="35"/>
       <c r="E145" s="29"/>
@@ -4855,10 +4869,10 @@
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="35"/>
       <c r="B146" s="7" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="D146" s="35"/>
       <c r="E146" s="29"/>
@@ -4873,10 +4887,10 @@
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="35"/>
       <c r="B147" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D147" s="35"/>
       <c r="E147" s="29"/>
@@ -4888,23 +4902,31 @@
       </c>
       <c r="H147" s="35"/>
     </row>
-    <row r="148" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="35"/>
-      <c r="B148" s="11"/>
-      <c r="C148" s="12"/>
+      <c r="B148" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>281</v>
+      </c>
       <c r="D148" s="35"/>
-      <c r="E148" s="32"/>
-      <c r="F148" s="23"/>
-      <c r="G148" s="24"/>
+      <c r="E148" s="29"/>
+      <c r="F148" s="19">
+        <v>1</v>
+      </c>
+      <c r="G148" s="20">
+        <v>0</v>
+      </c>
       <c r="H148" s="35"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="35"/>
       <c r="B149" s="7" t="s">
-        <v>144</v>
+        <v>276</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>214</v>
+        <v>280</v>
       </c>
       <c r="D149" s="35"/>
       <c r="E149" s="29"/>
@@ -4919,10 +4941,10 @@
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="35"/>
       <c r="B150" s="7" t="s">
-        <v>215</v>
+        <v>277</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>216</v>
+        <v>279</v>
       </c>
       <c r="D150" s="35"/>
       <c r="E150" s="29"/>
@@ -4947,10 +4969,10 @@
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="35"/>
       <c r="B152" s="7" t="s">
-        <v>288</v>
+        <v>144</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>296</v>
+        <v>214</v>
       </c>
       <c r="D152" s="35"/>
       <c r="E152" s="29"/>
@@ -4965,10 +4987,10 @@
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="35"/>
       <c r="B153" s="7" t="s">
-        <v>289</v>
+        <v>215</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>290</v>
+        <v>216</v>
       </c>
       <c r="D153" s="35"/>
       <c r="E153" s="29"/>
@@ -4980,31 +5002,23 @@
       </c>
       <c r="H153" s="35"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="35"/>
-      <c r="B154" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C154" s="4" t="s">
-        <v>297</v>
-      </c>
+      <c r="B154" s="11"/>
+      <c r="C154" s="12"/>
       <c r="D154" s="35"/>
-      <c r="E154" s="29"/>
-      <c r="F154" s="19">
-        <v>1</v>
-      </c>
-      <c r="G154" s="20">
-        <v>0</v>
-      </c>
+      <c r="E154" s="32"/>
+      <c r="F154" s="23"/>
+      <c r="G154" s="24"/>
       <c r="H154" s="35"/>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="35"/>
       <c r="B155" s="7" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D155" s="35"/>
       <c r="E155" s="29"/>
@@ -5019,10 +5033,10 @@
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="35"/>
       <c r="B156" s="7" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D156" s="35"/>
       <c r="E156" s="29"/>
@@ -5036,95 +5050,89 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="35"/>
-      <c r="B157" s="7"/>
-      <c r="C157" s="4"/>
+      <c r="B157" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>297</v>
+      </c>
       <c r="D157" s="35"/>
       <c r="E157" s="29"/>
-      <c r="F157" s="19"/>
-      <c r="G157" s="20"/>
+      <c r="F157" s="19">
+        <v>1</v>
+      </c>
+      <c r="G157" s="20">
+        <v>0</v>
+      </c>
       <c r="H157" s="35"/>
     </row>
-    <row r="158" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="35"/>
-      <c r="B158" s="9"/>
-      <c r="C158" s="10"/>
+      <c r="B158" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>293</v>
+      </c>
       <c r="D158" s="35"/>
-      <c r="E158" s="30"/>
-      <c r="F158" s="21"/>
-      <c r="G158" s="22"/>
+      <c r="E158" s="29"/>
+      <c r="F158" s="19">
+        <v>1</v>
+      </c>
+      <c r="G158" s="20">
+        <v>0</v>
+      </c>
       <c r="H158" s="35"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="35"/>
       <c r="B159" s="7" t="s">
-        <v>52</v>
+        <v>294</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>53</v>
+        <v>295</v>
       </c>
       <c r="D159" s="35"/>
-      <c r="E159" s="29">
-        <v>44207</v>
-      </c>
+      <c r="E159" s="29"/>
       <c r="F159" s="19">
         <v>1</v>
       </c>
       <c r="G159" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H159" s="35"/>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="35"/>
-      <c r="B160" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C160" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="B160" s="7"/>
+      <c r="C160" s="4"/>
       <c r="D160" s="35"/>
-      <c r="E160" s="29">
-        <v>44211</v>
-      </c>
-      <c r="F160" s="19">
-        <v>1</v>
-      </c>
-      <c r="G160" s="20">
-        <v>1</v>
-      </c>
+      <c r="E160" s="29"/>
+      <c r="F160" s="19"/>
+      <c r="G160" s="20"/>
       <c r="H160" s="35"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="35"/>
-      <c r="B161" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C161" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="B161" s="9"/>
+      <c r="C161" s="10"/>
       <c r="D161" s="35"/>
-      <c r="E161" s="29">
-        <v>44211</v>
-      </c>
-      <c r="F161" s="19">
-        <v>1</v>
-      </c>
-      <c r="G161" s="20">
-        <v>1</v>
-      </c>
+      <c r="E161" s="30"/>
+      <c r="F161" s="21"/>
+      <c r="G161" s="22"/>
       <c r="H161" s="35"/>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="35"/>
       <c r="B162" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D162" s="35"/>
       <c r="E162" s="29">
-        <v>44211</v>
+        <v>44207</v>
       </c>
       <c r="F162" s="19">
         <v>1</v>
@@ -5137,10 +5145,10 @@
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="35"/>
       <c r="B163" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D163" s="35"/>
       <c r="E163" s="29">
@@ -5157,10 +5165,10 @@
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="35"/>
       <c r="B164" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D164" s="35"/>
       <c r="E164" s="29">
@@ -5177,10 +5185,10 @@
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="35"/>
       <c r="B165" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D165" s="35"/>
       <c r="E165" s="29">
@@ -5197,10 +5205,10 @@
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="35"/>
       <c r="B166" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D166" s="35"/>
       <c r="E166" s="29">
@@ -5217,10 +5225,10 @@
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="35"/>
       <c r="B167" s="7" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D167" s="35"/>
       <c r="E167" s="29">
@@ -5237,10 +5245,10 @@
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="35"/>
       <c r="B168" s="7" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D168" s="35"/>
       <c r="E168" s="29">
@@ -5257,10 +5265,10 @@
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="35"/>
       <c r="B169" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D169" s="35"/>
       <c r="E169" s="29">
@@ -5277,10 +5285,10 @@
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="35"/>
       <c r="B170" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D170" s="35"/>
       <c r="E170" s="29">
@@ -5297,10 +5305,10 @@
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="35"/>
       <c r="B171" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D171" s="35"/>
       <c r="E171" s="29">
@@ -5317,10 +5325,10 @@
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="35"/>
       <c r="B172" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D172" s="35"/>
       <c r="E172" s="29">
@@ -5337,10 +5345,10 @@
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="35"/>
       <c r="B173" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D173" s="35"/>
       <c r="E173" s="29">
@@ -5357,10 +5365,10 @@
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="35"/>
       <c r="B174" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>207</v>
+        <v>84</v>
       </c>
       <c r="D174" s="35"/>
       <c r="E174" s="29">
@@ -5377,10 +5385,10 @@
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="35"/>
       <c r="B175" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D175" s="35"/>
       <c r="E175" s="29">
@@ -5397,10 +5405,10 @@
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="35"/>
       <c r="B176" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D176" s="35"/>
       <c r="E176" s="29">
@@ -5417,10 +5425,10 @@
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="35"/>
       <c r="B177" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>90</v>
+        <v>207</v>
       </c>
       <c r="D177" s="35"/>
       <c r="E177" s="29">
@@ -5437,10 +5445,10 @@
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="35"/>
       <c r="B178" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D178" s="35"/>
       <c r="E178" s="29">
@@ -5456,99 +5464,105 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="35"/>
-      <c r="B179" s="7"/>
-      <c r="C179" s="4"/>
+      <c r="B179" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C179" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="D179" s="35"/>
-      <c r="E179" s="29"/>
-      <c r="F179" s="19"/>
-      <c r="G179" s="20"/>
+      <c r="E179" s="29">
+        <v>44211</v>
+      </c>
+      <c r="F179" s="19">
+        <v>1</v>
+      </c>
+      <c r="G179" s="20">
+        <v>1</v>
+      </c>
       <c r="H179" s="35"/>
     </row>
-    <row r="180" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="35"/>
-      <c r="B180" s="9"/>
-      <c r="C180" s="10"/>
+      <c r="B180" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="D180" s="35"/>
-      <c r="E180" s="30"/>
-      <c r="F180" s="21"/>
-      <c r="G180" s="22"/>
+      <c r="E180" s="29">
+        <v>44211</v>
+      </c>
+      <c r="F180" s="19">
+        <v>1</v>
+      </c>
+      <c r="G180" s="20">
+        <v>1</v>
+      </c>
       <c r="H180" s="35"/>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="35"/>
       <c r="B181" s="7" t="s">
-        <v>422</v>
+        <v>79</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>423</v>
+        <v>91</v>
       </c>
       <c r="D181" s="35"/>
-      <c r="E181" s="29"/>
-      <c r="F181" s="19"/>
-      <c r="G181" s="20"/>
+      <c r="E181" s="29">
+        <v>44211</v>
+      </c>
+      <c r="F181" s="19">
+        <v>1</v>
+      </c>
+      <c r="G181" s="20">
+        <v>1</v>
+      </c>
       <c r="H181" s="35"/>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="35"/>
-      <c r="B182" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C182" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="B182" s="7"/>
+      <c r="C182" s="4"/>
       <c r="D182" s="35"/>
       <c r="E182" s="29"/>
-      <c r="F182" s="19">
-        <v>1</v>
-      </c>
-      <c r="G182" s="20">
-        <v>0</v>
-      </c>
+      <c r="F182" s="19"/>
+      <c r="G182" s="20"/>
       <c r="H182" s="35"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="35"/>
-      <c r="B183" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C183" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="B183" s="9"/>
+      <c r="C183" s="10"/>
       <c r="D183" s="35"/>
-      <c r="E183" s="29"/>
-      <c r="F183" s="19">
-        <v>1</v>
-      </c>
-      <c r="G183" s="20">
-        <v>0</v>
-      </c>
+      <c r="E183" s="30"/>
+      <c r="F183" s="21"/>
+      <c r="G183" s="22"/>
       <c r="H183" s="35"/>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="35"/>
       <c r="B184" s="7" t="s">
-        <v>16</v>
+        <v>422</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>18</v>
+        <v>423</v>
       </c>
       <c r="D184" s="35"/>
       <c r="E184" s="29"/>
-      <c r="F184" s="19">
-        <v>1</v>
-      </c>
-      <c r="G184" s="20">
-        <v>0</v>
-      </c>
+      <c r="F184" s="19"/>
+      <c r="G184" s="20"/>
       <c r="H184" s="35"/>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="35"/>
       <c r="B185" s="7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D185" s="35"/>
       <c r="E185" s="29"/>
@@ -5563,10 +5577,10 @@
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="35"/>
       <c r="B186" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D186" s="35"/>
       <c r="E186" s="29"/>
@@ -5581,10 +5595,10 @@
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="35"/>
       <c r="B187" s="7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D187" s="35"/>
       <c r="E187" s="29"/>
@@ -5599,10 +5613,10 @@
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="35"/>
       <c r="B188" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D188" s="35"/>
       <c r="E188" s="29"/>
@@ -5617,10 +5631,10 @@
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="35"/>
       <c r="B189" s="7" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D189" s="35"/>
       <c r="E189" s="29"/>
@@ -5635,10 +5649,10 @@
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="35"/>
       <c r="B190" s="7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D190" s="35"/>
       <c r="E190" s="29"/>
@@ -5653,10 +5667,10 @@
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="35"/>
       <c r="B191" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D191" s="35"/>
       <c r="E191" s="29"/>
@@ -5671,10 +5685,10 @@
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="35"/>
       <c r="B192" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D192" s="35"/>
       <c r="E192" s="29"/>
@@ -5689,10 +5703,10 @@
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="35"/>
       <c r="B193" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="D193" s="35"/>
       <c r="E193" s="29"/>
@@ -5707,10 +5721,10 @@
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="35"/>
       <c r="B194" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D194" s="35"/>
       <c r="E194" s="29"/>
@@ -5725,10 +5739,10 @@
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="35"/>
       <c r="B195" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D195" s="35"/>
       <c r="E195" s="29"/>
@@ -5743,10 +5757,10 @@
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="35"/>
       <c r="B196" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D196" s="35"/>
       <c r="E196" s="29"/>
@@ -5761,10 +5775,10 @@
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="35"/>
       <c r="B197" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C197" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D197" s="35"/>
       <c r="E197" s="29"/>
@@ -5779,10 +5793,10 @@
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="35"/>
       <c r="B198" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D198" s="35"/>
       <c r="E198" s="29"/>
@@ -5797,10 +5811,10 @@
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="35"/>
       <c r="B199" s="7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D199" s="35"/>
       <c r="E199" s="29"/>
@@ -5815,10 +5829,10 @@
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="35"/>
       <c r="B200" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C200" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+      <c r="C200" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D200" s="35"/>
       <c r="E200" s="29"/>
@@ -5830,65 +5844,77 @@
       </c>
       <c r="H200" s="35"/>
     </row>
-    <row r="201" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="35"/>
-      <c r="B201" s="11"/>
-      <c r="C201" s="12"/>
+      <c r="B201" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="D201" s="35"/>
-      <c r="E201" s="32"/>
-      <c r="F201" s="23"/>
-      <c r="G201" s="24"/>
+      <c r="E201" s="29"/>
+      <c r="F201" s="19">
+        <v>1</v>
+      </c>
+      <c r="G201" s="20">
+        <v>0</v>
+      </c>
       <c r="H201" s="35"/>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="35"/>
       <c r="B202" s="7" t="s">
-        <v>484</v>
+        <v>47</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>487</v>
+        <v>36</v>
       </c>
       <c r="D202" s="35"/>
       <c r="E202" s="29"/>
-      <c r="F202" s="19"/>
-      <c r="G202" s="20"/>
+      <c r="F202" s="19">
+        <v>1</v>
+      </c>
+      <c r="G202" s="20">
+        <v>0</v>
+      </c>
       <c r="H202" s="35"/>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="35"/>
       <c r="B203" s="7" t="s">
-        <v>500</v>
+        <v>48</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>501</v>
+        <v>49</v>
       </c>
       <c r="D203" s="35"/>
       <c r="E203" s="29"/>
-      <c r="F203" s="19"/>
-      <c r="G203" s="20"/>
+      <c r="F203" s="19">
+        <v>1</v>
+      </c>
+      <c r="G203" s="20">
+        <v>0</v>
+      </c>
       <c r="H203" s="35"/>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="35"/>
-      <c r="B204" s="7" t="s">
-        <v>490</v>
-      </c>
-      <c r="C204" s="4" t="s">
-        <v>491</v>
-      </c>
+      <c r="B204" s="11"/>
+      <c r="C204" s="12"/>
       <c r="D204" s="35"/>
-      <c r="E204" s="29"/>
-      <c r="F204" s="19"/>
-      <c r="G204" s="20"/>
+      <c r="E204" s="32"/>
+      <c r="F204" s="23"/>
+      <c r="G204" s="24"/>
       <c r="H204" s="35"/>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="35"/>
       <c r="B205" s="7" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="D205" s="35"/>
       <c r="E205" s="29"/>
@@ -5899,10 +5925,10 @@
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="35"/>
       <c r="B206" s="7" t="s">
-        <v>485</v>
+        <v>500</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>488</v>
+        <v>501</v>
       </c>
       <c r="D206" s="35"/>
       <c r="E206" s="29"/>
@@ -5913,10 +5939,10 @@
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="35"/>
       <c r="B207" s="7" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D207" s="35"/>
       <c r="E207" s="29"/>
@@ -5924,23 +5950,27 @@
       <c r="G207" s="20"/>
       <c r="H207" s="35"/>
     </row>
-    <row r="208" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="35"/>
-      <c r="B208" s="11"/>
-      <c r="C208" s="12"/>
+      <c r="B208" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="C208" s="4" t="s">
+        <v>493</v>
+      </c>
       <c r="D208" s="35"/>
-      <c r="E208" s="32"/>
-      <c r="F208" s="23"/>
-      <c r="G208" s="24"/>
+      <c r="E208" s="29"/>
+      <c r="F208" s="19"/>
+      <c r="G208" s="20"/>
       <c r="H208" s="35"/>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="35"/>
       <c r="B209" s="7" t="s">
-        <v>424</v>
+        <v>485</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>425</v>
+        <v>488</v>
       </c>
       <c r="D209" s="35"/>
       <c r="E209" s="29"/>
@@ -5951,10 +5981,10 @@
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="35"/>
       <c r="B210" s="7" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="D210" s="35"/>
       <c r="E210" s="29"/>
@@ -5975,10 +6005,10 @@
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="35"/>
       <c r="B212" s="7" t="s">
-        <v>474</v>
+        <v>424</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>475</v>
+        <v>425</v>
       </c>
       <c r="D212" s="35"/>
       <c r="E212" s="29"/>
@@ -5989,10 +6019,10 @@
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="35"/>
       <c r="B213" s="7" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="D213" s="35"/>
       <c r="E213" s="29"/>
@@ -6013,10 +6043,10 @@
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="35"/>
       <c r="B215" s="7" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D215" s="35"/>
       <c r="E215" s="29"/>
@@ -6027,10 +6057,10 @@
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="35"/>
       <c r="B216" s="7" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D216" s="35"/>
       <c r="E216" s="29"/>
@@ -6038,87 +6068,71 @@
       <c r="G216" s="20"/>
       <c r="H216" s="35"/>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="35"/>
-      <c r="B217" s="7"/>
-      <c r="C217" s="4"/>
+      <c r="B217" s="11"/>
+      <c r="C217" s="12"/>
       <c r="D217" s="35"/>
-      <c r="E217" s="29"/>
-      <c r="F217" s="19"/>
-      <c r="G217" s="20"/>
+      <c r="E217" s="32"/>
+      <c r="F217" s="23"/>
+      <c r="G217" s="24"/>
       <c r="H217" s="35"/>
     </row>
-    <row r="218" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="35"/>
-      <c r="B218" s="9"/>
-      <c r="C218" s="10"/>
+      <c r="B218" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="C218" s="4" t="s">
+        <v>477</v>
+      </c>
       <c r="D218" s="35"/>
-      <c r="E218" s="30"/>
-      <c r="F218" s="21"/>
-      <c r="G218" s="22"/>
+      <c r="E218" s="29"/>
+      <c r="F218" s="19"/>
+      <c r="G218" s="20"/>
       <c r="H218" s="35"/>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="35"/>
       <c r="B219" s="7" t="s">
-        <v>309</v>
+        <v>478</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>310</v>
+        <v>479</v>
       </c>
       <c r="D219" s="35"/>
       <c r="E219" s="29"/>
-      <c r="F219" s="19">
-        <v>1</v>
-      </c>
-      <c r="G219" s="20">
-        <v>0</v>
-      </c>
+      <c r="F219" s="19"/>
+      <c r="G219" s="20"/>
       <c r="H219" s="35"/>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="35"/>
-      <c r="B220" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="C220" s="4" t="s">
-        <v>427</v>
-      </c>
+      <c r="B220" s="7"/>
+      <c r="C220" s="4"/>
       <c r="D220" s="35"/>
       <c r="E220" s="29"/>
-      <c r="F220" s="19">
-        <v>1</v>
-      </c>
-      <c r="G220" s="20">
-        <v>0</v>
-      </c>
+      <c r="F220" s="19"/>
+      <c r="G220" s="20"/>
       <c r="H220" s="35"/>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="35"/>
-      <c r="B221" s="7" t="s">
-        <v>428</v>
-      </c>
-      <c r="C221" s="4" t="s">
-        <v>429</v>
-      </c>
+      <c r="B221" s="9"/>
+      <c r="C221" s="10"/>
       <c r="D221" s="35"/>
-      <c r="E221" s="29"/>
-      <c r="F221" s="19">
-        <v>1</v>
-      </c>
-      <c r="G221" s="20">
-        <v>0</v>
-      </c>
+      <c r="E221" s="30"/>
+      <c r="F221" s="21"/>
+      <c r="G221" s="22"/>
       <c r="H221" s="35"/>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="35"/>
       <c r="B222" s="7" t="s">
-        <v>410</v>
+        <v>309</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>411</v>
+        <v>310</v>
       </c>
       <c r="D222" s="35"/>
       <c r="E222" s="29"/>
@@ -6132,109 +6146,121 @@
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="35"/>
-      <c r="B223" s="48" t="s">
-        <v>462</v>
-      </c>
-      <c r="C223" s="49" t="s">
-        <v>463</v>
-      </c>
-      <c r="D223" s="50"/>
-      <c r="E223" s="51"/>
-      <c r="F223" s="52">
-        <v>1</v>
-      </c>
-      <c r="G223" s="53">
+      <c r="B223" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="C223" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="D223" s="35"/>
+      <c r="E223" s="29"/>
+      <c r="F223" s="19">
+        <v>1</v>
+      </c>
+      <c r="G223" s="20">
         <v>0</v>
       </c>
       <c r="H223" s="35"/>
     </row>
-    <row r="224" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="35"/>
-      <c r="B224" s="11"/>
-      <c r="C224" s="12"/>
+      <c r="B224" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="C224" s="4" t="s">
+        <v>429</v>
+      </c>
       <c r="D224" s="35"/>
-      <c r="E224" s="32"/>
-      <c r="F224" s="23"/>
-      <c r="G224" s="24"/>
+      <c r="E224" s="29"/>
+      <c r="F224" s="19">
+        <v>1</v>
+      </c>
+      <c r="G224" s="20">
+        <v>0</v>
+      </c>
       <c r="H224" s="35"/>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="35"/>
       <c r="B225" s="7" t="s">
-        <v>458</v>
+        <v>410</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>459</v>
+        <v>411</v>
       </c>
       <c r="D225" s="35"/>
       <c r="E225" s="29"/>
-      <c r="F225" s="19"/>
-      <c r="G225" s="20"/>
+      <c r="F225" s="19">
+        <v>1</v>
+      </c>
+      <c r="G225" s="20">
+        <v>0</v>
+      </c>
       <c r="H225" s="35"/>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="35"/>
-      <c r="B226" s="7" t="s">
-        <v>454</v>
-      </c>
-      <c r="C226" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="D226" s="35"/>
-      <c r="E226" s="29"/>
-      <c r="F226" s="19"/>
-      <c r="G226" s="20"/>
+      <c r="B226" s="48" t="s">
+        <v>462</v>
+      </c>
+      <c r="C226" s="49" t="s">
+        <v>463</v>
+      </c>
+      <c r="D226" s="50"/>
+      <c r="E226" s="51"/>
+      <c r="F226" s="52">
+        <v>1</v>
+      </c>
+      <c r="G226" s="53">
+        <v>0</v>
+      </c>
       <c r="H226" s="35"/>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="35"/>
-      <c r="B227" s="7" t="s">
-        <v>456</v>
-      </c>
-      <c r="C227" s="4" t="s">
-        <v>457</v>
-      </c>
+      <c r="B227" s="11"/>
+      <c r="C227" s="12"/>
       <c r="D227" s="35"/>
-      <c r="E227" s="29"/>
-      <c r="F227" s="19"/>
-      <c r="G227" s="20"/>
+      <c r="E227" s="32"/>
+      <c r="F227" s="23"/>
+      <c r="G227" s="24"/>
       <c r="H227" s="35"/>
     </row>
-    <row r="228" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="35"/>
-      <c r="B228" s="11"/>
-      <c r="C228" s="12"/>
+      <c r="B228" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="C228" s="4" t="s">
+        <v>459</v>
+      </c>
       <c r="D228" s="35"/>
-      <c r="E228" s="32"/>
-      <c r="F228" s="23"/>
-      <c r="G228" s="24"/>
+      <c r="E228" s="29"/>
+      <c r="F228" s="19"/>
+      <c r="G228" s="20"/>
       <c r="H228" s="35"/>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="35"/>
       <c r="B229" s="7" t="s">
-        <v>102</v>
+        <v>454</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>103</v>
+        <v>455</v>
       </c>
       <c r="D229" s="35"/>
       <c r="E229" s="29"/>
-      <c r="F229" s="19">
-        <v>1</v>
-      </c>
-      <c r="G229" s="20">
-        <v>0</v>
-      </c>
+      <c r="F229" s="19"/>
+      <c r="G229" s="20"/>
       <c r="H229" s="35"/>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="35"/>
       <c r="B230" s="7" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D230" s="35"/>
       <c r="E230" s="29"/>
@@ -6255,24 +6281,28 @@
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="35"/>
       <c r="B232" s="7" t="s">
-        <v>464</v>
+        <v>102</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>465</v>
+        <v>103</v>
       </c>
       <c r="D232" s="35"/>
       <c r="E232" s="29"/>
-      <c r="F232" s="19"/>
-      <c r="G232" s="20"/>
+      <c r="F232" s="19">
+        <v>1</v>
+      </c>
+      <c r="G232" s="20">
+        <v>0</v>
+      </c>
       <c r="H232" s="35"/>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="35"/>
       <c r="B233" s="7" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="D233" s="35"/>
       <c r="E233" s="29"/>
@@ -6280,27 +6310,23 @@
       <c r="G233" s="20"/>
       <c r="H233" s="35"/>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="35"/>
-      <c r="B234" s="7" t="s">
-        <v>466</v>
-      </c>
-      <c r="C234" s="4" t="s">
-        <v>467</v>
-      </c>
+      <c r="B234" s="11"/>
+      <c r="C234" s="12"/>
       <c r="D234" s="35"/>
-      <c r="E234" s="29"/>
-      <c r="F234" s="19"/>
-      <c r="G234" s="20"/>
+      <c r="E234" s="32"/>
+      <c r="F234" s="23"/>
+      <c r="G234" s="24"/>
       <c r="H234" s="35"/>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="35"/>
       <c r="B235" s="7" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D235" s="35"/>
       <c r="E235" s="29"/>
@@ -6308,61 +6334,65 @@
       <c r="G235" s="20"/>
       <c r="H235" s="35"/>
     </row>
-    <row r="236" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="35"/>
-      <c r="B236" s="11"/>
-      <c r="C236" s="12"/>
+      <c r="B236" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="C236" s="4" t="s">
+        <v>471</v>
+      </c>
       <c r="D236" s="35"/>
-      <c r="E236" s="32"/>
-      <c r="F236" s="23"/>
-      <c r="G236" s="24"/>
+      <c r="E236" s="29"/>
+      <c r="F236" s="19"/>
+      <c r="G236" s="20"/>
       <c r="H236" s="35"/>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="35"/>
       <c r="B237" s="7" t="s">
-        <v>412</v>
+        <v>466</v>
       </c>
       <c r="C237" s="4" t="s">
-        <v>413</v>
+        <v>467</v>
       </c>
       <c r="D237" s="35"/>
       <c r="E237" s="29"/>
-      <c r="F237" s="19">
-        <v>1</v>
-      </c>
-      <c r="G237" s="20">
-        <v>0</v>
-      </c>
+      <c r="F237" s="19"/>
+      <c r="G237" s="20"/>
       <c r="H237" s="35"/>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="35"/>
-      <c r="B238" s="7"/>
-      <c r="C238" s="4"/>
+      <c r="B238" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="C238" s="4" t="s">
+        <v>469</v>
+      </c>
       <c r="D238" s="35"/>
       <c r="E238" s="29"/>
       <c r="F238" s="19"/>
       <c r="G238" s="20"/>
       <c r="H238" s="35"/>
     </row>
-    <row r="239" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="35"/>
-      <c r="B239" s="9"/>
-      <c r="C239" s="10"/>
+      <c r="B239" s="11"/>
+      <c r="C239" s="12"/>
       <c r="D239" s="35"/>
-      <c r="E239" s="30"/>
-      <c r="F239" s="21"/>
-      <c r="G239" s="22"/>
+      <c r="E239" s="32"/>
+      <c r="F239" s="23"/>
+      <c r="G239" s="24"/>
       <c r="H239" s="35"/>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="35"/>
       <c r="B240" s="7" t="s">
-        <v>51</v>
+        <v>412</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>93</v>
+        <v>413</v>
       </c>
       <c r="D240" s="35"/>
       <c r="E240" s="29"/>
@@ -6376,47 +6406,31 @@
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="35"/>
-      <c r="B241" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C241" s="4" t="s">
-        <v>145</v>
-      </c>
+      <c r="B241" s="7"/>
+      <c r="C241" s="4"/>
       <c r="D241" s="35"/>
       <c r="E241" s="29"/>
-      <c r="F241" s="19">
-        <v>1</v>
-      </c>
-      <c r="G241" s="20">
-        <v>0</v>
-      </c>
+      <c r="F241" s="19"/>
+      <c r="G241" s="20"/>
       <c r="H241" s="35"/>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="35"/>
-      <c r="B242" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="C242" s="4" t="s">
-        <v>316</v>
-      </c>
+      <c r="B242" s="9"/>
+      <c r="C242" s="10"/>
       <c r="D242" s="35"/>
-      <c r="E242" s="29"/>
-      <c r="F242" s="19">
-        <v>1</v>
-      </c>
-      <c r="G242" s="20">
-        <v>0</v>
-      </c>
+      <c r="E242" s="30"/>
+      <c r="F242" s="21"/>
+      <c r="G242" s="22"/>
       <c r="H242" s="35"/>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="35"/>
       <c r="B243" s="7" t="s">
-        <v>165</v>
+        <v>51</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>146</v>
+        <v>93</v>
       </c>
       <c r="D243" s="35"/>
       <c r="E243" s="29"/>
@@ -6431,10 +6445,10 @@
     <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="35"/>
       <c r="B244" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D244" s="35"/>
       <c r="E244" s="29"/>
@@ -6449,10 +6463,10 @@
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="35"/>
       <c r="B245" s="7" t="s">
-        <v>167</v>
+        <v>315</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>148</v>
+        <v>316</v>
       </c>
       <c r="D245" s="35"/>
       <c r="E245" s="29"/>
@@ -6467,10 +6481,10 @@
     <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="35"/>
       <c r="B246" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D246" s="35"/>
       <c r="E246" s="29"/>
@@ -6485,10 +6499,10 @@
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="35"/>
       <c r="B247" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D247" s="35"/>
       <c r="E247" s="29"/>
@@ -6503,10 +6517,10 @@
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="35"/>
       <c r="B248" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C248" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D248" s="35"/>
       <c r="E248" s="29"/>
@@ -6521,10 +6535,10 @@
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="35"/>
       <c r="B249" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D249" s="35"/>
       <c r="E249" s="29"/>
@@ -6539,10 +6553,10 @@
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="35"/>
       <c r="B250" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D250" s="35"/>
       <c r="E250" s="29"/>
@@ -6557,10 +6571,10 @@
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="35"/>
       <c r="B251" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D251" s="35"/>
       <c r="E251" s="29"/>
@@ -6575,10 +6589,10 @@
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="35"/>
       <c r="B252" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D252" s="35"/>
       <c r="E252" s="29"/>
@@ -6593,10 +6607,10 @@
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="35"/>
       <c r="B253" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D253" s="35"/>
       <c r="E253" s="29"/>
@@ -6611,10 +6625,10 @@
     <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="35"/>
       <c r="B254" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D254" s="35"/>
       <c r="E254" s="29"/>
@@ -6629,10 +6643,10 @@
     <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="35"/>
       <c r="B255" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D255" s="35"/>
       <c r="E255" s="29"/>
@@ -6647,10 +6661,10 @@
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="35"/>
       <c r="B256" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D256" s="35"/>
       <c r="E256" s="29"/>
@@ -6665,10 +6679,10 @@
     <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="35"/>
       <c r="B257" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D257" s="35"/>
       <c r="E257" s="29"/>
@@ -6683,10 +6697,10 @@
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="35"/>
       <c r="B258" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D258" s="35"/>
       <c r="E258" s="29"/>
@@ -6701,10 +6715,10 @@
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="35"/>
       <c r="B259" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C259" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D259" s="35"/>
       <c r="E259" s="29"/>
@@ -6719,10 +6733,10 @@
     <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="35"/>
       <c r="B260" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D260" s="35"/>
       <c r="E260" s="29"/>
@@ -6737,10 +6751,10 @@
     <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="35"/>
       <c r="B261" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C261" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D261" s="35"/>
       <c r="E261" s="29"/>
@@ -6755,10 +6769,10 @@
     <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" s="35"/>
       <c r="B262" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C262" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D262" s="35"/>
       <c r="E262" s="29"/>
@@ -6773,7 +6787,7 @@
     <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="35"/>
       <c r="B263" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C263" s="4" t="s">
         <v>163</v>
@@ -6791,7 +6805,7 @@
     <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" s="35"/>
       <c r="B264" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C264" s="4" t="s">
         <v>163</v>
@@ -6809,7 +6823,7 @@
     <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" s="35"/>
       <c r="B265" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C265" s="4" t="s">
         <v>163</v>
@@ -6827,7 +6841,7 @@
     <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" s="35"/>
       <c r="B266" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C266" s="4" t="s">
         <v>163</v>
@@ -6845,7 +6859,7 @@
     <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" s="35"/>
       <c r="B267" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C267" s="4" t="s">
         <v>163</v>
@@ -6863,7 +6877,7 @@
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" s="35"/>
       <c r="B268" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C268" s="4" t="s">
         <v>163</v>
@@ -6881,7 +6895,7 @@
     <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" s="35"/>
       <c r="B269" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C269" s="4" t="s">
         <v>163</v>
@@ -6899,7 +6913,7 @@
     <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270" s="35"/>
       <c r="B270" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C270" s="4" t="s">
         <v>163</v>
@@ -6917,7 +6931,7 @@
     <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" s="35"/>
       <c r="B271" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C271" s="4" t="s">
         <v>163</v>
@@ -6935,7 +6949,7 @@
     <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" s="35"/>
       <c r="B272" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C272" s="4" t="s">
         <v>163</v>
@@ -6953,7 +6967,7 @@
     <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="35"/>
       <c r="B273" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C273" s="4" t="s">
         <v>163</v>
@@ -6971,7 +6985,7 @@
     <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="35"/>
       <c r="B274" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C274" s="4" t="s">
         <v>163</v>
@@ -6989,7 +7003,7 @@
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="35"/>
       <c r="B275" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C275" s="4" t="s">
         <v>163</v>
@@ -7007,7 +7021,7 @@
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="35"/>
       <c r="B276" s="7" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="C276" s="4" t="s">
         <v>163</v>
@@ -7024,31 +7038,47 @@
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="35"/>
-      <c r="B277" s="7"/>
-      <c r="C277" s="4"/>
+      <c r="B277" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C277" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="D277" s="35"/>
       <c r="E277" s="29"/>
-      <c r="F277" s="19"/>
-      <c r="G277" s="20"/>
+      <c r="F277" s="19">
+        <v>1</v>
+      </c>
+      <c r="G277" s="20">
+        <v>0</v>
+      </c>
       <c r="H277" s="35"/>
     </row>
-    <row r="278" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="35"/>
-      <c r="B278" s="9"/>
-      <c r="C278" s="10"/>
+      <c r="B278" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C278" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="D278" s="35"/>
-      <c r="E278" s="30"/>
-      <c r="F278" s="21"/>
-      <c r="G278" s="22"/>
+      <c r="E278" s="29"/>
+      <c r="F278" s="19">
+        <v>1</v>
+      </c>
+      <c r="G278" s="20">
+        <v>0</v>
+      </c>
       <c r="H278" s="35"/>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="35"/>
       <c r="B279" s="7" t="s">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="C279" s="4" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="D279" s="35"/>
       <c r="E279" s="29"/>
@@ -7060,289 +7090,257 @@
       </c>
       <c r="H279" s="35"/>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="35"/>
-      <c r="B280" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="C280" s="4" t="s">
-        <v>327</v>
-      </c>
+      <c r="B280" s="11"/>
+      <c r="C280" s="12"/>
       <c r="D280" s="35"/>
-      <c r="E280" s="29"/>
-      <c r="F280" s="19">
-        <v>1</v>
-      </c>
-      <c r="G280" s="20">
-        <v>0</v>
-      </c>
+      <c r="E280" s="32"/>
+      <c r="F280" s="23"/>
+      <c r="G280" s="24"/>
       <c r="H280" s="35"/>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="35"/>
       <c r="B281" s="7" t="s">
-        <v>326</v>
+        <v>510</v>
       </c>
       <c r="C281" s="4" t="s">
-        <v>328</v>
+        <v>511</v>
       </c>
       <c r="D281" s="35"/>
       <c r="E281" s="29"/>
-      <c r="F281" s="19">
-        <v>1</v>
-      </c>
-      <c r="G281" s="20">
-        <v>0</v>
-      </c>
+      <c r="F281" s="19"/>
+      <c r="G281" s="20"/>
       <c r="H281" s="35"/>
     </row>
     <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282" s="35"/>
       <c r="B282" s="7" t="s">
-        <v>319</v>
+        <v>502</v>
       </c>
       <c r="C282" s="4" t="s">
-        <v>320</v>
+        <v>503</v>
       </c>
       <c r="D282" s="35"/>
       <c r="E282" s="29"/>
-      <c r="F282" s="19">
-        <v>1</v>
-      </c>
-      <c r="G282" s="20">
-        <v>0</v>
-      </c>
+      <c r="F282" s="19"/>
+      <c r="G282" s="20"/>
       <c r="H282" s="35"/>
     </row>
-    <row r="283" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A283" s="37"/>
-      <c r="B283" s="13" t="s">
-        <v>369</v>
-      </c>
-      <c r="C283" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="D283" s="37"/>
-      <c r="E283" s="31"/>
-      <c r="F283" s="19">
-        <v>1</v>
-      </c>
-      <c r="G283" s="20">
-        <v>0</v>
-      </c>
-      <c r="H283" s="37"/>
-    </row>
-    <row r="284" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A284" s="37"/>
-      <c r="B284" s="13" t="s">
-        <v>370</v>
-      </c>
-      <c r="C284" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="D284" s="37"/>
-      <c r="E284" s="31"/>
-      <c r="F284" s="19">
-        <v>1</v>
-      </c>
-      <c r="G284" s="20">
-        <v>0</v>
-      </c>
-      <c r="H284" s="37"/>
-    </row>
-    <row r="285" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A285" s="37"/>
-      <c r="B285" s="13" t="s">
-        <v>371</v>
-      </c>
-      <c r="C285" s="14" t="s">
-        <v>375</v>
-      </c>
-      <c r="D285" s="37"/>
-      <c r="E285" s="31"/>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A283" s="35"/>
+      <c r="B283" s="7"/>
+      <c r="C283" s="4"/>
+      <c r="D283" s="35"/>
+      <c r="E283" s="29"/>
+      <c r="F283" s="19"/>
+      <c r="G283" s="20"/>
+      <c r="H283" s="35"/>
+    </row>
+    <row r="284" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A284" s="35"/>
+      <c r="B284" s="9"/>
+      <c r="C284" s="10"/>
+      <c r="D284" s="35"/>
+      <c r="E284" s="30"/>
+      <c r="F284" s="21"/>
+      <c r="G284" s="22"/>
+      <c r="H284" s="35"/>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A285" s="35"/>
+      <c r="B285" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C285" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D285" s="35"/>
+      <c r="E285" s="29"/>
       <c r="F285" s="19">
         <v>1</v>
       </c>
       <c r="G285" s="20">
         <v>0</v>
       </c>
-      <c r="H285" s="37"/>
-    </row>
-    <row r="286" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A286" s="37"/>
-      <c r="B286" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="C286" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="D286" s="37"/>
-      <c r="E286" s="31"/>
+      <c r="H285" s="35"/>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A286" s="35"/>
+      <c r="B286" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="C286" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D286" s="35"/>
+      <c r="E286" s="29"/>
       <c r="F286" s="19">
         <v>1</v>
       </c>
       <c r="G286" s="20">
         <v>0</v>
       </c>
-      <c r="H286" s="37"/>
-    </row>
-    <row r="287" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="37"/>
+      <c r="H286" s="35"/>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A287" s="35"/>
       <c r="B287" s="7" t="s">
-        <v>436</v>
+        <v>326</v>
       </c>
       <c r="C287" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="D287" s="37"/>
-      <c r="E287" s="31"/>
-      <c r="F287" s="19"/>
-      <c r="G287" s="20"/>
-      <c r="H287" s="37"/>
-    </row>
-    <row r="288" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A288" s="37"/>
+        <v>328</v>
+      </c>
+      <c r="D287" s="35"/>
+      <c r="E287" s="29"/>
+      <c r="F287" s="19">
+        <v>1</v>
+      </c>
+      <c r="G287" s="20">
+        <v>0</v>
+      </c>
+      <c r="H287" s="35"/>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A288" s="35"/>
       <c r="B288" s="7" t="s">
-        <v>438</v>
+        <v>319</v>
       </c>
       <c r="C288" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="D288" s="37"/>
-      <c r="E288" s="31"/>
-      <c r="F288" s="19"/>
-      <c r="G288" s="20"/>
-      <c r="H288" s="37"/>
+        <v>320</v>
+      </c>
+      <c r="D288" s="35"/>
+      <c r="E288" s="29"/>
+      <c r="F288" s="19">
+        <v>1</v>
+      </c>
+      <c r="G288" s="20">
+        <v>0</v>
+      </c>
+      <c r="H288" s="35"/>
     </row>
     <row r="289" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A289" s="37"/>
-      <c r="B289" s="7" t="s">
-        <v>439</v>
-      </c>
-      <c r="C289" s="4" t="s">
-        <v>440</v>
+      <c r="B289" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="C289" s="14" t="s">
+        <v>373</v>
       </c>
       <c r="D289" s="37"/>
       <c r="E289" s="31"/>
-      <c r="F289" s="19"/>
-      <c r="G289" s="20"/>
+      <c r="F289" s="19">
+        <v>1</v>
+      </c>
+      <c r="G289" s="20">
+        <v>0</v>
+      </c>
       <c r="H289" s="37"/>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A290" s="35"/>
-      <c r="B290" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="C290" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D290" s="35"/>
-      <c r="E290" s="29"/>
+    <row r="290" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="37"/>
+      <c r="B290" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="C290" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="D290" s="37"/>
+      <c r="E290" s="31"/>
       <c r="F290" s="19">
         <v>1</v>
       </c>
       <c r="G290" s="20">
         <v>0</v>
       </c>
-      <c r="H290" s="35"/>
-    </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A291" s="35"/>
-      <c r="B291" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="C291" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D291" s="35"/>
-      <c r="E291" s="29"/>
+      <c r="H290" s="37"/>
+    </row>
+    <row r="291" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="37"/>
+      <c r="B291" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="C291" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="D291" s="37"/>
+      <c r="E291" s="31"/>
       <c r="F291" s="19">
         <v>1</v>
       </c>
       <c r="G291" s="20">
         <v>0</v>
       </c>
-      <c r="H291" s="35"/>
-    </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A292" s="35"/>
-      <c r="B292" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="C292" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="D292" s="35"/>
-      <c r="E292" s="29"/>
+      <c r="H291" s="37"/>
+    </row>
+    <row r="292" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A292" s="37"/>
+      <c r="B292" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="C292" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="D292" s="37"/>
+      <c r="E292" s="31"/>
       <c r="F292" s="19">
         <v>1</v>
       </c>
       <c r="G292" s="20">
         <v>0</v>
       </c>
-      <c r="H292" s="35"/>
-    </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A293" s="35"/>
+      <c r="H292" s="37"/>
+    </row>
+    <row r="293" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="37"/>
       <c r="B293" s="7" t="s">
-        <v>349</v>
+        <v>436</v>
       </c>
       <c r="C293" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="D293" s="35"/>
-      <c r="E293" s="29"/>
-      <c r="F293" s="19">
-        <v>1</v>
-      </c>
-      <c r="G293" s="20">
-        <v>0</v>
-      </c>
-      <c r="H293" s="35"/>
-    </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A294" s="35"/>
+        <v>437</v>
+      </c>
+      <c r="D293" s="37"/>
+      <c r="E293" s="31"/>
+      <c r="F293" s="19"/>
+      <c r="G293" s="20"/>
+      <c r="H293" s="37"/>
+    </row>
+    <row r="294" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A294" s="37"/>
       <c r="B294" s="7" t="s">
-        <v>348</v>
+        <v>438</v>
       </c>
       <c r="C294" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="D294" s="35"/>
-      <c r="E294" s="29"/>
-      <c r="F294" s="19">
-        <v>1</v>
-      </c>
-      <c r="G294" s="20">
-        <v>0</v>
-      </c>
-      <c r="H294" s="35"/>
-    </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A295" s="35"/>
+        <v>441</v>
+      </c>
+      <c r="D294" s="37"/>
+      <c r="E294" s="31"/>
+      <c r="F294" s="19"/>
+      <c r="G294" s="20"/>
+      <c r="H294" s="37"/>
+    </row>
+    <row r="295" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A295" s="37"/>
       <c r="B295" s="7" t="s">
-        <v>347</v>
+        <v>439</v>
       </c>
       <c r="C295" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="D295" s="35"/>
-      <c r="E295" s="29"/>
-      <c r="F295" s="19">
-        <v>1</v>
-      </c>
-      <c r="G295" s="20">
-        <v>0</v>
-      </c>
-      <c r="H295" s="35"/>
+        <v>440</v>
+      </c>
+      <c r="D295" s="37"/>
+      <c r="E295" s="31"/>
+      <c r="F295" s="19"/>
+      <c r="G295" s="20"/>
+      <c r="H295" s="37"/>
     </row>
     <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296" s="35"/>
       <c r="B296" s="7" t="s">
-        <v>337</v>
+        <v>353</v>
       </c>
       <c r="C296" s="4" t="s">
-        <v>338</v>
+        <v>357</v>
       </c>
       <c r="D296" s="35"/>
       <c r="E296" s="29"/>
@@ -7357,10 +7355,10 @@
     <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297" s="35"/>
       <c r="B297" s="7" t="s">
-        <v>335</v>
+        <v>354</v>
       </c>
       <c r="C297" s="4" t="s">
-        <v>336</v>
+        <v>356</v>
       </c>
       <c r="D297" s="35"/>
       <c r="E297" s="29"/>
@@ -7375,10 +7373,10 @@
     <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298" s="35"/>
       <c r="B298" s="7" t="s">
-        <v>329</v>
+        <v>355</v>
       </c>
       <c r="C298" s="4" t="s">
-        <v>330</v>
+        <v>358</v>
       </c>
       <c r="D298" s="35"/>
       <c r="E298" s="29"/>
@@ -7390,101 +7388,209 @@
       </c>
       <c r="H298" s="35"/>
     </row>
-    <row r="299" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299" s="35"/>
-      <c r="B299" s="11"/>
-      <c r="C299" s="12"/>
+      <c r="B299" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C299" s="4" t="s">
+        <v>350</v>
+      </c>
       <c r="D299" s="35"/>
-      <c r="E299" s="32"/>
-      <c r="F299" s="23"/>
-      <c r="G299" s="24"/>
+      <c r="E299" s="29"/>
+      <c r="F299" s="19">
+        <v>1</v>
+      </c>
+      <c r="G299" s="20">
+        <v>0</v>
+      </c>
       <c r="H299" s="35"/>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300" s="35"/>
       <c r="B300" s="7" t="s">
-        <v>498</v>
+        <v>348</v>
       </c>
       <c r="C300" s="4" t="s">
-        <v>499</v>
+        <v>351</v>
       </c>
       <c r="D300" s="35"/>
       <c r="E300" s="29"/>
-      <c r="F300" s="19"/>
-      <c r="G300" s="20"/>
+      <c r="F300" s="19">
+        <v>1</v>
+      </c>
+      <c r="G300" s="20">
+        <v>0</v>
+      </c>
       <c r="H300" s="35"/>
     </row>
-    <row r="301" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301" s="35"/>
-      <c r="B301" s="11"/>
-      <c r="C301" s="12"/>
+      <c r="B301" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C301" s="4" t="s">
+        <v>352</v>
+      </c>
       <c r="D301" s="35"/>
-      <c r="E301" s="32"/>
-      <c r="F301" s="23"/>
-      <c r="G301" s="24"/>
+      <c r="E301" s="29"/>
+      <c r="F301" s="19">
+        <v>1</v>
+      </c>
+      <c r="G301" s="20">
+        <v>0</v>
+      </c>
       <c r="H301" s="35"/>
     </row>
     <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302" s="35"/>
       <c r="B302" s="7" t="s">
-        <v>442</v>
+        <v>337</v>
       </c>
       <c r="C302" s="4" t="s">
-        <v>443</v>
+        <v>338</v>
       </c>
       <c r="D302" s="35"/>
       <c r="E302" s="29"/>
-      <c r="F302" s="19"/>
-      <c r="G302" s="20"/>
+      <c r="F302" s="19">
+        <v>1</v>
+      </c>
+      <c r="G302" s="20">
+        <v>0</v>
+      </c>
       <c r="H302" s="35"/>
     </row>
     <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303" s="35"/>
       <c r="B303" s="7" t="s">
-        <v>452</v>
+        <v>335</v>
       </c>
       <c r="C303" s="4" t="s">
-        <v>453</v>
+        <v>336</v>
       </c>
       <c r="D303" s="35"/>
       <c r="E303" s="29"/>
-      <c r="F303" s="19"/>
-      <c r="G303" s="20"/>
+      <c r="F303" s="19">
+        <v>1</v>
+      </c>
+      <c r="G303" s="20">
+        <v>0</v>
+      </c>
       <c r="H303" s="35"/>
     </row>
     <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304" s="35"/>
       <c r="B304" s="7" t="s">
-        <v>444</v>
+        <v>329</v>
       </c>
       <c r="C304" s="4" t="s">
-        <v>445</v>
+        <v>330</v>
       </c>
       <c r="D304" s="35"/>
       <c r="E304" s="29"/>
-      <c r="F304" s="19"/>
-      <c r="G304" s="20"/>
+      <c r="F304" s="19">
+        <v>1</v>
+      </c>
+      <c r="G304" s="20">
+        <v>0</v>
+      </c>
       <c r="H304" s="35"/>
     </row>
-    <row r="305" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="35"/>
-      <c r="B305" s="8"/>
-      <c r="C305" s="6"/>
+      <c r="B305" s="11"/>
+      <c r="C305" s="12"/>
       <c r="D305" s="35"/>
-      <c r="E305" s="33"/>
-      <c r="F305" s="25"/>
-      <c r="G305" s="26"/>
+      <c r="E305" s="32"/>
+      <c r="F305" s="23"/>
+      <c r="G305" s="24"/>
       <c r="H305" s="35"/>
     </row>
-    <row r="306" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306" s="35"/>
-      <c r="B306" s="38"/>
-      <c r="C306" s="39"/>
+      <c r="B306" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="C306" s="4" t="s">
+        <v>499</v>
+      </c>
       <c r="D306" s="35"/>
-      <c r="E306" s="40"/>
-      <c r="F306" s="41"/>
-      <c r="G306" s="41"/>
+      <c r="E306" s="29"/>
+      <c r="F306" s="19"/>
+      <c r="G306" s="20"/>
       <c r="H306" s="35"/>
+    </row>
+    <row r="307" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A307" s="35"/>
+      <c r="B307" s="11"/>
+      <c r="C307" s="12"/>
+      <c r="D307" s="35"/>
+      <c r="E307" s="32"/>
+      <c r="F307" s="23"/>
+      <c r="G307" s="24"/>
+      <c r="H307" s="35"/>
+    </row>
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A308" s="35"/>
+      <c r="B308" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="C308" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="D308" s="35"/>
+      <c r="E308" s="29"/>
+      <c r="F308" s="19"/>
+      <c r="G308" s="20"/>
+      <c r="H308" s="35"/>
+    </row>
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A309" s="35"/>
+      <c r="B309" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="C309" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="D309" s="35"/>
+      <c r="E309" s="29"/>
+      <c r="F309" s="19"/>
+      <c r="G309" s="20"/>
+      <c r="H309" s="35"/>
+    </row>
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A310" s="35"/>
+      <c r="B310" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="C310" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D310" s="35"/>
+      <c r="E310" s="29"/>
+      <c r="F310" s="19"/>
+      <c r="G310" s="20"/>
+      <c r="H310" s="35"/>
+    </row>
+    <row r="311" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A311" s="35"/>
+      <c r="B311" s="8"/>
+      <c r="C311" s="6"/>
+      <c r="D311" s="35"/>
+      <c r="E311" s="33"/>
+      <c r="F311" s="25"/>
+      <c r="G311" s="26"/>
+      <c r="H311" s="35"/>
+    </row>
+    <row r="312" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A312" s="35"/>
+      <c r="B312" s="38"/>
+      <c r="C312" s="39"/>
+      <c r="D312" s="35"/>
+      <c r="E312" s="40"/>
+      <c r="F312" s="41"/>
+      <c r="G312" s="41"/>
+      <c r="H312" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Penambahan API dan Update Data API Catalogue
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="675">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -2117,6 +2117,36 @@
   </si>
   <si>
     <t>Membatalkan Penghapusan Data Sales Order</t>
+  </si>
+  <si>
+    <t>transaction.undelete.dataAcquisition.setLog_Device_PersonAccess</t>
+  </si>
+  <si>
+    <t>transaction.undelete.dataAcquisition.setLog_Device_PersonAccessFetch</t>
+  </si>
+  <si>
+    <t>Membatalkan Penghapusan Data Log Alat Akses Orang</t>
+  </si>
+  <si>
+    <t>Membatalkan Penghapusan Data Log Fetch Alat Akses Orang</t>
+  </si>
+  <si>
+    <t>transaction.undelete.finance.setAdvance</t>
+  </si>
+  <si>
+    <t>transaction.undelete.finance.setAdvanceDetail</t>
+  </si>
+  <si>
+    <t>Membatalkan Penghapusan Data Uang Muka</t>
+  </si>
+  <si>
+    <t>Membatalkan Penghapusan Data Perician Uang Muka</t>
+  </si>
+  <si>
+    <t>transaction.undelete.fixedAsset.setGoodsIdentity</t>
+  </si>
+  <si>
+    <t>Membatalkan Penghapusan Data Identitas Barang</t>
   </si>
 </sst>
 </file>
@@ -3022,13 +3052,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L401"/>
+  <dimension ref="A1:L409"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C310" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C320" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C322" sqref="C322"/>
+      <selection pane="bottomRight" activeCell="F333" sqref="F333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5172,14 +5202,14 @@
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="35"/>
       <c r="B101" s="7" t="s">
-        <v>204</v>
+        <v>647</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>206</v>
+        <v>649</v>
       </c>
       <c r="D101" s="35"/>
       <c r="E101" s="29">
-        <v>44154</v>
+        <v>44378</v>
       </c>
       <c r="F101" s="60" t="s">
         <v>632</v>
@@ -5197,14 +5227,14 @@
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="35"/>
       <c r="B102" s="7" t="s">
-        <v>205</v>
+        <v>648</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>207</v>
+        <v>650</v>
       </c>
       <c r="D102" s="35"/>
       <c r="E102" s="29">
-        <v>44154</v>
+        <v>44378</v>
       </c>
       <c r="F102" s="60" t="s">
         <v>632</v>
@@ -5235,14 +5265,14 @@
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
       <c r="B104" s="7" t="s">
-        <v>647</v>
+        <v>204</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>649</v>
+        <v>206</v>
       </c>
       <c r="D104" s="35"/>
       <c r="E104" s="29">
-        <v>44378</v>
+        <v>44154</v>
       </c>
       <c r="F104" s="60" t="s">
         <v>632</v>
@@ -5260,14 +5290,14 @@
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="35"/>
       <c r="B105" s="7" t="s">
-        <v>648</v>
+        <v>205</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>650</v>
+        <v>207</v>
       </c>
       <c r="D105" s="35"/>
       <c r="E105" s="29">
-        <v>44378</v>
+        <v>44154</v>
       </c>
       <c r="F105" s="60" t="s">
         <v>632</v>
@@ -10124,14 +10154,18 @@
     <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321" s="35"/>
       <c r="B321" s="7" t="s">
-        <v>32</v>
+        <v>665</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>74</v>
+        <v>667</v>
       </c>
       <c r="D321" s="35"/>
-      <c r="E321" s="29"/>
-      <c r="F321" s="60"/>
+      <c r="E321" s="29">
+        <v>44379</v>
+      </c>
+      <c r="F321" s="60" t="s">
+        <v>632</v>
+      </c>
       <c r="G321" s="35"/>
       <c r="H321" s="29"/>
       <c r="I321" s="19">
@@ -10145,14 +10179,18 @@
     <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322" s="35"/>
       <c r="B322" s="7" t="s">
-        <v>145</v>
+        <v>666</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>126</v>
+        <v>668</v>
       </c>
       <c r="D322" s="35"/>
-      <c r="E322" s="29"/>
-      <c r="F322" s="60"/>
+      <c r="E322" s="29">
+        <v>44379</v>
+      </c>
+      <c r="F322" s="60" t="s">
+        <v>632</v>
+      </c>
       <c r="G322" s="35"/>
       <c r="H322" s="29"/>
       <c r="I322" s="19">
@@ -10163,38 +10201,34 @@
       </c>
       <c r="K322" s="35"/>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A323" s="35"/>
-      <c r="B323" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="C323" s="4" t="s">
-        <v>286</v>
-      </c>
+      <c r="B323" s="11"/>
+      <c r="C323" s="12"/>
       <c r="D323" s="35"/>
-      <c r="E323" s="29"/>
-      <c r="F323" s="60"/>
+      <c r="E323" s="32"/>
+      <c r="F323" s="62"/>
       <c r="G323" s="35"/>
-      <c r="H323" s="29"/>
-      <c r="I323" s="19">
-        <v>1</v>
-      </c>
-      <c r="J323" s="20">
-        <v>0</v>
-      </c>
+      <c r="H323" s="32"/>
+      <c r="I323" s="23"/>
+      <c r="J323" s="24"/>
       <c r="K323" s="35"/>
     </row>
     <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324" s="35"/>
       <c r="B324" s="7" t="s">
-        <v>146</v>
+        <v>669</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>127</v>
+        <v>671</v>
       </c>
       <c r="D324" s="35"/>
-      <c r="E324" s="29"/>
-      <c r="F324" s="60"/>
+      <c r="E324" s="29">
+        <v>44379</v>
+      </c>
+      <c r="F324" s="60" t="s">
+        <v>632</v>
+      </c>
       <c r="G324" s="35"/>
       <c r="H324" s="29"/>
       <c r="I324" s="19">
@@ -10208,14 +10242,18 @@
     <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A325" s="35"/>
       <c r="B325" s="7" t="s">
-        <v>147</v>
+        <v>670</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>128</v>
+        <v>672</v>
       </c>
       <c r="D325" s="35"/>
-      <c r="E325" s="29"/>
-      <c r="F325" s="60"/>
+      <c r="E325" s="29">
+        <v>44379</v>
+      </c>
+      <c r="F325" s="60" t="s">
+        <v>632</v>
+      </c>
       <c r="G325" s="35"/>
       <c r="H325" s="29"/>
       <c r="I325" s="19">
@@ -10226,38 +10264,34 @@
       </c>
       <c r="K325" s="35"/>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A326" s="35"/>
-      <c r="B326" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C326" s="4" t="s">
-        <v>129</v>
-      </c>
+      <c r="B326" s="11"/>
+      <c r="C326" s="12"/>
       <c r="D326" s="35"/>
-      <c r="E326" s="29"/>
-      <c r="F326" s="60"/>
+      <c r="E326" s="32"/>
+      <c r="F326" s="62"/>
       <c r="G326" s="35"/>
-      <c r="H326" s="29"/>
-      <c r="I326" s="19">
-        <v>1</v>
-      </c>
-      <c r="J326" s="20">
-        <v>0</v>
-      </c>
+      <c r="H326" s="32"/>
+      <c r="I326" s="23"/>
+      <c r="J326" s="24"/>
       <c r="K326" s="35"/>
     </row>
     <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" s="35"/>
       <c r="B327" s="7" t="s">
-        <v>149</v>
+        <v>673</v>
       </c>
       <c r="C327" s="4" t="s">
-        <v>130</v>
+        <v>674</v>
       </c>
       <c r="D327" s="35"/>
-      <c r="E327" s="29"/>
-      <c r="F327" s="60"/>
+      <c r="E327" s="29">
+        <v>44379</v>
+      </c>
+      <c r="F327" s="60" t="s">
+        <v>632</v>
+      </c>
       <c r="G327" s="35"/>
       <c r="H327" s="29"/>
       <c r="I327" s="19">
@@ -10268,34 +10302,26 @@
       </c>
       <c r="K327" s="35"/>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A328" s="35"/>
-      <c r="B328" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C328" s="4" t="s">
-        <v>131</v>
-      </c>
+      <c r="B328" s="11"/>
+      <c r="C328" s="12"/>
       <c r="D328" s="35"/>
-      <c r="E328" s="29"/>
-      <c r="F328" s="60"/>
+      <c r="E328" s="32"/>
+      <c r="F328" s="62"/>
       <c r="G328" s="35"/>
-      <c r="H328" s="29"/>
-      <c r="I328" s="19">
-        <v>1</v>
-      </c>
-      <c r="J328" s="20">
-        <v>0</v>
-      </c>
+      <c r="H328" s="32"/>
+      <c r="I328" s="23"/>
+      <c r="J328" s="24"/>
       <c r="K328" s="35"/>
     </row>
     <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329" s="35"/>
       <c r="B329" s="7" t="s">
-        <v>151</v>
+        <v>32</v>
       </c>
       <c r="C329" s="4" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
       <c r="D329" s="35"/>
       <c r="E329" s="29"/>
@@ -10313,10 +10339,10 @@
     <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330" s="35"/>
       <c r="B330" s="7" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C330" s="4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D330" s="35"/>
       <c r="E330" s="29"/>
@@ -10334,10 +10360,10 @@
     <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331" s="35"/>
       <c r="B331" s="7" t="s">
-        <v>153</v>
+        <v>285</v>
       </c>
       <c r="C331" s="4" t="s">
-        <v>134</v>
+        <v>286</v>
       </c>
       <c r="D331" s="35"/>
       <c r="E331" s="29"/>
@@ -10355,10 +10381,10 @@
     <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332" s="35"/>
       <c r="B332" s="7" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C332" s="4" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D332" s="35"/>
       <c r="E332" s="29"/>
@@ -10376,10 +10402,10 @@
     <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333" s="35"/>
       <c r="B333" s="7" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C333" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D333" s="35"/>
       <c r="E333" s="29"/>
@@ -10397,10 +10423,10 @@
     <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A334" s="35"/>
       <c r="B334" s="7" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C334" s="4" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D334" s="35"/>
       <c r="E334" s="29"/>
@@ -10418,10 +10444,10 @@
     <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335" s="35"/>
       <c r="B335" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C335" s="4" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D335" s="35"/>
       <c r="E335" s="29"/>
@@ -10439,10 +10465,10 @@
     <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336" s="35"/>
       <c r="B336" s="7" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C336" s="4" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D336" s="35"/>
       <c r="E336" s="29"/>
@@ -10460,10 +10486,10 @@
     <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337" s="35"/>
       <c r="B337" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C337" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D337" s="35"/>
       <c r="E337" s="29"/>
@@ -10481,10 +10507,10 @@
     <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338" s="35"/>
       <c r="B338" s="7" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C338" s="4" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D338" s="35"/>
       <c r="E338" s="29"/>
@@ -10502,10 +10528,10 @@
     <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339" s="35"/>
       <c r="B339" s="7" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C339" s="4" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D339" s="35"/>
       <c r="E339" s="29"/>
@@ -10523,10 +10549,10 @@
     <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A340" s="35"/>
       <c r="B340" s="7" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C340" s="4" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D340" s="35"/>
       <c r="E340" s="29"/>
@@ -10544,10 +10570,10 @@
     <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A341" s="35"/>
       <c r="B341" s="7" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C341" s="4" t="s">
-        <v>628</v>
+        <v>136</v>
       </c>
       <c r="D341" s="35"/>
       <c r="E341" s="29"/>
@@ -10565,10 +10591,10 @@
     <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342" s="35"/>
       <c r="B342" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C342" s="4" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D342" s="35"/>
       <c r="E342" s="29"/>
@@ -10586,10 +10612,10 @@
     <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343" s="35"/>
       <c r="B343" s="7" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C343" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D343" s="35"/>
       <c r="E343" s="29"/>
@@ -10607,10 +10633,10 @@
     <row r="344" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A344" s="35"/>
       <c r="B344" s="7" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C344" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D344" s="35"/>
       <c r="E344" s="29"/>
@@ -10628,10 +10654,10 @@
     <row r="345" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A345" s="35"/>
       <c r="B345" s="7" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C345" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D345" s="35"/>
       <c r="E345" s="29"/>
@@ -10649,10 +10675,10 @@
     <row r="346" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A346" s="35"/>
       <c r="B346" s="7" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C346" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D346" s="35"/>
       <c r="E346" s="29"/>
@@ -10670,10 +10696,10 @@
     <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A347" s="35"/>
       <c r="B347" s="7" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C347" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D347" s="35"/>
       <c r="E347" s="29"/>
@@ -10691,10 +10717,10 @@
     <row r="348" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A348" s="35"/>
       <c r="B348" s="7" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C348" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D348" s="35"/>
       <c r="E348" s="29"/>
@@ -10712,10 +10738,10 @@
     <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349" s="35"/>
       <c r="B349" s="7" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C349" s="4" t="s">
-        <v>144</v>
+        <v>628</v>
       </c>
       <c r="D349" s="35"/>
       <c r="E349" s="29"/>
@@ -10733,7 +10759,7 @@
     <row r="350" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A350" s="35"/>
       <c r="B350" s="7" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C350" s="4" t="s">
         <v>144</v>
@@ -10754,7 +10780,7 @@
     <row r="351" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A351" s="35"/>
       <c r="B351" s="7" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C351" s="4" t="s">
         <v>144</v>
@@ -10775,7 +10801,7 @@
     <row r="352" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A352" s="35"/>
       <c r="B352" s="7" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C352" s="4" t="s">
         <v>144</v>
@@ -10796,7 +10822,7 @@
     <row r="353" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A353" s="35"/>
       <c r="B353" s="7" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C353" s="4" t="s">
         <v>144</v>
@@ -10817,7 +10843,7 @@
     <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354" s="35"/>
       <c r="B354" s="7" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C354" s="4" t="s">
         <v>144</v>
@@ -10838,7 +10864,7 @@
     <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A355" s="35"/>
       <c r="B355" s="7" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C355" s="4" t="s">
         <v>144</v>
@@ -10856,23 +10882,31 @@
       </c>
       <c r="K355" s="35"/>
     </row>
-    <row r="356" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A356" s="35"/>
-      <c r="B356" s="11"/>
-      <c r="C356" s="12"/>
+      <c r="B356" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C356" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="D356" s="35"/>
-      <c r="E356" s="32"/>
-      <c r="F356" s="62"/>
+      <c r="E356" s="29"/>
+      <c r="F356" s="60"/>
       <c r="G356" s="35"/>
-      <c r="H356" s="32"/>
-      <c r="I356" s="23"/>
-      <c r="J356" s="24"/>
+      <c r="H356" s="29"/>
+      <c r="I356" s="19">
+        <v>1</v>
+      </c>
+      <c r="J356" s="20">
+        <v>0</v>
+      </c>
       <c r="K356" s="35"/>
     </row>
     <row r="357" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A357" s="35"/>
       <c r="B357" s="7" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C357" s="4" t="s">
         <v>144</v>
@@ -10893,7 +10927,7 @@
     <row r="358" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A358" s="35"/>
       <c r="B358" s="7" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="C358" s="4" t="s">
         <v>144</v>
@@ -10913,79 +10947,107 @@
     </row>
     <row r="359" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A359" s="35"/>
-      <c r="B359" s="7"/>
-      <c r="C359" s="4"/>
+      <c r="B359" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C359" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="D359" s="35"/>
       <c r="E359" s="29"/>
       <c r="F359" s="60"/>
       <c r="G359" s="35"/>
       <c r="H359" s="29"/>
-      <c r="I359" s="19"/>
-      <c r="J359" s="20"/>
+      <c r="I359" s="19">
+        <v>1</v>
+      </c>
+      <c r="J359" s="20">
+        <v>0</v>
+      </c>
       <c r="K359" s="35"/>
     </row>
-    <row r="360" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A360" s="35"/>
-      <c r="B360" s="9"/>
-      <c r="C360" s="10"/>
+      <c r="B360" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C360" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="D360" s="35"/>
-      <c r="E360" s="30"/>
-      <c r="F360" s="61"/>
+      <c r="E360" s="29"/>
+      <c r="F360" s="60"/>
       <c r="G360" s="35"/>
-      <c r="H360" s="30"/>
-      <c r="I360" s="21"/>
-      <c r="J360" s="22"/>
+      <c r="H360" s="29"/>
+      <c r="I360" s="19">
+        <v>1</v>
+      </c>
+      <c r="J360" s="20">
+        <v>0</v>
+      </c>
       <c r="K360" s="35"/>
     </row>
     <row r="361" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A361" s="35"/>
       <c r="B361" s="7" t="s">
-        <v>462</v>
+        <v>175</v>
       </c>
       <c r="C361" s="4" t="s">
-        <v>464</v>
+        <v>144</v>
       </c>
       <c r="D361" s="35"/>
       <c r="E361" s="29"/>
       <c r="F361" s="60"/>
       <c r="G361" s="35"/>
       <c r="H361" s="29"/>
-      <c r="I361" s="19"/>
-      <c r="J361" s="20"/>
+      <c r="I361" s="19">
+        <v>1</v>
+      </c>
+      <c r="J361" s="20">
+        <v>0</v>
+      </c>
       <c r="K361" s="35"/>
     </row>
     <row r="362" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A362" s="35"/>
       <c r="B362" s="7" t="s">
-        <v>451</v>
+        <v>176</v>
       </c>
       <c r="C362" s="4" t="s">
-        <v>452</v>
+        <v>144</v>
       </c>
       <c r="D362" s="35"/>
       <c r="E362" s="29"/>
       <c r="F362" s="60"/>
       <c r="G362" s="35"/>
       <c r="H362" s="29"/>
-      <c r="I362" s="19"/>
-      <c r="J362" s="20"/>
+      <c r="I362" s="19">
+        <v>1</v>
+      </c>
+      <c r="J362" s="20">
+        <v>0</v>
+      </c>
       <c r="K362" s="35"/>
     </row>
     <row r="363" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A363" s="35"/>
       <c r="B363" s="7" t="s">
-        <v>463</v>
+        <v>177</v>
       </c>
       <c r="C363" s="4" t="s">
-        <v>465</v>
+        <v>144</v>
       </c>
       <c r="D363" s="35"/>
       <c r="E363" s="29"/>
       <c r="F363" s="60"/>
       <c r="G363" s="35"/>
       <c r="H363" s="29"/>
-      <c r="I363" s="19"/>
-      <c r="J363" s="20"/>
+      <c r="I363" s="19">
+        <v>1</v>
+      </c>
+      <c r="J363" s="20">
+        <v>0</v>
+      </c>
       <c r="K363" s="35"/>
     </row>
     <row r="364" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11004,45 +11066,49 @@
     <row r="365" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A365" s="35"/>
       <c r="B365" s="7" t="s">
-        <v>409</v>
+        <v>178</v>
       </c>
       <c r="C365" s="4" t="s">
-        <v>410</v>
+        <v>144</v>
       </c>
       <c r="D365" s="35"/>
       <c r="E365" s="29"/>
       <c r="F365" s="60"/>
       <c r="G365" s="35"/>
       <c r="H365" s="29"/>
-      <c r="I365" s="19"/>
-      <c r="J365" s="20"/>
+      <c r="I365" s="19">
+        <v>1</v>
+      </c>
+      <c r="J365" s="20">
+        <v>0</v>
+      </c>
       <c r="K365" s="35"/>
     </row>
     <row r="366" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A366" s="35"/>
       <c r="B366" s="7" t="s">
-        <v>419</v>
+        <v>198</v>
       </c>
       <c r="C366" s="4" t="s">
-        <v>420</v>
+        <v>144</v>
       </c>
       <c r="D366" s="35"/>
       <c r="E366" s="29"/>
       <c r="F366" s="60"/>
       <c r="G366" s="35"/>
       <c r="H366" s="29"/>
-      <c r="I366" s="19"/>
-      <c r="J366" s="20"/>
+      <c r="I366" s="19">
+        <v>1</v>
+      </c>
+      <c r="J366" s="20">
+        <v>0</v>
+      </c>
       <c r="K366" s="35"/>
     </row>
     <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A367" s="35"/>
-      <c r="B367" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="C367" s="4" t="s">
-        <v>412</v>
-      </c>
+      <c r="B367" s="7"/>
+      <c r="C367" s="4"/>
       <c r="D367" s="35"/>
       <c r="E367" s="29"/>
       <c r="F367" s="60"/>
@@ -11052,47 +11118,43 @@
       <c r="J367" s="20"/>
       <c r="K367" s="35"/>
     </row>
-    <row r="368" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="35"/>
-      <c r="B368" s="11"/>
-      <c r="C368" s="12"/>
+      <c r="B368" s="9"/>
+      <c r="C368" s="10"/>
       <c r="D368" s="35"/>
-      <c r="E368" s="32"/>
-      <c r="F368" s="62"/>
+      <c r="E368" s="30"/>
+      <c r="F368" s="61"/>
       <c r="G368" s="35"/>
-      <c r="H368" s="32"/>
-      <c r="I368" s="23"/>
-      <c r="J368" s="24"/>
+      <c r="H368" s="30"/>
+      <c r="I368" s="21"/>
+      <c r="J368" s="22"/>
       <c r="K368" s="35"/>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A369" s="35"/>
       <c r="B369" s="7" t="s">
-        <v>0</v>
+        <v>462</v>
       </c>
       <c r="C369" s="4" t="s">
-        <v>85</v>
+        <v>464</v>
       </c>
       <c r="D369" s="35"/>
       <c r="E369" s="29"/>
       <c r="F369" s="60"/>
       <c r="G369" s="35"/>
       <c r="H369" s="29"/>
-      <c r="I369" s="19">
-        <v>1</v>
-      </c>
-      <c r="J369" s="20">
-        <v>0</v>
-      </c>
+      <c r="I369" s="19"/>
+      <c r="J369" s="20"/>
       <c r="K369" s="35"/>
     </row>
     <row r="370" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A370" s="35"/>
       <c r="B370" s="7" t="s">
-        <v>599</v>
+        <v>451</v>
       </c>
       <c r="C370" s="4" t="s">
-        <v>600</v>
+        <v>452</v>
       </c>
       <c r="D370" s="35"/>
       <c r="E370" s="29"/>
@@ -11106,10 +11168,10 @@
     <row r="371" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A371" s="35"/>
       <c r="B371" s="7" t="s">
-        <v>295</v>
+        <v>463</v>
       </c>
       <c r="C371" s="4" t="s">
-        <v>297</v>
+        <v>465</v>
       </c>
       <c r="D371" s="35"/>
       <c r="E371" s="29"/>
@@ -11120,51 +11182,43 @@
       <c r="J371" s="20"/>
       <c r="K371" s="35"/>
     </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A372" s="35"/>
-      <c r="B372" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="C372" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="B372" s="11"/>
+      <c r="C372" s="12"/>
       <c r="D372" s="35"/>
-      <c r="E372" s="29"/>
-      <c r="F372" s="60"/>
+      <c r="E372" s="32"/>
+      <c r="F372" s="62"/>
       <c r="G372" s="35"/>
-      <c r="H372" s="29"/>
-      <c r="I372" s="19"/>
-      <c r="J372" s="20"/>
+      <c r="H372" s="32"/>
+      <c r="I372" s="23"/>
+      <c r="J372" s="24"/>
       <c r="K372" s="35"/>
     </row>
     <row r="373" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A373" s="35"/>
       <c r="B373" s="7" t="s">
-        <v>289</v>
+        <v>409</v>
       </c>
       <c r="C373" s="4" t="s">
-        <v>290</v>
+        <v>410</v>
       </c>
       <c r="D373" s="35"/>
       <c r="E373" s="29"/>
       <c r="F373" s="60"/>
       <c r="G373" s="35"/>
       <c r="H373" s="29"/>
-      <c r="I373" s="19">
-        <v>1</v>
-      </c>
-      <c r="J373" s="20">
-        <v>0</v>
-      </c>
+      <c r="I373" s="19"/>
+      <c r="J373" s="20"/>
       <c r="K373" s="35"/>
     </row>
     <row r="374" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A374" s="35"/>
       <c r="B374" s="7" t="s">
-        <v>629</v>
+        <v>419</v>
       </c>
       <c r="C374" s="4" t="s">
-        <v>630</v>
+        <v>420</v>
       </c>
       <c r="D374" s="35"/>
       <c r="E374" s="29"/>
@@ -11178,10 +11232,10 @@
     <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A375" s="35"/>
       <c r="B375" s="7" t="s">
-        <v>583</v>
+        <v>411</v>
       </c>
       <c r="C375" s="4" t="s">
-        <v>589</v>
+        <v>412</v>
       </c>
       <c r="D375" s="35"/>
       <c r="E375" s="29"/>
@@ -11192,47 +11246,47 @@
       <c r="J375" s="20"/>
       <c r="K375" s="35"/>
     </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A376" s="35"/>
-      <c r="B376" s="7" t="s">
-        <v>584</v>
-      </c>
-      <c r="C376" s="4" t="s">
-        <v>588</v>
-      </c>
+      <c r="B376" s="11"/>
+      <c r="C376" s="12"/>
       <c r="D376" s="35"/>
-      <c r="E376" s="29"/>
-      <c r="F376" s="60"/>
+      <c r="E376" s="32"/>
+      <c r="F376" s="62"/>
       <c r="G376" s="35"/>
-      <c r="H376" s="29"/>
-      <c r="I376" s="19"/>
-      <c r="J376" s="20"/>
+      <c r="H376" s="32"/>
+      <c r="I376" s="23"/>
+      <c r="J376" s="24"/>
       <c r="K376" s="35"/>
     </row>
     <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A377" s="35"/>
       <c r="B377" s="7" t="s">
-        <v>585</v>
+        <v>0</v>
       </c>
       <c r="C377" s="4" t="s">
-        <v>590</v>
+        <v>85</v>
       </c>
       <c r="D377" s="35"/>
       <c r="E377" s="29"/>
       <c r="F377" s="60"/>
       <c r="G377" s="35"/>
       <c r="H377" s="29"/>
-      <c r="I377" s="19"/>
-      <c r="J377" s="20"/>
+      <c r="I377" s="19">
+        <v>1</v>
+      </c>
+      <c r="J377" s="20">
+        <v>0</v>
+      </c>
       <c r="K377" s="35"/>
     </row>
     <row r="378" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A378" s="35"/>
       <c r="B378" s="7" t="s">
-        <v>586</v>
+        <v>599</v>
       </c>
       <c r="C378" s="4" t="s">
-        <v>591</v>
+        <v>600</v>
       </c>
       <c r="D378" s="35"/>
       <c r="E378" s="29"/>
@@ -11246,10 +11300,10 @@
     <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379" s="35"/>
       <c r="B379" s="7" t="s">
-        <v>587</v>
+        <v>295</v>
       </c>
       <c r="C379" s="4" t="s">
-        <v>592</v>
+        <v>297</v>
       </c>
       <c r="D379" s="35"/>
       <c r="E379" s="29"/>
@@ -11263,10 +11317,10 @@
     <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380" s="35"/>
       <c r="B380" s="7" t="s">
-        <v>593</v>
+        <v>296</v>
       </c>
       <c r="C380" s="4" t="s">
-        <v>594</v>
+        <v>298</v>
       </c>
       <c r="D380" s="35"/>
       <c r="E380" s="29"/>
@@ -11277,316 +11331,288 @@
       <c r="J380" s="20"/>
       <c r="K380" s="35"/>
     </row>
-    <row r="381" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A381" s="37"/>
-      <c r="B381" s="13" t="s">
-        <v>339</v>
-      </c>
-      <c r="C381" s="14" t="s">
-        <v>343</v>
-      </c>
-      <c r="D381" s="37"/>
-      <c r="E381" s="31"/>
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A381" s="35"/>
+      <c r="B381" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C381" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D381" s="35"/>
+      <c r="E381" s="29"/>
       <c r="F381" s="60"/>
-      <c r="G381" s="37"/>
-      <c r="H381" s="31"/>
+      <c r="G381" s="35"/>
+      <c r="H381" s="29"/>
       <c r="I381" s="19">
         <v>1</v>
       </c>
       <c r="J381" s="20">
         <v>0</v>
       </c>
-      <c r="K381" s="37"/>
-    </row>
-    <row r="382" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A382" s="37"/>
-      <c r="B382" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="C382" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="D382" s="37"/>
-      <c r="E382" s="31"/>
+      <c r="K381" s="35"/>
+    </row>
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A382" s="35"/>
+      <c r="B382" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="C382" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="D382" s="35"/>
+      <c r="E382" s="29"/>
       <c r="F382" s="60"/>
-      <c r="G382" s="37"/>
-      <c r="H382" s="31"/>
-      <c r="I382" s="19">
-        <v>1</v>
-      </c>
-      <c r="J382" s="20">
-        <v>0</v>
-      </c>
-      <c r="K382" s="37"/>
-    </row>
-    <row r="383" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A383" s="37"/>
-      <c r="B383" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="C383" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="D383" s="37"/>
-      <c r="E383" s="31"/>
+      <c r="G382" s="35"/>
+      <c r="H382" s="29"/>
+      <c r="I382" s="19"/>
+      <c r="J382" s="20"/>
+      <c r="K382" s="35"/>
+    </row>
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A383" s="35"/>
+      <c r="B383" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="C383" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="D383" s="35"/>
+      <c r="E383" s="29"/>
       <c r="F383" s="60"/>
-      <c r="G383" s="37"/>
-      <c r="H383" s="31"/>
-      <c r="I383" s="19">
-        <v>1</v>
-      </c>
-      <c r="J383" s="20">
-        <v>0</v>
-      </c>
-      <c r="K383" s="37"/>
-    </row>
-    <row r="384" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A384" s="37"/>
-      <c r="B384" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="C384" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="D384" s="37"/>
-      <c r="E384" s="31"/>
+      <c r="G383" s="35"/>
+      <c r="H383" s="29"/>
+      <c r="I383" s="19"/>
+      <c r="J383" s="20"/>
+      <c r="K383" s="35"/>
+    </row>
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A384" s="35"/>
+      <c r="B384" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="C384" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="D384" s="35"/>
+      <c r="E384" s="29"/>
       <c r="F384" s="60"/>
-      <c r="G384" s="37"/>
-      <c r="H384" s="31"/>
-      <c r="I384" s="19">
-        <v>1</v>
-      </c>
-      <c r="J384" s="20">
-        <v>0</v>
-      </c>
-      <c r="K384" s="37"/>
-    </row>
-    <row r="385" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A385" s="37"/>
+      <c r="G384" s="35"/>
+      <c r="H384" s="29"/>
+      <c r="I384" s="19"/>
+      <c r="J384" s="20"/>
+      <c r="K384" s="35"/>
+    </row>
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A385" s="35"/>
       <c r="B385" s="7" t="s">
-        <v>403</v>
+        <v>585</v>
       </c>
       <c r="C385" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="D385" s="37"/>
-      <c r="E385" s="31"/>
+        <v>590</v>
+      </c>
+      <c r="D385" s="35"/>
+      <c r="E385" s="29"/>
       <c r="F385" s="60"/>
-      <c r="G385" s="37"/>
-      <c r="H385" s="31"/>
+      <c r="G385" s="35"/>
+      <c r="H385" s="29"/>
       <c r="I385" s="19"/>
       <c r="J385" s="20"/>
-      <c r="K385" s="37"/>
-    </row>
-    <row r="386" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A386" s="37"/>
+      <c r="K385" s="35"/>
+    </row>
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A386" s="35"/>
       <c r="B386" s="7" t="s">
-        <v>405</v>
+        <v>586</v>
       </c>
       <c r="C386" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="D386" s="37"/>
-      <c r="E386" s="31"/>
+        <v>591</v>
+      </c>
+      <c r="D386" s="35"/>
+      <c r="E386" s="29"/>
       <c r="F386" s="60"/>
-      <c r="G386" s="37"/>
-      <c r="H386" s="31"/>
+      <c r="G386" s="35"/>
+      <c r="H386" s="29"/>
       <c r="I386" s="19"/>
       <c r="J386" s="20"/>
-      <c r="K386" s="37"/>
-    </row>
-    <row r="387" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A387" s="37"/>
+      <c r="K386" s="35"/>
+    </row>
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A387" s="35"/>
       <c r="B387" s="7" t="s">
-        <v>406</v>
+        <v>587</v>
       </c>
       <c r="C387" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="D387" s="37"/>
-      <c r="E387" s="31"/>
+        <v>592</v>
+      </c>
+      <c r="D387" s="35"/>
+      <c r="E387" s="29"/>
       <c r="F387" s="60"/>
-      <c r="G387" s="37"/>
-      <c r="H387" s="31"/>
+      <c r="G387" s="35"/>
+      <c r="H387" s="29"/>
       <c r="I387" s="19"/>
       <c r="J387" s="20"/>
-      <c r="K387" s="37"/>
+      <c r="K387" s="35"/>
     </row>
     <row r="388" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A388" s="35"/>
       <c r="B388" s="7" t="s">
-        <v>323</v>
+        <v>593</v>
       </c>
       <c r="C388" s="4" t="s">
-        <v>327</v>
+        <v>594</v>
       </c>
       <c r="D388" s="35"/>
       <c r="E388" s="29"/>
       <c r="F388" s="60"/>
       <c r="G388" s="35"/>
       <c r="H388" s="29"/>
-      <c r="I388" s="19">
-        <v>1</v>
-      </c>
-      <c r="J388" s="20">
-        <v>0</v>
-      </c>
+      <c r="I388" s="19"/>
+      <c r="J388" s="20"/>
       <c r="K388" s="35"/>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A389" s="35"/>
-      <c r="B389" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="C389" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D389" s="35"/>
-      <c r="E389" s="29"/>
+    <row r="389" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A389" s="37"/>
+      <c r="B389" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="C389" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D389" s="37"/>
+      <c r="E389" s="31"/>
       <c r="F389" s="60"/>
-      <c r="G389" s="35"/>
-      <c r="H389" s="29"/>
+      <c r="G389" s="37"/>
+      <c r="H389" s="31"/>
       <c r="I389" s="19">
         <v>1</v>
       </c>
       <c r="J389" s="20">
         <v>0</v>
       </c>
-      <c r="K389" s="35"/>
-    </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A390" s="35"/>
-      <c r="B390" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="C390" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="D390" s="35"/>
-      <c r="E390" s="29"/>
+      <c r="K389" s="37"/>
+    </row>
+    <row r="390" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A390" s="37"/>
+      <c r="B390" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="C390" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="D390" s="37"/>
+      <c r="E390" s="31"/>
       <c r="F390" s="60"/>
-      <c r="G390" s="35"/>
-      <c r="H390" s="29"/>
+      <c r="G390" s="37"/>
+      <c r="H390" s="31"/>
       <c r="I390" s="19">
         <v>1</v>
       </c>
       <c r="J390" s="20">
         <v>0</v>
       </c>
-      <c r="K390" s="35"/>
-    </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A391" s="35"/>
-      <c r="B391" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="C391" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="D391" s="35"/>
-      <c r="E391" s="29"/>
+      <c r="K390" s="37"/>
+    </row>
+    <row r="391" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A391" s="37"/>
+      <c r="B391" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C391" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="D391" s="37"/>
+      <c r="E391" s="31"/>
       <c r="F391" s="60"/>
-      <c r="G391" s="35"/>
-      <c r="H391" s="29"/>
+      <c r="G391" s="37"/>
+      <c r="H391" s="31"/>
       <c r="I391" s="19">
         <v>1</v>
       </c>
       <c r="J391" s="20">
         <v>0</v>
       </c>
-      <c r="K391" s="35"/>
-    </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A392" s="35"/>
-      <c r="B392" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="C392" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="D392" s="35"/>
-      <c r="E392" s="29"/>
+      <c r="K391" s="37"/>
+    </row>
+    <row r="392" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A392" s="37"/>
+      <c r="B392" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="C392" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="D392" s="37"/>
+      <c r="E392" s="31"/>
       <c r="F392" s="60"/>
-      <c r="G392" s="35"/>
-      <c r="H392" s="29"/>
+      <c r="G392" s="37"/>
+      <c r="H392" s="31"/>
       <c r="I392" s="19">
         <v>1</v>
       </c>
       <c r="J392" s="20">
         <v>0</v>
       </c>
-      <c r="K392" s="35"/>
-    </row>
-    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A393" s="35"/>
+      <c r="K392" s="37"/>
+    </row>
+    <row r="393" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A393" s="37"/>
       <c r="B393" s="7" t="s">
-        <v>317</v>
+        <v>403</v>
       </c>
       <c r="C393" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="D393" s="35"/>
-      <c r="E393" s="29"/>
+        <v>404</v>
+      </c>
+      <c r="D393" s="37"/>
+      <c r="E393" s="31"/>
       <c r="F393" s="60"/>
-      <c r="G393" s="35"/>
-      <c r="H393" s="29"/>
-      <c r="I393" s="19">
-        <v>1</v>
-      </c>
-      <c r="J393" s="20">
-        <v>0</v>
-      </c>
-      <c r="K393" s="35"/>
-    </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A394" s="35"/>
+      <c r="G393" s="37"/>
+      <c r="H393" s="31"/>
+      <c r="I393" s="19"/>
+      <c r="J393" s="20"/>
+      <c r="K393" s="37"/>
+    </row>
+    <row r="394" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A394" s="37"/>
       <c r="B394" s="7" t="s">
-        <v>307</v>
+        <v>405</v>
       </c>
       <c r="C394" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="D394" s="35"/>
-      <c r="E394" s="29"/>
+        <v>408</v>
+      </c>
+      <c r="D394" s="37"/>
+      <c r="E394" s="31"/>
       <c r="F394" s="60"/>
-      <c r="G394" s="35"/>
-      <c r="H394" s="29"/>
-      <c r="I394" s="19">
-        <v>1</v>
-      </c>
-      <c r="J394" s="20">
-        <v>0</v>
-      </c>
-      <c r="K394" s="35"/>
-    </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A395" s="35"/>
+      <c r="G394" s="37"/>
+      <c r="H394" s="31"/>
+      <c r="I394" s="19"/>
+      <c r="J394" s="20"/>
+      <c r="K394" s="37"/>
+    </row>
+    <row r="395" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A395" s="37"/>
       <c r="B395" s="7" t="s">
-        <v>305</v>
+        <v>406</v>
       </c>
       <c r="C395" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="D395" s="35"/>
-      <c r="E395" s="29"/>
+        <v>407</v>
+      </c>
+      <c r="D395" s="37"/>
+      <c r="E395" s="31"/>
       <c r="F395" s="60"/>
-      <c r="G395" s="35"/>
-      <c r="H395" s="29"/>
-      <c r="I395" s="19">
-        <v>1</v>
-      </c>
-      <c r="J395" s="20">
-        <v>0</v>
-      </c>
-      <c r="K395" s="35"/>
+      <c r="G395" s="37"/>
+      <c r="H395" s="31"/>
+      <c r="I395" s="19"/>
+      <c r="J395" s="20"/>
+      <c r="K395" s="37"/>
     </row>
     <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A396" s="35"/>
       <c r="B396" s="7" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="C396" s="4" t="s">
-        <v>300</v>
+        <v>327</v>
       </c>
       <c r="D396" s="35"/>
       <c r="E396" s="29"/>
@@ -11601,61 +11627,229 @@
       </c>
       <c r="K396" s="35"/>
     </row>
-    <row r="397" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A397" s="35"/>
-      <c r="B397" s="8"/>
-      <c r="C397" s="6"/>
+      <c r="B397" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="C397" s="4" t="s">
+        <v>326</v>
+      </c>
       <c r="D397" s="35"/>
-      <c r="E397" s="33"/>
-      <c r="F397" s="63"/>
+      <c r="E397" s="29"/>
+      <c r="F397" s="60"/>
       <c r="G397" s="35"/>
-      <c r="H397" s="33"/>
-      <c r="I397" s="25"/>
-      <c r="J397" s="26"/>
+      <c r="H397" s="29"/>
+      <c r="I397" s="19">
+        <v>1</v>
+      </c>
+      <c r="J397" s="20">
+        <v>0</v>
+      </c>
       <c r="K397" s="35"/>
     </row>
-    <row r="398" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A398" s="35"/>
-      <c r="B398" s="38"/>
-      <c r="C398" s="39"/>
+      <c r="B398" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="C398" s="4" t="s">
+        <v>328</v>
+      </c>
       <c r="D398" s="35"/>
-      <c r="E398" s="40"/>
-      <c r="F398" s="57"/>
+      <c r="E398" s="29"/>
+      <c r="F398" s="60"/>
       <c r="G398" s="35"/>
-      <c r="H398" s="40"/>
-      <c r="I398" s="41"/>
-      <c r="J398" s="41"/>
+      <c r="H398" s="29"/>
+      <c r="I398" s="19">
+        <v>1</v>
+      </c>
+      <c r="J398" s="20">
+        <v>0</v>
+      </c>
       <c r="K398" s="35"/>
+    </row>
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A399" s="35"/>
+      <c r="B399" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="C399" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="D399" s="35"/>
+      <c r="E399" s="29"/>
+      <c r="F399" s="60"/>
+      <c r="G399" s="35"/>
+      <c r="H399" s="29"/>
+      <c r="I399" s="19">
+        <v>1</v>
+      </c>
+      <c r="J399" s="20">
+        <v>0</v>
+      </c>
+      <c r="K399" s="35"/>
     </row>
     <row r="400" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A400" s="35"/>
       <c r="B400" s="7" t="s">
-        <v>390</v>
+        <v>318</v>
       </c>
       <c r="C400" s="4" t="s">
-        <v>391</v>
+        <v>321</v>
       </c>
       <c r="D400" s="35"/>
       <c r="E400" s="29"/>
       <c r="F400" s="60"/>
       <c r="G400" s="35"/>
       <c r="H400" s="29"/>
-      <c r="I400" s="19"/>
-      <c r="J400" s="20"/>
+      <c r="I400" s="19">
+        <v>1</v>
+      </c>
+      <c r="J400" s="20">
+        <v>0</v>
+      </c>
       <c r="K400" s="35"/>
     </row>
-    <row r="401" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A401" s="35"/>
-      <c r="B401" s="50"/>
-      <c r="C401" s="51"/>
+      <c r="B401" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="C401" s="4" t="s">
+        <v>322</v>
+      </c>
       <c r="D401" s="35"/>
-      <c r="E401" s="52"/>
-      <c r="F401" s="64"/>
+      <c r="E401" s="29"/>
+      <c r="F401" s="60"/>
       <c r="G401" s="35"/>
-      <c r="H401" s="52"/>
-      <c r="I401" s="53"/>
-      <c r="J401" s="54"/>
+      <c r="H401" s="29"/>
+      <c r="I401" s="19">
+        <v>1</v>
+      </c>
+      <c r="J401" s="20">
+        <v>0</v>
+      </c>
       <c r="K401" s="35"/>
+    </row>
+    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A402" s="35"/>
+      <c r="B402" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="C402" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D402" s="35"/>
+      <c r="E402" s="29"/>
+      <c r="F402" s="60"/>
+      <c r="G402" s="35"/>
+      <c r="H402" s="29"/>
+      <c r="I402" s="19">
+        <v>1</v>
+      </c>
+      <c r="J402" s="20">
+        <v>0</v>
+      </c>
+      <c r="K402" s="35"/>
+    </row>
+    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A403" s="35"/>
+      <c r="B403" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C403" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="D403" s="35"/>
+      <c r="E403" s="29"/>
+      <c r="F403" s="60"/>
+      <c r="G403" s="35"/>
+      <c r="H403" s="29"/>
+      <c r="I403" s="19">
+        <v>1</v>
+      </c>
+      <c r="J403" s="20">
+        <v>0</v>
+      </c>
+      <c r="K403" s="35"/>
+    </row>
+    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A404" s="35"/>
+      <c r="B404" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C404" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D404" s="35"/>
+      <c r="E404" s="29"/>
+      <c r="F404" s="60"/>
+      <c r="G404" s="35"/>
+      <c r="H404" s="29"/>
+      <c r="I404" s="19">
+        <v>1</v>
+      </c>
+      <c r="J404" s="20">
+        <v>0</v>
+      </c>
+      <c r="K404" s="35"/>
+    </row>
+    <row r="405" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A405" s="35"/>
+      <c r="B405" s="8"/>
+      <c r="C405" s="6"/>
+      <c r="D405" s="35"/>
+      <c r="E405" s="33"/>
+      <c r="F405" s="63"/>
+      <c r="G405" s="35"/>
+      <c r="H405" s="33"/>
+      <c r="I405" s="25"/>
+      <c r="J405" s="26"/>
+      <c r="K405" s="35"/>
+    </row>
+    <row r="406" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A406" s="35"/>
+      <c r="B406" s="38"/>
+      <c r="C406" s="39"/>
+      <c r="D406" s="35"/>
+      <c r="E406" s="40"/>
+      <c r="F406" s="57"/>
+      <c r="G406" s="35"/>
+      <c r="H406" s="40"/>
+      <c r="I406" s="41"/>
+      <c r="J406" s="41"/>
+      <c r="K406" s="35"/>
+    </row>
+    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A408" s="35"/>
+      <c r="B408" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="C408" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="D408" s="35"/>
+      <c r="E408" s="29"/>
+      <c r="F408" s="60"/>
+      <c r="G408" s="35"/>
+      <c r="H408" s="29"/>
+      <c r="I408" s="19"/>
+      <c r="J408" s="20"/>
+      <c r="K408" s="35"/>
+    </row>
+    <row r="409" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A409" s="35"/>
+      <c r="B409" s="50"/>
+      <c r="C409" s="51"/>
+      <c r="D409" s="35"/>
+      <c r="E409" s="52"/>
+      <c r="F409" s="64"/>
+      <c r="G409" s="35"/>
+      <c r="H409" s="52"/>
+      <c r="I409" s="53"/>
+      <c r="J409" s="54"/>
+      <c r="K409" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -11667,7 +11861,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F4:F6 F9 F12:F14 F17:F18 F20 F22:F24 F27:F33 F36:F41 F43:F74 F77:F81 F83:F87 F89:F95 F97:F99 F104:F105 F107 F109:F127 F101:F102 F129:F164 F166:F167 F169:F173 F176:F195 F198:F203 F205:F206 F208:F226 F228:F229 F231:F232 F235:F240 F242:F243 F245:F246 F248:F269 F271:F272 F274:F281 F283:F285 F288:F290 F292 F294:F298 F300:F303 F305:F306 F313:F315 F310:F312 F317:F319" numberStoredAsText="1"/>
+    <ignoredError sqref="F4:F6 F9 F12:F14 F17:F18 F20 F22:F24 F27:F33 F36:F41 F43:F74 F77:F81 F83:F87 F89:F95 F97:F99 F101:F102 F107 F109:F127 F129:F164 F166:F167 F169:F173 F176:F195 F198:F203 F205:F206 F208:F226 F228:F229 F231:F232 F235:F240 F242:F243 F245:F246 F248:F269 F271:F272 F274:F281 F283:F285 F288:F290 F292 F294:F298 F300:F303 F305:F306 F313:F315 F310:F312 F317:F319 F321:F322 F324:F325 F104:F105 F327" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Penambahan API, Update Data API Catalogue, Update Store Procedure
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="767">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -2405,6 +2405,24 @@
   </si>
   <si>
     <t>Menyimpan Data Baru Item Seksi Proyek</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Proyek</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Seksi Proyek</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Item Seksi Proyek</t>
+  </si>
+  <si>
+    <t>transaction.update.project.setProject</t>
+  </si>
+  <si>
+    <t>transaction.update.project.setProjectSection</t>
+  </si>
+  <si>
+    <t>transaction.update.project.setProjectSectionItem</t>
   </si>
 </sst>
 </file>
@@ -3291,13 +3309,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L453"/>
+  <dimension ref="A1:L457"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C440" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F76" sqref="F76"/>
+      <selection pane="bottomRight" activeCell="C451" sqref="C451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -13265,61 +13283,137 @@
       <c r="J448" s="20"/>
       <c r="K448" s="35"/>
     </row>
-    <row r="449" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A449" s="35"/>
-      <c r="B449" s="8"/>
-      <c r="C449" s="6"/>
+      <c r="B449" s="11"/>
+      <c r="C449" s="12"/>
       <c r="D449" s="35"/>
-      <c r="E449" s="33"/>
-      <c r="F449" s="61"/>
+      <c r="E449" s="32"/>
+      <c r="F449" s="60"/>
       <c r="G449" s="35"/>
-      <c r="H449" s="33"/>
-      <c r="I449" s="25"/>
-      <c r="J449" s="26"/>
+      <c r="H449" s="32"/>
+      <c r="I449" s="23"/>
+      <c r="J449" s="24"/>
       <c r="K449" s="35"/>
     </row>
-    <row r="450" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A450" s="35"/>
-      <c r="B450" s="38"/>
-      <c r="C450" s="39"/>
+      <c r="B450" s="7" t="s">
+        <v>764</v>
+      </c>
+      <c r="C450" s="4" t="s">
+        <v>761</v>
+      </c>
       <c r="D450" s="35"/>
-      <c r="E450" s="40"/>
-      <c r="F450" s="55"/>
+      <c r="E450" s="29">
+        <v>44384</v>
+      </c>
+      <c r="F450" s="58" t="s">
+        <v>631</v>
+      </c>
       <c r="G450" s="35"/>
-      <c r="H450" s="40"/>
-      <c r="I450" s="41"/>
-      <c r="J450" s="41"/>
+      <c r="H450" s="29"/>
+      <c r="I450" s="19"/>
+      <c r="J450" s="20"/>
       <c r="K450" s="35"/>
+    </row>
+    <row r="451" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A451" s="35"/>
+      <c r="B451" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="C451" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="D451" s="35"/>
+      <c r="E451" s="29">
+        <v>44384</v>
+      </c>
+      <c r="F451" s="58" t="s">
+        <v>631</v>
+      </c>
+      <c r="G451" s="35"/>
+      <c r="H451" s="29"/>
+      <c r="I451" s="19"/>
+      <c r="J451" s="20"/>
+      <c r="K451" s="35"/>
     </row>
     <row r="452" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A452" s="35"/>
       <c r="B452" s="7" t="s">
-        <v>389</v>
+        <v>766</v>
       </c>
       <c r="C452" s="4" t="s">
-        <v>390</v>
+        <v>763</v>
       </c>
       <c r="D452" s="35"/>
-      <c r="E452" s="29"/>
-      <c r="F452" s="58"/>
+      <c r="E452" s="29">
+        <v>44384</v>
+      </c>
+      <c r="F452" s="58" t="s">
+        <v>631</v>
+      </c>
       <c r="G452" s="35"/>
       <c r="H452" s="29"/>
       <c r="I452" s="19"/>
       <c r="J452" s="20"/>
       <c r="K452" s="35"/>
     </row>
-    <row r="453" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A453" s="35"/>
-      <c r="B453" s="50"/>
-      <c r="C453" s="51"/>
+      <c r="B453" s="8"/>
+      <c r="C453" s="6"/>
       <c r="D453" s="35"/>
-      <c r="E453" s="52"/>
-      <c r="F453" s="62"/>
+      <c r="E453" s="33"/>
+      <c r="F453" s="61"/>
       <c r="G453" s="35"/>
-      <c r="H453" s="52"/>
-      <c r="I453" s="53"/>
-      <c r="J453" s="54"/>
+      <c r="H453" s="33"/>
+      <c r="I453" s="25"/>
+      <c r="J453" s="26"/>
       <c r="K453" s="35"/>
+    </row>
+    <row r="454" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A454" s="35"/>
+      <c r="B454" s="38"/>
+      <c r="C454" s="39"/>
+      <c r="D454" s="35"/>
+      <c r="E454" s="40"/>
+      <c r="F454" s="55"/>
+      <c r="G454" s="35"/>
+      <c r="H454" s="40"/>
+      <c r="I454" s="41"/>
+      <c r="J454" s="41"/>
+      <c r="K454" s="35"/>
+    </row>
+    <row r="456" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A456" s="35"/>
+      <c r="B456" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="C456" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="D456" s="35"/>
+      <c r="E456" s="29"/>
+      <c r="F456" s="58"/>
+      <c r="G456" s="35"/>
+      <c r="H456" s="29"/>
+      <c r="I456" s="19"/>
+      <c r="J456" s="20"/>
+      <c r="K456" s="35"/>
+    </row>
+    <row r="457" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A457" s="35"/>
+      <c r="B457" s="50"/>
+      <c r="C457" s="51"/>
+      <c r="D457" s="35"/>
+      <c r="E457" s="52"/>
+      <c r="F457" s="62"/>
+      <c r="G457" s="35"/>
+      <c r="H457" s="52"/>
+      <c r="I457" s="53"/>
+      <c r="J457" s="54"/>
+      <c r="K457" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -13331,7 +13425,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F4:F6 F9 F12:F14 F17:F18 F20 F22:F24 F27:F33 F36:F41 F43:F74 F86:F90 F92:F96 F98:F104 F106:F108 F110:F111 F116 F118:F136 F138:F173 F175:F176 F178:F182 F185:F204 F207:F212 F214:F215 F238:F239 F241:F242 F249:F254 F256:F257 F259:F260 F296:F297 F299:F307 F310:F312 F314 F316:F320 F322:F325 F327:F328 F338:F343 F345:F347 F349:F350 F352:F353 F113:F114 F355 F357:F358 F360:F394 F396:F397 F399:F403 F332:F336 F406:F410 F412:F414 F416:F443 F76:F79 F445:F448 F281:F292 F217:F236 F262:F274 F275:F280 F294:F295 F245:F247 F81:F83" numberStoredAsText="1"/>
+    <ignoredError sqref="F4:F6 F9 F12:F14 F17:F18 F20 F22:F24 F27:F33 F36:F41 F43:F74 F86:F90 F92:F96 F98:F104 F106:F108 F110:F111 F116 F118:F136 F138:F173 F175:F176 F178:F182 F185:F204 F207:F212 F214:F215 F238:F239 F241:F242 F249:F254 F256:F257 F259:F260 F296:F297 F299:F307 F310:F312 F314 F316:F320 F322:F325 F327:F328 F338:F343 F345:F347 F349:F350 F352:F353 F113:F114 F355 F357:F358 F360:F394 F396:F397 F399:F403 F332:F336 F406:F410 F412:F414 F416:F443 F76:F79 F445:F448 F281:F292 F217:F236 F262:F274 F275:F280 F294:F295 F245:F247 F81:F83 F450:F452" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Penambahan API fileHandling.upload.setStagingFile, Update Data API Catalogue, Update Store Procedure
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
@@ -3480,7 +3480,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3827,7 +3827,7 @@
       </c>
       <c r="D17" s="35"/>
       <c r="E17" s="29">
-        <v>44397</v>
+        <v>44398</v>
       </c>
       <c r="F17" s="58" t="s">
         <v>627</v>

</xml_diff>

<commit_message>
Penambahan dan Rekonfigurasi API fileHandling.upload.getStagingFileNewID, Update Data API Catalogue, Update Store Procedure, Update Helper
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-Catalogue.xlsx
@@ -2719,7 +2719,7 @@
     </r>
   </si>
   <si>
-    <t>fileHandling.upload.getNewStagingFileID</t>
+    <t>fileHandling.upload.getStagingFileNewID</t>
   </si>
 </sst>
 </file>
@@ -3612,7 +3612,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>